<commit_message>
Ananth - Updated Test data for Inventory case
</commit_message>
<xml_diff>
--- a/Basic Test Suite/TestData/TestData.xlsx
+++ b/Basic Test Suite/TestData/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ITL-PC07\SharedExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.137\SharedExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="240" windowWidth="20460" windowHeight="7515" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7155" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="SparcsN4Login" sheetId="1" r:id="rId1"/>
@@ -21,23 +21,20 @@
     <sheet name="Orders" sheetId="6" r:id="rId7"/>
     <sheet name="Inventory" sheetId="7" r:id="rId8"/>
     <sheet name="UnitFacilityVisit" sheetId="8" r:id="rId9"/>
-    <sheet name="Sheet1" sheetId="10" r:id="rId10"/>
+    <sheet name="N4MobileCommonRoutines" sheetId="10" r:id="rId10"/>
+    <sheet name="SparcsN4CommonRoutines" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="ITL-USER - Personal View" guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1380" windowHeight="744" activeSheetId="10"/>
     <customWorkbookView name="itluser - Personal View" guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="5"/>
-    <customWorkbookView name="ITLAdmin - Personal View" guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1362" windowHeight="503" activeSheetId="2"/>
+    <customWorkbookView name="ITLAdmin - Personal View" guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1362" windowHeight="503" activeSheetId="11"/>
   </customWorkbookViews>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="341">
   <si>
     <t>Flow Name</t>
   </si>
@@ -804,12 +801,6 @@
     <t>MessageClass</t>
   </si>
   <si>
-    <t>LineOperator</t>
-  </si>
-  <si>
-    <t>CAS</t>
-  </si>
-  <si>
     <t>MessageID</t>
   </si>
   <si>
@@ -927,7 +918,145 @@
     <t>TrainVisit</t>
   </si>
   <si>
-    <t>LineOperatorName</t>
+    <t>n4MobileUserName</t>
+  </si>
+  <si>
+    <t>n4MobilePassword</t>
+  </si>
+  <si>
+    <t>n4MobileOperator</t>
+  </si>
+  <si>
+    <t>n4MobileComplex</t>
+  </si>
+  <si>
+    <t>n4MobileFacility</t>
+  </si>
+  <si>
+    <t>n4MobileYard</t>
+  </si>
+  <si>
+    <t>n4MobileProgram</t>
+  </si>
+  <si>
+    <t>n4MobileYardInventoryOperation</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainer</t>
+  </si>
+  <si>
+    <t>N4MobileCommonRoutines</t>
+  </si>
+  <si>
+    <t>Yard Inventory</t>
+  </si>
+  <si>
+    <t>Query</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerSeal1</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>YINV_101</t>
+  </si>
+  <si>
+    <t>SBSU1234570</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerSeal2</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerSeal3</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerSeal4</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerDamageComponent1</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerDamageType1</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerDamageSeverity1</t>
+  </si>
+  <si>
+    <t>DOOR</t>
+  </si>
+  <si>
+    <t>DAT</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerDamageLocation1</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerDamageQuantity1</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerDamageWidth1</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerDamageLength1</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerDamageDeep1</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerSafeWeight</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerTareWeight</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerCSCDate</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerMNF</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerMNRStatus</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerOverHeight</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerOverLeft</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerOverRight</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerOverFore</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerOverAft</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerUnits</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerGradeValue</t>
+  </si>
+  <si>
+    <t>FOOD</t>
   </si>
 </sst>
 </file>
@@ -969,7 +1098,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -984,6 +1113,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1003,7 +1133,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{02B4E074-E18F-4670-BFA1-6241F3EB49EB}" diskRevisions="1" revisionId="489" version="129">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{0D847394-68DB-4FEB-828F-2A6960EA0820}" diskRevisions="1" revisionId="574" version="156">
   <header guid="{0C6C8E69-ABD3-4A89-B740-FE71B52466B3}" dateTime="2018-04-13T11:32:52" maxSheetId="9" userName="itluser" r:id="rId1">
     <sheetIdMap count="8">
       <sheetId val="1"/>
@@ -2723,6 +2853,410 @@
       <sheetId val="7"/>
       <sheetId val="8"/>
       <sheetId val="10"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{17EFF5E6-C655-4E09-B326-D1C3A4D7C6C6}" dateTime="2018-05-04T15:36:11" maxSheetId="11" userName="ITLAdmin" r:id="rId130" minRId="490" maxRId="510">
+    <sheetIdMap count="10">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{BDDB1815-0772-4660-AE86-E364D600DA8C}" dateTime="2018-05-04T15:37:31" maxSheetId="12" userName="ITLAdmin" r:id="rId131" minRId="511" maxRId="521">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{094652D6-D9A8-433E-9635-4E9234F3518D}" dateTime="2018-05-07T15:13:28" maxSheetId="12" userName="ITL-USER" r:id="rId132" minRId="522" maxRId="523">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{C221CC44-A118-4B2E-9DD9-2FED6875AAA6}" dateTime="2018-05-07T15:13:41" maxSheetId="12" userName="ITL-USER" r:id="rId133" minRId="524" maxRId="533">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{53696515-73F7-4CA7-9EB3-FBB2FD14654B}" dateTime="2018-05-07T15:15:47" maxSheetId="12" userName="ITL-USER" r:id="rId134" minRId="534" maxRId="535">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{7E340121-56E7-47B1-A847-EBBFAF4CEA4E}" dateTime="2018-05-07T15:17:44" maxSheetId="12" userName="ITL-USER" r:id="rId135" minRId="536" maxRId="537">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{54A50B94-A441-4A99-A7C3-A5B9F610F409}" dateTime="2018-05-07T15:19:02" maxSheetId="12" userName="ITL-USER" r:id="rId136" minRId="538" maxRId="539">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{895D6C27-60EB-4919-8832-40BCB1C0085E}" dateTime="2018-05-07T16:02:25" maxSheetId="12" userName="ITL-USER" r:id="rId137" minRId="540" maxRId="548">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A41CA12C-AFA7-41E8-A435-50F3F59A4F11}" dateTime="2018-05-07T16:04:17" maxSheetId="12" userName="ITL-USER" r:id="rId138" minRId="549">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{DA1BCC47-657A-4E54-9EFF-27E62A42057A}" dateTime="2018-05-07T16:04:21" maxSheetId="12" userName="ITL-USER" r:id="rId139">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{2C190334-D5B4-4822-AB97-228E4EBE03DF}" dateTime="2018-05-07T16:06:21" maxSheetId="12" userName="ITL-USER" r:id="rId140" minRId="550">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{4A114344-534E-4A3B-BB19-3D755B20681B}" dateTime="2018-05-07T16:10:06" maxSheetId="12" userName="ITL-USER" r:id="rId141" minRId="551">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B6745ED7-5B2F-4E5E-B3CF-65EDF2B203EB}" dateTime="2018-05-07T16:10:26" maxSheetId="12" userName="ITL-USER" r:id="rId142" minRId="552">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{16DDB71F-FEB9-493A-8470-F27AE85B7820}" dateTime="2018-05-07T16:10:54" maxSheetId="12" userName="ITL-USER" r:id="rId143" minRId="553">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{8A53AE1C-4291-4A85-BF08-C7FC11960330}" dateTime="2018-05-07T16:34:26" maxSheetId="12" userName="ITL-USER" r:id="rId144" minRId="554" maxRId="555">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B465D8AC-B021-4E4F-B4EB-F0425D001898}" dateTime="2018-05-07T16:37:34" maxSheetId="12" userName="ITL-USER" r:id="rId145" minRId="556" maxRId="557">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{0AF98FD8-DF12-40BD-838D-A5B78B417972}" dateTime="2018-05-07T16:39:25" maxSheetId="12" userName="ITL-USER" r:id="rId146" minRId="558">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{D8C1E410-4C9A-4105-9FD6-620BFABEDD55}" dateTime="2018-05-07T16:40:20" maxSheetId="12" userName="ITL-USER" r:id="rId147" minRId="559">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{51D49957-AE90-4A20-96AE-8F46722BFD72}" dateTime="2018-05-07T16:41:50" maxSheetId="12" userName="ITL-USER" r:id="rId148" minRId="560">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{53DFA0C9-5F52-4186-866D-DF81E5128DC2}" dateTime="2018-05-07T17:08:03" maxSheetId="12" userName="ITL-USER" r:id="rId149" minRId="561" maxRId="562">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{02C162DF-B47C-42CB-9562-0187183D0572}" dateTime="2018-05-07T17:10:39" maxSheetId="12" userName="ITL-USER" r:id="rId150" minRId="563" maxRId="564">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{E1AEA4E3-BA4E-496B-9CAE-09691939490C}" dateTime="2018-05-07T17:12:39" maxSheetId="12" userName="ITL-USER" r:id="rId151" minRId="565" maxRId="566">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{77498283-26CE-439C-B3E2-6B57D34D9D4D}" dateTime="2018-05-07T17:14:14" maxSheetId="12" userName="ITL-USER" r:id="rId152" minRId="567" maxRId="568">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{DFA03B02-BDFB-4004-BB84-B12588735CC5}" dateTime="2018-05-07T17:15:12" maxSheetId="12" userName="ITL-USER" r:id="rId153" minRId="569" maxRId="570">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{85CDF29B-7EE6-4FB7-ADBA-7D9DD69E36F4}" dateTime="2018-05-07T17:16:29" maxSheetId="12" userName="ITL-USER" r:id="rId154" minRId="571" maxRId="572">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{22F45F2C-C410-4DA2-968A-C25BB34BD207}" dateTime="2018-05-07T17:33:13" maxSheetId="12" userName="ITL-USER" r:id="rId155" minRId="573">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{0D847394-68DB-4FEB-828F-2A6960EA0820}" dateTime="2018-05-07T17:33:18" maxSheetId="12" userName="ITL-USER" r:id="rId156" minRId="574">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
     </sheetIdMap>
   </header>
 </headers>
@@ -7518,6 +8052,599 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog130.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="10" xfDxf="1" sqref="A1" start="0" length="0"/>
+  <rfmt sheetId="10" xfDxf="1" sqref="B1" start="0" length="0"/>
+  <rfmt sheetId="10" xfDxf="1" sqref="C1" start="0" length="0"/>
+  <rfmt sheetId="10" xfDxf="1" sqref="D1" start="0" length="0"/>
+  <rfmt sheetId="10" xfDxf="1" sqref="E1" start="0" length="0"/>
+  <rfmt sheetId="10" xfDxf="1" sqref="F1" start="0" length="0"/>
+  <rfmt sheetId="10" xfDxf="1" sqref="G1" start="0" length="0"/>
+  <rfmt sheetId="10" xfDxf="1" sqref="H1" start="0" length="0"/>
+  <rfmt sheetId="10" xfDxf="1" sqref="I1" start="0" length="0"/>
+  <rfmt sheetId="10" xfDxf="1" sqref="J1" start="0" length="0"/>
+  <rfmt sheetId="10" xfDxf="1" sqref="A2" start="0" length="0"/>
+  <rfmt sheetId="10" xfDxf="1" sqref="B2" start="0" length="0"/>
+  <rfmt sheetId="10" xfDxf="1" sqref="C2" start="0" length="0"/>
+  <rfmt sheetId="10" xfDxf="1" sqref="D2" start="0" length="0"/>
+  <rfmt sheetId="10" xfDxf="1" sqref="E2" start="0" length="0"/>
+  <rfmt sheetId="10" xfDxf="1" sqref="F2" start="0" length="0"/>
+  <rfmt sheetId="10" xfDxf="1" sqref="G2" start="0" length="0"/>
+  <rfmt sheetId="10" xfDxf="1" sqref="H2" start="0" length="0"/>
+  <rfmt sheetId="10" xfDxf="1" sqref="I2" start="0" length="0"/>
+  <rfmt sheetId="10" xfDxf="1" sqref="J2" start="0" length="0"/>
+  <rfmt sheetId="10" xfDxf="1" sqref="A1" start="0" length="0"/>
+  <rcc rId="490" sId="10" xfDxf="1" dxf="1">
+    <oc r="B1" t="inlineStr">
+      <is>
+        <t>EnterKey</t>
+      </is>
+    </oc>
+    <nc r="B1" t="inlineStr">
+      <is>
+        <t>n4MobileUserName</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="491" sId="10" xfDxf="1" dxf="1">
+    <oc r="C1" t="inlineStr">
+      <is>
+        <t>EscapeKey</t>
+      </is>
+    </oc>
+    <nc r="C1" t="inlineStr">
+      <is>
+        <t>n4MobilePassword</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="492" sId="10" xfDxf="1" dxf="1">
+    <oc r="D1" t="inlineStr">
+      <is>
+        <t>TabKey</t>
+      </is>
+    </oc>
+    <nc r="D1" t="inlineStr">
+      <is>
+        <t>n4MobileOperator</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="493" sId="10" xfDxf="1" dxf="1">
+    <oc r="E1" t="inlineStr">
+      <is>
+        <t>FileName</t>
+      </is>
+    </oc>
+    <nc r="E1" t="inlineStr">
+      <is>
+        <t>n4MobileComplex</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="494" sId="10" xfDxf="1" dxf="1">
+    <oc r="F1" t="inlineStr">
+      <is>
+        <t>LineOperator</t>
+      </is>
+    </oc>
+    <nc r="F1" t="inlineStr">
+      <is>
+        <t>n4MobileFacility</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="495" sId="10" xfDxf="1" dxf="1">
+    <oc r="G1" t="inlineStr">
+      <is>
+        <t>LineOperatorName</t>
+      </is>
+    </oc>
+    <nc r="G1" t="inlineStr">
+      <is>
+        <t>n4MobileYard</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="496" sId="10" xfDxf="1" dxf="1">
+    <nc r="H1" t="inlineStr">
+      <is>
+        <t>n4MobileProgram</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="497" sId="10" xfDxf="1" dxf="1">
+    <nc r="I1" t="inlineStr">
+      <is>
+        <t>n4MobileYardInventoryOperation</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="498" sId="10" xfDxf="1" dxf="1">
+    <nc r="J1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainer</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="499" sId="10" xfDxf="1" dxf="1">
+    <oc r="A2" t="inlineStr">
+      <is>
+        <t>SparcsN4CommonRoutines</t>
+      </is>
+    </oc>
+    <nc r="A2" t="inlineStr">
+      <is>
+        <t>N4MobileCommonRoutines</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="500" sId="10" xfDxf="1" dxf="1">
+    <oc r="B2" t="inlineStr">
+      <is>
+        <t>[Enter]</t>
+      </is>
+    </oc>
+    <nc r="B2" t="inlineStr">
+      <is>
+        <t>admin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="501" sId="10" xfDxf="1" dxf="1">
+    <oc r="C2" t="inlineStr">
+      <is>
+        <t>[Esc]</t>
+      </is>
+    </oc>
+    <nc r="C2" t="inlineStr">
+      <is>
+        <t>Admin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="502" sId="10" xfDxf="1" dxf="1">
+    <oc r="D2" t="inlineStr">
+      <is>
+        <t>[Tab]</t>
+      </is>
+    </oc>
+    <nc r="D2" t="inlineStr">
+      <is>
+        <t>OPR1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="503" sId="10" xfDxf="1" dxf="1">
+    <oc r="E2" t="inlineStr">
+      <is>
+        <t>ICY_Commodity.xml</t>
+      </is>
+    </oc>
+    <nc r="E2" t="inlineStr">
+      <is>
+        <t>CPX11</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="504" sId="10" xfDxf="1" dxf="1">
+    <nc r="F2" t="inlineStr">
+      <is>
+        <t>FCY111</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="505" sId="10" xfDxf="1" dxf="1">
+    <nc r="G2" t="inlineStr">
+      <is>
+        <t>YRD1111</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="506" sId="10" xfDxf="1" dxf="1">
+    <nc r="H2" t="inlineStr">
+      <is>
+        <t>Yard Inventory</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="507" sId="10" xfDxf="1" dxf="1">
+    <nc r="I2" t="inlineStr">
+      <is>
+        <t>Query</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="10" xfDxf="1" sqref="J2" start="0" length="0"/>
+  <rrc rId="508" sId="10" ref="A3:XFD3" action="deleteRow">
+    <rfmt sheetId="10" xfDxf="1" sqref="A3:XFD3" start="0" length="0"/>
+    <rcc rId="0" sId="10">
+      <nc r="A3" t="inlineStr">
+        <is>
+          <t>n4Vesselcreate</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="10">
+      <nc r="F3" t="inlineStr">
+        <is>
+          <t>ASW</t>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+  <rrc rId="509" sId="10" ref="A3:XFD3" action="deleteRow">
+    <rfmt sheetId="10" xfDxf="1" sqref="A3:XFD3" start="0" length="0"/>
+    <rcc rId="0" sId="10">
+      <nc r="A3" t="inlineStr">
+        <is>
+          <t>n4LineOperator</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="10">
+      <nc r="F3" t="inlineStr">
+        <is>
+          <t>CAS</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="10">
+      <nc r="G3" t="inlineStr">
+        <is>
+          <t>CAS</t>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+  <rcv guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" action="delete"/>
+  <rcv guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" action="add"/>
+  <rsnm rId="510" sheetId="10" oldName="[TestData_Shared.xlsx]Sheet1" newName="[TestData_Shared.xlsx]N4MobileCommonRoutines"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog131.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <ris rId="511" sheetId="11" name="[TestData_Shared.xlsx]SparcsN4CommonRoutines" sheetPosition="10"/>
+  <rcc rId="512" sId="11" xfDxf="1" dxf="1">
+    <nc r="A1" t="inlineStr">
+      <is>
+        <t>Flow Name</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="513" sId="11" xfDxf="1" dxf="1">
+    <nc r="B1" t="inlineStr">
+      <is>
+        <t>EnterKey</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="514" sId="11" xfDxf="1" dxf="1">
+    <nc r="C1" t="inlineStr">
+      <is>
+        <t>EscapeKey</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="515" sId="11" xfDxf="1" dxf="1">
+    <nc r="D1" t="inlineStr">
+      <is>
+        <t>TabKey</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="516" sId="11" xfDxf="1" dxf="1">
+    <nc r="E1" t="inlineStr">
+      <is>
+        <t>FileName</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="517" sId="11" xfDxf="1" dxf="1">
+    <nc r="A2" t="inlineStr">
+      <is>
+        <t>SparcsN4CommonRoutines</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="518" sId="11" xfDxf="1" dxf="1">
+    <nc r="B2" t="inlineStr">
+      <is>
+        <t>[Enter]</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="519" sId="11" xfDxf="1" dxf="1">
+    <nc r="C2" t="inlineStr">
+      <is>
+        <t>[Esc]</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="520" sId="11" xfDxf="1" dxf="1">
+    <nc r="D2" t="inlineStr">
+      <is>
+        <t>[Tab]</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="521" sId="11" xfDxf="1" dxf="1">
+    <nc r="E2" t="inlineStr">
+      <is>
+        <t>ICY_Commodity.xml</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" action="delete"/>
+  <rcv guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog132.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="522" sId="10" odxf="1">
+    <nc r="K1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerSeal1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="523" sId="10" odxf="1">
+    <nc r="K3" t="inlineStr">
+      <is>
+        <t>S1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog133.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="524" sId="10" odxf="1">
+    <nc r="A3" t="inlineStr">
+      <is>
+        <t>YINV_101</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="525" sId="10" odxf="1">
+    <nc r="B3" t="inlineStr">
+      <is>
+        <t>admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="526" sId="10" odxf="1">
+    <nc r="C3" t="inlineStr">
+      <is>
+        <t>Admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="527" sId="10" odxf="1">
+    <nc r="D3" t="inlineStr">
+      <is>
+        <t>OPR1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="528" sId="10" odxf="1">
+    <nc r="E3" t="inlineStr">
+      <is>
+        <t>CPX11</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="529" sId="10" odxf="1">
+    <nc r="F3" t="inlineStr">
+      <is>
+        <t>FCY111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="530" sId="10" odxf="1">
+    <nc r="G3" t="inlineStr">
+      <is>
+        <t>YRD1111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="531" sId="10" odxf="1">
+    <nc r="H3" t="inlineStr">
+      <is>
+        <t>Yard Inventory</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="532" sId="10" odxf="1">
+    <nc r="I3" t="inlineStr">
+      <is>
+        <t>Query</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="533" sId="10" odxf="1">
+    <nc r="J3" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog134.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="534" sId="10" odxf="1">
+    <nc r="L1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerSeal2</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="535" sId="10">
+    <nc r="L3" t="inlineStr">
+      <is>
+        <t>S2</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog135.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="536" sId="10" odxf="1">
+    <nc r="M1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerSeal3</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="537" sId="10">
+    <nc r="M3" t="inlineStr">
+      <is>
+        <t>S3</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog136.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="538" sId="10" xfDxf="1" dxf="1">
+    <nc r="N1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerSeal4</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="539" sId="10">
+    <nc r="N3" t="inlineStr">
+      <is>
+        <t>S4</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog137.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="540" sId="10" odxf="1">
+    <nc r="O1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageComponent1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="541" sId="10" odxf="1">
+    <nc r="P1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageType1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="542" sId="10" odxf="1">
+    <nc r="Q1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageSeverity1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="543" sId="10" odxf="1">
+    <nc r="O2" t="inlineStr">
+      <is>
+        <t>DOOR</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="544" sId="10" odxf="1">
+    <nc r="P2" t="inlineStr">
+      <is>
+        <t>DAT</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="545" sId="10" odxf="1">
+    <nc r="Q2" t="inlineStr">
+      <is>
+        <t>Major</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="546" sId="10">
+    <nc r="O3" t="inlineStr">
+      <is>
+        <t>DOOR</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="547" sId="10">
+    <nc r="P3" t="inlineStr">
+      <is>
+        <t>DAT</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="548" sId="10">
+    <nc r="Q3" t="inlineStr">
+      <is>
+        <t>Major</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog138.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="549" sId="10" xfDxf="1" dxf="1">
+    <nc r="R1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageLocation1</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog139.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="15" sId="3" xfDxf="1" dxf="1">
@@ -7534,6 +8661,159 @@
       </is>
     </nc>
   </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog140.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="550" sId="10">
+    <nc r="S1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageQuantity1</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog141.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="551" sId="10">
+    <nc r="T1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageWidth1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog142.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="552" sId="10">
+    <nc r="U1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageLength1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog143.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="553" sId="10">
+    <nc r="V1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageDeep1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog144.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="554" sId="10" odxf="1">
+    <nc r="W1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerSafeWeight</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="555" sId="10" odxf="1">
+    <nc r="W2">
+      <v>26000</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog145.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="556" sId="10" odxf="1">
+    <nc r="X1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerTareWeight</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="557" sId="10" odxf="1">
+    <nc r="X2">
+      <v>2000</v>
+    </nc>
+    <odxf/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog146.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="558" sId="10">
+    <nc r="Y1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerCSCDate</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog147.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="559" sId="10">
+    <nc r="Z1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerMNF</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog148.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="560" sId="10">
+    <nc r="AA1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerMNRStatus</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog149.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="561" sId="10">
+    <nc r="AB1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerOverHeight</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="562" sId="10">
+    <nc r="AB2">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
 </revisions>
 </file>
 
@@ -7549,6 +8829,129 @@
   </rcc>
   <rcv guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" action="delete"/>
   <rcv guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog150.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="563" sId="10">
+    <nc r="AC1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerOverLeft</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="564" sId="10">
+    <nc r="AC2">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog151.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="565" sId="10">
+    <nc r="AD1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerOverRight</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="566" sId="10">
+    <nc r="AD2">
+      <v>12</v>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog152.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="567" sId="10">
+    <nc r="AE1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerOverFore</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="568" sId="10">
+    <nc r="AE2">
+      <v>11</v>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog153.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="569" sId="10">
+    <nc r="AF1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerOverAft</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="570" sId="10">
+    <nc r="AF2">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog154.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="571" sId="10">
+    <nc r="AG1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerUnits</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="572" sId="10">
+    <nc r="AG2" t="inlineStr">
+      <is>
+        <t>cm</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog155.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="573" sId="10">
+    <nc r="AH1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerGradeValue</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog156.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="574" sId="10">
+    <nc r="AH2" t="inlineStr">
+      <is>
+        <t>FOOD</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
 </revisions>
 </file>
 
@@ -9354,12 +10757,13 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="5">
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="6">
   <userInfo guid="{0FC3EEC7-1253-40C9-80FE-72015618EED8}" name="ITLAdmin" id="-2068730528" dateTime="2018-04-13T11:51:21"/>
   <userInfo guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" name="itluser" id="-446795219" dateTime="2018-04-13T11:51:26"/>
   <userInfo guid="{44866337-4EB8-44FB-BDBC-D3FE257C9028}" name="ITLAdmin" id="-2068734883" dateTime="2018-04-26T11:22:09"/>
   <userInfo guid="{95EE2E05-20D2-463A-8E2E-2247B0718DDE}" name="itluser" id="-446759165" dateTime="2018-04-26T11:51:19"/>
   <userInfo guid="{643B5170-02EC-4179-A42E-444C0001D79C}" name="itluser" id="-446801440" dateTime="2018-04-26T12:21:33"/>
+  <userInfo guid="{0D847394-68DB-4FEB-828F-2A6960EA0820}" name="ITL-USER" id="-1580107082" dateTime="2018-05-07T15:13:24"/>
 </users>
 </file>
 
@@ -9629,12 +11033,12 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="9.42578125" customWidth="1"/>
@@ -9723,7 +11127,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -9737,7 +11141,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -9751,7 +11155,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -9784,104 +11188,371 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="G9" sqref="G9"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="A3" sqref="A3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="A2" sqref="A2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
+      <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:AH3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AH2" sqref="AH2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="26.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="39.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="37.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="36" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="32" style="15" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="30" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="32.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>295</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>299</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>306</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="N1" t="s">
+        <v>314</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="R1" t="s">
+        <v>322</v>
+      </c>
+      <c r="S1" t="s">
+        <v>323</v>
+      </c>
+      <c r="T1" t="s">
+        <v>324</v>
+      </c>
+      <c r="U1" t="s">
+        <v>325</v>
+      </c>
+      <c r="V1" t="s">
+        <v>326</v>
+      </c>
+      <c r="W1" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="X1" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>329</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>330</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>331</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>332</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>333</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>334</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>335</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>336</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>337</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="J2" s="14"/>
+      <c r="O2" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>321</v>
+      </c>
+      <c r="W2" s="15">
+        <v>26000</v>
+      </c>
+      <c r="X2" s="15">
+        <v>2000</v>
+      </c>
+      <c r="AB2">
+        <v>10</v>
+      </c>
+      <c r="AC2">
+        <v>10</v>
+      </c>
+      <c r="AD2">
+        <v>12</v>
+      </c>
+      <c r="AE2">
+        <v>11</v>
+      </c>
+      <c r="AF2">
+        <v>10</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>338</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="P3" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>321</v>
+      </c>
+    </row>
+  </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="AC1">
+      <selection activeCell="AH2" sqref="AH2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="D11" sqref="D11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+      <selection activeCell="E11" sqref="E11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>255</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>296</v>
-      </c>
-      <c r="H1" s="14"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="15" t="s">
         <v>184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>239</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>230</v>
-      </c>
-      <c r="F4" t="s">
-        <v>256</v>
-      </c>
-      <c r="G4" t="s">
-        <v>256</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="D11" sqref="D11"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -9941,11 +11612,16 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="K12" sqref="K12"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="K12" sqref="K12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+      <selection activeCell="K12" sqref="K12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -9957,8 +11633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10048,19 +11724,19 @@
         <v>254</v>
       </c>
       <c r="U1" t="s">
+        <v>255</v>
+      </c>
+      <c r="V1" t="s">
+        <v>256</v>
+      </c>
+      <c r="W1" t="s">
         <v>257</v>
       </c>
-      <c r="V1" t="s">
-        <v>258</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>259</v>
       </c>
-      <c r="X1" t="s">
-        <v>261</v>
-      </c>
       <c r="Y1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -10097,6 +11773,10 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="O1">
+      <selection activeCell="Y1" sqref="Y1"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="D2" sqref="D2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10114,8 +11794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE2"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10451,19 +12131,24 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="V1">
+      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="J1">
       <selection activeCell="U3" sqref="U3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="V1">
       <selection activeCell="AA1" sqref="AA1:AA1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
+      <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -10471,8 +12156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT25"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AT1" sqref="AT1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10544,22 +12229,22 @@
         <v>87</v>
       </c>
       <c r="T1" s="11" t="s">
+        <v>270</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>271</v>
+      </c>
+      <c r="V1" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="W1" s="11" t="s">
         <v>273</v>
-      </c>
-      <c r="V1" s="11" t="s">
-        <v>274</v>
-      </c>
-      <c r="W1" s="11" t="s">
-        <v>275</v>
       </c>
       <c r="X1" s="11" t="s">
         <v>233</v>
       </c>
       <c r="Y1" s="11" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="Z1" s="11" t="s">
         <v>234</v>
@@ -10574,55 +12259,55 @@
         <v>237</v>
       </c>
       <c r="AD1" s="11" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="AE1" s="11" t="s">
         <v>238</v>
       </c>
       <c r="AF1" s="11" t="s">
+        <v>276</v>
+      </c>
+      <c r="AG1" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="AH1" s="11" t="s">
         <v>278</v>
       </c>
-      <c r="AG1" s="11" t="s">
+      <c r="AI1" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="AH1" s="11" t="s">
+      <c r="AJ1" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="AI1" s="11" t="s">
+      <c r="AK1" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="AJ1" s="11" t="s">
+      <c r="AL1" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="AK1" s="11" t="s">
+      <c r="AM1" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="AL1" s="11" t="s">
+      <c r="AN1" s="11" t="s">
         <v>284</v>
       </c>
-      <c r="AM1" s="11" t="s">
+      <c r="AO1" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="AN1" s="11" t="s">
+      <c r="AP1" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="AO1" s="11" t="s">
+      <c r="AQ1" s="11" t="s">
         <v>287</v>
       </c>
-      <c r="AP1" s="11" t="s">
+      <c r="AR1" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="AQ1" s="11" t="s">
+      <c r="AS1" s="11" t="s">
         <v>289</v>
       </c>
-      <c r="AR1" s="11" t="s">
-        <v>290</v>
-      </c>
-      <c r="AS1" s="11" t="s">
-        <v>291</v>
-      </c>
       <c r="AT1" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
@@ -10809,7 +12494,7 @@
       <c r="AQ4" s="11"/>
       <c r="AR4" s="11"/>
       <c r="AS4" s="11" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="AT4" s="11"/>
     </row>
@@ -10819,7 +12504,7 @@
       </c>
       <c r="T5" s="11"/>
       <c r="U5" s="11" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="V5" s="11"/>
       <c r="W5" s="11"/>
@@ -10871,7 +12556,7 @@
         <v>0.67083333333333339</v>
       </c>
       <c r="AS5" s="11" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="AT5" s="11"/>
     </row>
@@ -10944,6 +12629,10 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="A3" sqref="A3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10961,7 +12650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q1" sqref="Q1:Y1"/>
     </sheetView>
   </sheetViews>
@@ -10975,13 +12664,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>263</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>265</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>217</v>
@@ -10993,19 +12682,19 @@
         <v>219</v>
       </c>
       <c r="H1" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>268</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>270</v>
       </c>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
@@ -11017,7 +12706,7 @@
         <v>220</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>221</v>
@@ -11052,7 +12741,7 @@
         <v>224</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>225</v>
@@ -11124,11 +12813,16 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="Q1" sqref="Q1:Y1"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="Q1" sqref="Q1:Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+      <selection activeCell="Q1" sqref="Q1:Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -11140,7 +12834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="W1" workbookViewId="0">
       <selection activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
@@ -11366,6 +13060,11 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="W1">
+      <selection activeCell="AI2" sqref="AI2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="AI2" sqref="AI2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11373,10 +13072,11 @@
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="W1">
       <selection activeCell="AI2" sqref="AI2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -11453,19 +13153,24 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="G1" sqref="G1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="G1" sqref="G1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+      <selection activeCell="G1" sqref="G1"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId3"/>
+    </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -11489,6 +13194,10 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="B1" sqref="B1"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ananth - Updated test data excel
</commit_message>
<xml_diff>
--- a/Basic Test Suite/TestData/TestData.xlsx
+++ b/Basic Test Suite/TestData/TestData.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="347">
   <si>
     <t>Flow Name</t>
   </si>
@@ -1057,6 +1057,24 @@
   </si>
   <si>
     <t>FOOD</t>
+  </si>
+  <si>
+    <t>YINV_103</t>
+  </si>
+  <si>
+    <t>UnitId</t>
+  </si>
+  <si>
+    <t>YINV_104</t>
+  </si>
+  <si>
+    <t>YINV_105</t>
+  </si>
+  <si>
+    <t>YINV_106</t>
+  </si>
+  <si>
+    <t>YINV_107</t>
   </si>
 </sst>
 </file>
@@ -1133,7 +1151,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{0D847394-68DB-4FEB-828F-2A6960EA0820}" diskRevisions="1" revisionId="574" version="156">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{DA9B9AA6-9824-4498-8B11-67108356B4C6}" diskRevisions="1" revisionId="699" version="169">
   <header guid="{0C6C8E69-ABD3-4A89-B740-FE71B52466B3}" dateTime="2018-04-13T11:32:52" maxSheetId="9" userName="itluser" r:id="rId1">
     <sheetIdMap count="8">
       <sheetId val="1"/>
@@ -3245,6 +3263,201 @@
     </sheetIdMap>
   </header>
   <header guid="{0D847394-68DB-4FEB-828F-2A6960EA0820}" dateTime="2018-05-07T17:33:18" maxSheetId="12" userName="ITL-USER" r:id="rId156" minRId="574">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{367A61BB-AE66-4CA6-B1D0-4C333D870C97}" dateTime="2018-05-08T12:10:59" maxSheetId="12" userName="ITL-USER" r:id="rId157" minRId="575" maxRId="588">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{FE2144F4-D788-49F4-90A7-B537CF7B53AA}" dateTime="2018-05-08T12:12:26" maxSheetId="12" userName="ITL-USER" r:id="rId158" minRId="589">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{225788DB-C5D6-433D-BE07-3B814C3CDD52}" dateTime="2018-05-08T14:23:29" maxSheetId="12" userName="ITL-USER" r:id="rId159" minRId="590" maxRId="592">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{D364C1FA-D153-48D2-90E8-4A2B95349BD8}" dateTime="2018-05-08T15:57:06" maxSheetId="12" userName="itluser" r:id="rId160" minRId="593">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{4AD15B65-EDF4-441E-A579-F0CB076CE2A8}" dateTime="2018-05-08T15:57:54" maxSheetId="12" userName="ITL-USER" r:id="rId161" minRId="594" maxRId="609">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{E50C86A3-BFD1-4DC3-9E99-A30860AC5C11}" dateTime="2018-05-08T16:04:42" maxSheetId="12" userName="ITL-USER" r:id="rId162" minRId="610" maxRId="626">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{866BF670-6FDB-4811-95C1-C3B53501848D}" dateTime="2018-05-09T11:13:45" maxSheetId="12" userName="ITL-USER" r:id="rId163" minRId="627" maxRId="638">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{682B8145-0A24-41E9-A272-B2694C98A17F}" dateTime="2018-05-09T11:13:58" maxSheetId="12" userName="ITL-USER" r:id="rId164" minRId="639" maxRId="640">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{BBA348C1-519C-4CA7-A502-674492F771E8}" dateTime="2018-05-09T11:18:52" maxSheetId="12" userName="ITL-USER" r:id="rId165" minRId="641" maxRId="656">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{4CEB6B81-995E-4817-A148-6F400EA4F2EE}" dateTime="2018-05-09T11:44:27" maxSheetId="12" userName="ITL-USER" r:id="rId166" minRId="657" maxRId="672">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{1DCFD4B7-3B3F-4269-A3C5-29575ADC77A6}" dateTime="2018-05-09T11:44:55" maxSheetId="12" userName="ITL-USER" r:id="rId167" minRId="673" maxRId="680">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{32CAEBC9-0199-4828-97A3-A0211B344A98}" dateTime="2018-05-09T11:48:05" maxSheetId="12" userName="ITL-USER" r:id="rId168" minRId="681" maxRId="688">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{DA9B9AA6-9824-4498-8B11-67108356B4C6}" dateTime="2018-05-09T11:49:35" maxSheetId="12" userName="ITL-USER" r:id="rId169" minRId="689" maxRId="699">
     <sheetIdMap count="11">
       <sheetId val="1"/>
       <sheetId val="9"/>
@@ -8955,12 +9168,1045 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog157.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="575" sId="10" odxf="1">
+    <nc r="A4" t="inlineStr">
+      <is>
+        <t>YINV_103</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="576" sId="10" odxf="1">
+    <nc r="B4" t="inlineStr">
+      <is>
+        <t>admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="577" sId="10" odxf="1">
+    <nc r="C4" t="inlineStr">
+      <is>
+        <t>Admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="578" sId="10" odxf="1">
+    <nc r="D4" t="inlineStr">
+      <is>
+        <t>OPR1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="579" sId="10" odxf="1">
+    <nc r="E4" t="inlineStr">
+      <is>
+        <t>CPX11</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="580" sId="10" odxf="1">
+    <nc r="F4" t="inlineStr">
+      <is>
+        <t>FCY111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="581" sId="10" odxf="1">
+    <nc r="G4" t="inlineStr">
+      <is>
+        <t>YRD1111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="582" sId="10" odxf="1">
+    <nc r="H4" t="inlineStr">
+      <is>
+        <t>Yard Inventory</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="583" sId="10" odxf="1">
+    <nc r="I4" t="inlineStr">
+      <is>
+        <t>Query</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="584" sId="10" odxf="1">
+    <nc r="J4" t="inlineStr">
+      <is>
+        <t>SBSU1234571</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="585" sId="10">
+    <nc r="K4" t="inlineStr">
+      <is>
+        <t>S1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="586" sId="10">
+    <nc r="L4" t="inlineStr">
+      <is>
+        <t>S2</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="587" sId="10">
+    <nc r="M4" t="inlineStr">
+      <is>
+        <t>S3</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="588" sId="10" odxf="1">
+    <nc r="N4" t="inlineStr">
+      <is>
+        <t>S4</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog158.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="589" sId="10">
+    <oc r="J4" t="inlineStr">
+      <is>
+        <t>SBSU1234571</t>
+      </is>
+    </oc>
+    <nc r="J4" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog159.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="590" sId="8" odxf="1">
+    <nc r="B1" t="inlineStr">
+      <is>
+        <t>UnitId</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="591" sId="8" odxf="1">
+    <nc r="A2" t="inlineStr">
+      <is>
+        <t>YINV_103</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="592" sId="8" odxf="1">
+    <nc r="B2" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog16.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="18" sId="3">
     <nc r="Z2">
       <v>16641</v>
     </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog160.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="593" sId="1" odxf="1">
+    <nc r="A11" t="inlineStr">
+      <is>
+        <t>YINV_101</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog161.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="594" sId="1" odxf="1">
+    <nc r="A10" t="inlineStr">
+      <is>
+        <t>N4MobileCommonRoutines</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="595" sId="1" odxf="1">
+    <nc r="B10" t="inlineStr">
+      <is>
+        <t>admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="596" sId="1" odxf="1">
+    <nc r="C10" t="inlineStr">
+      <is>
+        <t>Admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="597" sId="1" odxf="1">
+    <nc r="D10" t="inlineStr">
+      <is>
+        <t>OPR1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="598" sId="1" odxf="1">
+    <nc r="E10" t="inlineStr">
+      <is>
+        <t>CPX11</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="599" sId="1" odxf="1">
+    <nc r="F10" t="inlineStr">
+      <is>
+        <t>FCY111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="600" sId="1" odxf="1">
+    <nc r="G10" t="inlineStr">
+      <is>
+        <t>YRD1111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="601" sId="1" odxf="1">
+    <nc r="H10" t="inlineStr">
+      <is>
+        <t>Configuration</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="602" sId="1" odxf="1">
+    <nc r="A12" t="inlineStr">
+      <is>
+        <t>YINV_103</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="603" sId="1" odxf="1">
+    <nc r="B12" t="inlineStr">
+      <is>
+        <t>admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="604" sId="1" odxf="1">
+    <nc r="C12" t="inlineStr">
+      <is>
+        <t>Admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="605" sId="1" odxf="1">
+    <nc r="D12" t="inlineStr">
+      <is>
+        <t>OPR1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="606" sId="1" odxf="1">
+    <nc r="E12" t="inlineStr">
+      <is>
+        <t>CPX11</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="607" sId="1" odxf="1">
+    <nc r="F12" t="inlineStr">
+      <is>
+        <t>FCY111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="608" sId="1" odxf="1">
+    <nc r="G12" t="inlineStr">
+      <is>
+        <t>YRD1111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="609" sId="1" odxf="1">
+    <nc r="H12" t="inlineStr">
+      <is>
+        <t>Operations</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog162.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="610" sId="10" odxf="1">
+    <nc r="A5" t="inlineStr">
+      <is>
+        <t>YINV_104</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="611" sId="10" odxf="1">
+    <nc r="B5" t="inlineStr">
+      <is>
+        <t>admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="612" sId="10" odxf="1">
+    <nc r="C5" t="inlineStr">
+      <is>
+        <t>Admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="613" sId="10" odxf="1">
+    <nc r="D5" t="inlineStr">
+      <is>
+        <t>OPR1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="614" sId="10" odxf="1">
+    <nc r="E5" t="inlineStr">
+      <is>
+        <t>CPX11</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="615" sId="10" odxf="1">
+    <nc r="F5" t="inlineStr">
+      <is>
+        <t>FCY111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="616" sId="10" odxf="1">
+    <nc r="G5" t="inlineStr">
+      <is>
+        <t>YRD1111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="617" sId="10" odxf="1">
+    <nc r="H5" t="inlineStr">
+      <is>
+        <t>Yard Inventory</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="618" sId="10" odxf="1">
+    <nc r="I5" t="inlineStr">
+      <is>
+        <t>Query</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="619" sId="10" odxf="1">
+    <nc r="J5" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="620" sId="10">
+    <nc r="K5" t="inlineStr">
+      <is>
+        <t>S1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="621" sId="10">
+    <nc r="L5" t="inlineStr">
+      <is>
+        <t>S2</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="622" sId="10">
+    <nc r="M5" t="inlineStr">
+      <is>
+        <t>S3</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="623" sId="10" odxf="1">
+    <nc r="N5" t="inlineStr">
+      <is>
+        <t>S4</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="624" sId="10">
+    <nc r="O5" t="inlineStr">
+      <is>
+        <t>DOOR</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="625" sId="10">
+    <nc r="P5" t="inlineStr">
+      <is>
+        <t>DAT</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="626" sId="10">
+    <nc r="Q5" t="inlineStr">
+      <is>
+        <t>Major</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog163.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="627" sId="10" odxf="1">
+    <nc r="A6" t="inlineStr">
+      <is>
+        <t>YINV_105</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="628" sId="10" odxf="1">
+    <nc r="B6" t="inlineStr">
+      <is>
+        <t>admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="629" sId="10" odxf="1">
+    <nc r="C6" t="inlineStr">
+      <is>
+        <t>Admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="630" sId="10" odxf="1">
+    <nc r="D6" t="inlineStr">
+      <is>
+        <t>OPR1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="631" sId="10" odxf="1">
+    <nc r="E6" t="inlineStr">
+      <is>
+        <t>CPX11</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="632" sId="10" odxf="1">
+    <nc r="F6" t="inlineStr">
+      <is>
+        <t>FCY111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="633" sId="10" odxf="1">
+    <nc r="G6" t="inlineStr">
+      <is>
+        <t>YRD1111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="634" sId="10" odxf="1">
+    <nc r="H6" t="inlineStr">
+      <is>
+        <t>Yard Inventory</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="635" sId="10" odxf="1">
+    <nc r="I6" t="inlineStr">
+      <is>
+        <t>Query</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="636" sId="10" odxf="1">
+    <nc r="J6" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="637" sId="10">
+    <nc r="W6">
+      <v>26000</v>
+    </nc>
+  </rcc>
+  <rcc rId="638" sId="10">
+    <nc r="X6">
+      <v>2000</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog164.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="639" sId="1" eol="1" ref="A13:XFD13" action="insertRow"/>
+  <rcc rId="640" sId="1">
+    <nc r="A13" t="inlineStr">
+      <is>
+        <t>YINV_105</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog165.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="641" sId="1">
+    <oc r="A13" t="inlineStr">
+      <is>
+        <t>YINV_105</t>
+      </is>
+    </oc>
+    <nc r="A13" t="inlineStr">
+      <is>
+        <t>YINV_104</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="642" sId="1">
+    <nc r="B13" t="inlineStr">
+      <is>
+        <t>admin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="643" sId="1">
+    <nc r="C13" t="inlineStr">
+      <is>
+        <t>Admin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="644" sId="1">
+    <nc r="D13" t="inlineStr">
+      <is>
+        <t>OPR1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="645" sId="1">
+    <nc r="E13" t="inlineStr">
+      <is>
+        <t>CPX11</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="646" sId="1">
+    <nc r="F13" t="inlineStr">
+      <is>
+        <t>FCY111</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="647" sId="1">
+    <nc r="G13" t="inlineStr">
+      <is>
+        <t>YRD1111</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="648" sId="1">
+    <nc r="H13" t="inlineStr">
+      <is>
+        <t>Operations</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="649" sId="1" odxf="1">
+    <nc r="A14" t="inlineStr">
+      <is>
+        <t>YINV_105</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="650" sId="1" odxf="1">
+    <nc r="B14" t="inlineStr">
+      <is>
+        <t>admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="651" sId="1" odxf="1">
+    <nc r="C14" t="inlineStr">
+      <is>
+        <t>Admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="652" sId="1" odxf="1">
+    <nc r="D14" t="inlineStr">
+      <is>
+        <t>OPR1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="653" sId="1" odxf="1">
+    <nc r="E14" t="inlineStr">
+      <is>
+        <t>CPX11</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="654" sId="1" odxf="1">
+    <nc r="F14" t="inlineStr">
+      <is>
+        <t>FCY111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="655" sId="1" odxf="1">
+    <nc r="G14" t="inlineStr">
+      <is>
+        <t>YRD1111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="656" sId="1" odxf="1">
+    <nc r="H14" t="inlineStr">
+      <is>
+        <t>Operations</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog166.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="657" sId="10" odxf="1">
+    <nc r="A7" t="inlineStr">
+      <is>
+        <t>YINV_106</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="658" sId="10" odxf="1">
+    <nc r="B7" t="inlineStr">
+      <is>
+        <t>admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="659" sId="10" odxf="1">
+    <nc r="C7" t="inlineStr">
+      <is>
+        <t>Admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="660" sId="10" odxf="1">
+    <nc r="D7" t="inlineStr">
+      <is>
+        <t>OPR1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="661" sId="10" odxf="1">
+    <nc r="E7" t="inlineStr">
+      <is>
+        <t>CPX11</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="662" sId="10" odxf="1">
+    <nc r="F7" t="inlineStr">
+      <is>
+        <t>FCY111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="663" sId="10" odxf="1">
+    <nc r="G7" t="inlineStr">
+      <is>
+        <t>YRD1111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="664" sId="10" odxf="1">
+    <nc r="H7" t="inlineStr">
+      <is>
+        <t>Yard Inventory</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="665" sId="10" odxf="1">
+    <nc r="I7" t="inlineStr">
+      <is>
+        <t>Query</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="666" sId="10" odxf="1">
+    <nc r="J7" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="667" sId="10" odxf="1">
+    <nc r="AB7">
+      <v>10</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="668" sId="10" odxf="1">
+    <nc r="AC7">
+      <v>11</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="669" sId="10" odxf="1">
+    <nc r="AD7">
+      <v>12</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="670" sId="10" odxf="1">
+    <nc r="AE7">
+      <v>13</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="671" sId="10" odxf="1">
+    <nc r="AF7">
+      <v>10</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="672" sId="10" odxf="1">
+    <nc r="AG7" t="inlineStr">
+      <is>
+        <t>cm</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog167.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="673" sId="1" odxf="1">
+    <nc r="A15" t="inlineStr">
+      <is>
+        <t>YINV_106</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="674" sId="1" odxf="1">
+    <nc r="B15" t="inlineStr">
+      <is>
+        <t>admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="675" sId="1" odxf="1">
+    <nc r="C15" t="inlineStr">
+      <is>
+        <t>Admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="676" sId="1" odxf="1">
+    <nc r="D15" t="inlineStr">
+      <is>
+        <t>OPR1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="677" sId="1" odxf="1">
+    <nc r="E15" t="inlineStr">
+      <is>
+        <t>CPX11</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="678" sId="1" odxf="1">
+    <nc r="F15" t="inlineStr">
+      <is>
+        <t>FCY111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="679" sId="1" odxf="1">
+    <nc r="G15" t="inlineStr">
+      <is>
+        <t>YRD1111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="680" sId="1" odxf="1">
+    <nc r="H15" t="inlineStr">
+      <is>
+        <t>Operations</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog168.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="681" sId="1" odxf="1">
+    <nc r="A16" t="inlineStr">
+      <is>
+        <t>YINV_107</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="682" sId="1" odxf="1">
+    <nc r="B16" t="inlineStr">
+      <is>
+        <t>admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="683" sId="1" odxf="1">
+    <nc r="C16" t="inlineStr">
+      <is>
+        <t>Admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="684" sId="1" odxf="1">
+    <nc r="D16" t="inlineStr">
+      <is>
+        <t>OPR1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="685" sId="1" odxf="1">
+    <nc r="E16" t="inlineStr">
+      <is>
+        <t>CPX11</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="686" sId="1" odxf="1">
+    <nc r="F16" t="inlineStr">
+      <is>
+        <t>FCY111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="687" sId="1" odxf="1">
+    <nc r="G16" t="inlineStr">
+      <is>
+        <t>YRD1111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="688" sId="1" odxf="1">
+    <nc r="H16" t="inlineStr">
+      <is>
+        <t>Operations</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog169.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="689" sId="10" odxf="1">
+    <nc r="A8" t="inlineStr">
+      <is>
+        <t>YINV_107</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="690" sId="10" odxf="1">
+    <nc r="B8" t="inlineStr">
+      <is>
+        <t>admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="691" sId="10" odxf="1">
+    <nc r="C8" t="inlineStr">
+      <is>
+        <t>Admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="692" sId="10" odxf="1">
+    <nc r="D8" t="inlineStr">
+      <is>
+        <t>OPR1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="693" sId="10" odxf="1">
+    <nc r="E8" t="inlineStr">
+      <is>
+        <t>CPX11</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="694" sId="10" odxf="1">
+    <nc r="F8" t="inlineStr">
+      <is>
+        <t>FCY111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="695" sId="10" odxf="1">
+    <nc r="G8" t="inlineStr">
+      <is>
+        <t>YRD1111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="696" sId="10" odxf="1">
+    <nc r="H8" t="inlineStr">
+      <is>
+        <t>Yard Inventory</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="697" sId="10" odxf="1">
+    <nc r="I8" t="inlineStr">
+      <is>
+        <t>Query</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="698" sId="10" odxf="1">
+    <nc r="J8" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="699" sId="10" odxf="1">
+    <nc r="AH8" t="inlineStr">
+      <is>
+        <t>FOOD</t>
+      </is>
+    </nc>
+    <odxf/>
   </rcc>
 </revisions>
 </file>
@@ -10756,14 +12002,14 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="6">
   <userInfo guid="{0FC3EEC7-1253-40C9-80FE-72015618EED8}" name="ITLAdmin" id="-2068730528" dateTime="2018-04-13T11:51:21"/>
   <userInfo guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" name="itluser" id="-446795219" dateTime="2018-04-13T11:51:26"/>
   <userInfo guid="{44866337-4EB8-44FB-BDBC-D3FE257C9028}" name="ITLAdmin" id="-2068734883" dateTime="2018-04-26T11:22:09"/>
   <userInfo guid="{95EE2E05-20D2-463A-8E2E-2247B0718DDE}" name="itluser" id="-446759165" dateTime="2018-04-26T11:51:19"/>
   <userInfo guid="{643B5170-02EC-4179-A42E-444C0001D79C}" name="itluser" id="-446801440" dateTime="2018-04-26T12:21:33"/>
-  <userInfo guid="{0D847394-68DB-4FEB-828F-2A6960EA0820}" name="ITL-USER" id="-1580107082" dateTime="2018-05-07T15:13:24"/>
+  <userInfo guid="{D364C1FA-D153-48D2-90E8-4A2B95349BD8}" name="itluser" id="-446801266" dateTime="2018-05-08T15:56:31"/>
 </users>
 </file>
 
@@ -11030,10 +12276,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B16" sqref="B16:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11183,6 +12429,174 @@
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
       <c r="H9" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>308</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="15" t="s">
         <v>132</v>
       </c>
     </row>
@@ -11211,10 +12625,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH3"/>
+  <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AH2" sqref="AH2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11475,6 +12889,256 @@
         <v>321</v>
       </c>
     </row>
+    <row r="4" spans="1:34" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="N5" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="O5" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="P5" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q5" s="15" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="N6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15">
+        <v>26000</v>
+      </c>
+      <c r="X6" s="15">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="N7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="15"/>
+      <c r="AB7" s="15">
+        <v>10</v>
+      </c>
+      <c r="AC7" s="15">
+        <v>11</v>
+      </c>
+      <c r="AD7" s="15">
+        <v>12</v>
+      </c>
+      <c r="AE7" s="15">
+        <v>13</v>
+      </c>
+      <c r="AF7" s="15">
+        <v>10</v>
+      </c>
+      <c r="AG7" s="15" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="N8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
+      <c r="AA8" s="15"/>
+      <c r="AB8" s="15"/>
+      <c r="AC8" s="15"/>
+      <c r="AD8" s="15"/>
+      <c r="AE8" s="15"/>
+      <c r="AF8" s="15"/>
+      <c r="AG8" s="15"/>
+      <c r="AH8" s="15" t="s">
+        <v>340</v>
+      </c>
+    </row>
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="AC1">
@@ -11499,7 +13163,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13176,20 +14840,32 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ananth - Updated method "fetchData" in file name CommonRoutines for creating dictionary and mapping key value Also have updated test data excel
</commit_message>
<xml_diff>
--- a/Basic Test Suite/TestData/TestData.xlsx
+++ b/Basic Test Suite/TestData/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7155" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="SparcsN4Login" sheetId="1" r:id="rId1"/>
@@ -26,15 +26,15 @@
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="ITLAdmin - Personal View" guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1362" windowHeight="503" activeSheetId="11"/>
+    <customWorkbookView name="itluser - Personal View" guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="5"/>
     <customWorkbookView name="ITL-USER - Personal View" guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1380" windowHeight="744" activeSheetId="10"/>
-    <customWorkbookView name="itluser - Personal View" guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="5"/>
-    <customWorkbookView name="ITLAdmin - Personal View" guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1362" windowHeight="503" activeSheetId="11"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="348">
   <si>
     <t>Flow Name</t>
   </si>
@@ -1075,6 +1075,9 @@
   </si>
   <si>
     <t>YINV_107</t>
+  </si>
+  <si>
+    <t>YINV_102</t>
   </si>
 </sst>
 </file>
@@ -1151,7 +1154,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{DA9B9AA6-9824-4498-8B11-67108356B4C6}" diskRevisions="1" revisionId="699" version="169">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{34246483-AB61-4467-BA99-A34781EAEA0F}" diskRevisions="1" revisionId="738" version="172">
   <header guid="{0C6C8E69-ABD3-4A89-B740-FE71B52466B3}" dateTime="2018-04-13T11:32:52" maxSheetId="9" userName="itluser" r:id="rId1">
     <sheetIdMap count="8">
       <sheetId val="1"/>
@@ -3458,6 +3461,51 @@
     </sheetIdMap>
   </header>
   <header guid="{DA9B9AA6-9824-4498-8B11-67108356B4C6}" dateTime="2018-05-09T11:49:35" maxSheetId="12" userName="ITL-USER" r:id="rId169" minRId="689" maxRId="699">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{39280401-B48C-4FAF-9943-A0A000BD6D3C}" dateTime="2018-05-11T12:28:18" maxSheetId="12" userName="ITL-USER" r:id="rId170" minRId="700" maxRId="710">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5B87912C-1671-4BED-81EB-CBBF172E41FE}" dateTime="2018-05-11T12:28:40" maxSheetId="12" userName="ITL-USER" r:id="rId171" minRId="711" maxRId="718">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{34246483-AB61-4467-BA99-A34781EAEA0F}" dateTime="2018-05-11T12:29:57" maxSheetId="12" userName="ITL-USER" r:id="rId172" minRId="719" maxRId="738">
     <sheetIdMap count="11">
       <sheetId val="1"/>
       <sheetId val="9"/>
@@ -10235,6 +10283,321 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog170.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="700" sId="10" ref="A4:XFD4" action="insertRow"/>
+  <rcc rId="701" sId="10">
+    <nc r="A4" t="inlineStr">
+      <is>
+        <t>YINV_102</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="702" sId="10">
+    <nc r="B4" t="inlineStr">
+      <is>
+        <t>admin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="703" sId="10">
+    <nc r="C4" t="inlineStr">
+      <is>
+        <t>Admin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="704" sId="10">
+    <nc r="D4" t="inlineStr">
+      <is>
+        <t>OPR1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="705" sId="10">
+    <nc r="E4" t="inlineStr">
+      <is>
+        <t>CPX11</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="706" sId="10">
+    <nc r="F4" t="inlineStr">
+      <is>
+        <t>FCY111</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="707" sId="10">
+    <nc r="G4" t="inlineStr">
+      <is>
+        <t>YRD1111</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="708" sId="10">
+    <nc r="H4" t="inlineStr">
+      <is>
+        <t>Yard Inventory</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="709" sId="10">
+    <nc r="I4" t="inlineStr">
+      <is>
+        <t>Query</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="710" sId="10">
+    <nc r="J4" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog171.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="711" sId="8">
+    <nc r="A3" t="inlineStr">
+      <is>
+        <t>YINV_104</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="712" sId="8">
+    <nc r="B3" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="713" sId="8">
+    <nc r="A4" t="inlineStr">
+      <is>
+        <t>YINV_105</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="714" sId="8">
+    <nc r="B4" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="715" sId="8">
+    <nc r="A5" t="inlineStr">
+      <is>
+        <t>YINV_106</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="716" sId="8">
+    <nc r="B5" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="717" sId="8">
+    <nc r="A6" t="inlineStr">
+      <is>
+        <t>YINV_107</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="718" sId="8">
+    <nc r="B6" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog172.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="719" sId="1">
+    <nc r="B11" t="inlineStr">
+      <is>
+        <t>admin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="720" sId="1">
+    <nc r="C11" t="inlineStr">
+      <is>
+        <t>Admin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="721" sId="1">
+    <nc r="D11" t="inlineStr">
+      <is>
+        <t>OPR1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="722" sId="1">
+    <nc r="E11" t="inlineStr">
+      <is>
+        <t>CPX11</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="723" sId="1">
+    <nc r="F11" t="inlineStr">
+      <is>
+        <t>FCY111</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="724" sId="1">
+    <nc r="G11" t="inlineStr">
+      <is>
+        <t>YRD1111</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="725" sId="1">
+    <nc r="H11" t="inlineStr">
+      <is>
+        <t>Operations</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="726" sId="1">
+    <oc r="A12" t="inlineStr">
+      <is>
+        <t>YINV_103</t>
+      </is>
+    </oc>
+    <nc r="A12" t="inlineStr">
+      <is>
+        <t>YINV_102</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="727" sId="1">
+    <oc r="A13" t="inlineStr">
+      <is>
+        <t>YINV_104</t>
+      </is>
+    </oc>
+    <nc r="A13" t="inlineStr">
+      <is>
+        <t>YINV_103</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="728" sId="1">
+    <oc r="A14" t="inlineStr">
+      <is>
+        <t>YINV_105</t>
+      </is>
+    </oc>
+    <nc r="A14" t="inlineStr">
+      <is>
+        <t>YINV_104</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="729" sId="1">
+    <oc r="A15" t="inlineStr">
+      <is>
+        <t>YINV_106</t>
+      </is>
+    </oc>
+    <nc r="A15" t="inlineStr">
+      <is>
+        <t>YINV_105</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="730" sId="1">
+    <oc r="A16" t="inlineStr">
+      <is>
+        <t>YINV_107</t>
+      </is>
+    </oc>
+    <nc r="A16" t="inlineStr">
+      <is>
+        <t>YINV_106</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="731" sId="1" odxf="1">
+    <nc r="A17" t="inlineStr">
+      <is>
+        <t>YINV_107</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="732" sId="1" odxf="1">
+    <nc r="B17" t="inlineStr">
+      <is>
+        <t>admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="733" sId="1" odxf="1">
+    <nc r="C17" t="inlineStr">
+      <is>
+        <t>Admin</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="734" sId="1" odxf="1">
+    <nc r="D17" t="inlineStr">
+      <is>
+        <t>OPR1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="735" sId="1" odxf="1">
+    <nc r="E17" t="inlineStr">
+      <is>
+        <t>CPX11</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="736" sId="1" odxf="1">
+    <nc r="F17" t="inlineStr">
+      <is>
+        <t>FCY111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="737" sId="1" odxf="1">
+    <nc r="G17" t="inlineStr">
+      <is>
+        <t>YRD1111</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="738" sId="1" odxf="1">
+    <nc r="H17" t="inlineStr">
+      <is>
+        <t>Operations</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog18.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcv guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" action="delete"/>
@@ -12002,14 +12365,15 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="6">
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="7">
   <userInfo guid="{0FC3EEC7-1253-40C9-80FE-72015618EED8}" name="ITLAdmin" id="-2068730528" dateTime="2018-04-13T11:51:21"/>
   <userInfo guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" name="itluser" id="-446795219" dateTime="2018-04-13T11:51:26"/>
   <userInfo guid="{44866337-4EB8-44FB-BDBC-D3FE257C9028}" name="ITLAdmin" id="-2068734883" dateTime="2018-04-26T11:22:09"/>
   <userInfo guid="{95EE2E05-20D2-463A-8E2E-2247B0718DDE}" name="itluser" id="-446759165" dateTime="2018-04-26T11:51:19"/>
   <userInfo guid="{643B5170-02EC-4179-A42E-444C0001D79C}" name="itluser" id="-446801440" dateTime="2018-04-26T12:21:33"/>
   <userInfo guid="{D364C1FA-D153-48D2-90E8-4A2B95349BD8}" name="itluser" id="-446801266" dateTime="2018-05-08T15:56:31"/>
+  <userInfo guid="{34246483-AB61-4467-BA99-A34781EAEA0F}" name="ITL-USER" id="-1580131676" dateTime="2018-05-11T12:28:00"/>
 </users>
 </file>
 
@@ -12276,10 +12640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12462,17 +12826,31 @@
       <c r="A11" s="15" t="s">
         <v>308</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
+      <c r="B11" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>3</v>
@@ -12498,7 +12876,7 @@
     </row>
     <row r="13" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>3</v>
@@ -12524,7 +12902,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>3</v>
@@ -12550,7 +12928,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>3</v>
@@ -12576,7 +12954,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>3</v>
@@ -12597,13 +12975,39 @@
         <v>15</v>
       </c>
       <c r="H16" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="15" t="s">
         <v>132</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="G9" sqref="G9"/>
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+      <selection activeCell="A2" sqref="A2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -12612,8 +13016,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
-      <selection activeCell="A2" sqref="A2"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="G9" sqref="G9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -12625,10 +13029,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH8"/>
+  <dimension ref="A1:AH9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12891,7 +13295,7 @@
     </row>
     <row r="4" spans="1:34" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>3</v>
@@ -12920,22 +13324,10 @@
       <c r="J4" s="15" t="s">
         <v>309</v>
       </c>
-      <c r="K4" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>311</v>
-      </c>
-      <c r="M4" s="15" t="s">
-        <v>313</v>
-      </c>
-      <c r="N4" s="15" t="s">
-        <v>315</v>
-      </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>3</v>
@@ -12975,20 +13367,11 @@
       </c>
       <c r="N5" s="15" t="s">
         <v>315</v>
-      </c>
-      <c r="O5" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="P5" s="15" t="s">
-        <v>320</v>
-      </c>
-      <c r="Q5" s="15" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>3</v>
@@ -13017,22 +13400,31 @@
       <c r="J6" s="15" t="s">
         <v>309</v>
       </c>
-      <c r="N6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15">
-        <v>26000</v>
-      </c>
-      <c r="X6" s="15">
-        <v>2000</v>
+      <c r="K6" s="15" t="s">
+        <v>307</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="N6" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="P6" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q6" s="15" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>3</v>
@@ -13067,31 +13459,16 @@
       <c r="T7" s="15"/>
       <c r="U7" s="15"/>
       <c r="V7" s="15"/>
-      <c r="Y7" s="15"/>
-      <c r="Z7" s="15"/>
-      <c r="AA7" s="15"/>
-      <c r="AB7" s="15">
-        <v>10</v>
-      </c>
-      <c r="AC7" s="15">
-        <v>11</v>
-      </c>
-      <c r="AD7" s="15">
-        <v>12</v>
-      </c>
-      <c r="AE7" s="15">
-        <v>13</v>
-      </c>
-      <c r="AF7" s="15">
-        <v>10</v>
-      </c>
-      <c r="AG7" s="15" t="s">
-        <v>338</v>
+      <c r="W7" s="15">
+        <v>26000</v>
+      </c>
+      <c r="X7" s="15">
+        <v>2000</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>3</v>
@@ -13129,28 +13506,87 @@
       <c r="Y8" s="15"/>
       <c r="Z8" s="15"/>
       <c r="AA8" s="15"/>
-      <c r="AB8" s="15"/>
-      <c r="AC8" s="15"/>
-      <c r="AD8" s="15"/>
-      <c r="AE8" s="15"/>
-      <c r="AF8" s="15"/>
-      <c r="AG8" s="15"/>
-      <c r="AH8" s="15" t="s">
+      <c r="AB8" s="15">
+        <v>10</v>
+      </c>
+      <c r="AC8" s="15">
+        <v>11</v>
+      </c>
+      <c r="AD8" s="15">
+        <v>12</v>
+      </c>
+      <c r="AE8" s="15">
+        <v>13</v>
+      </c>
+      <c r="AF8" s="15">
+        <v>10</v>
+      </c>
+      <c r="AG8" s="15" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>305</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>309</v>
+      </c>
+      <c r="N9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="15"/>
+      <c r="AB9" s="15"/>
+      <c r="AC9" s="15"/>
+      <c r="AD9" s="15"/>
+      <c r="AE9" s="15"/>
+      <c r="AF9" s="15"/>
+      <c r="AG9" s="15"/>
+      <c r="AH9" s="15" t="s">
         <v>340</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="AC1">
-      <selection activeCell="AH2" sqref="AH2"/>
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+      <selection activeCell="E11" sqref="E11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="D11" sqref="D11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
-      <selection activeCell="E11" sqref="E11"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="AC1">
+      <selection activeCell="AH2" sqref="AH2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -13163,7 +13599,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13211,11 +13647,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -13276,7 +13712,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="K12" sqref="K12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -13284,7 +13720,7 @@
       <selection activeCell="K12" sqref="K12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="K12" sqref="K12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -13437,7 +13873,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="O1">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="O1">
       <selection activeCell="Y1" sqref="Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -13445,7 +13881,7 @@
       <selection activeCell="D2" sqref="D2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="O1">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="O1">
       <selection activeCell="Y1" sqref="Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -13795,7 +14231,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="V1">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="V1">
       <selection activeCell="AA1" sqref="AA1:AA1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13805,7 +14241,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="V1">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="V1">
       <selection activeCell="AA1" sqref="AA1:AA1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -14293,7 +14729,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="A3" sqref="A3:XFD3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -14301,7 +14737,7 @@
       <selection activeCell="A3" sqref="A3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="A3" sqref="A3:XFD3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -14477,7 +14913,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="Q1" sqref="Q1:Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -14485,7 +14921,7 @@
       <selection activeCell="Q1" sqref="Q1:Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="Q1" sqref="Q1:Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -14724,7 +15160,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="W1">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="W1">
       <selection activeCell="AI2" sqref="AI2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14733,7 +15169,7 @@
       <selection activeCell="AI2" sqref="AI2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="W1">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="W1">
       <selection activeCell="AI2" sqref="AI2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -14817,7 +15253,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="G1" sqref="G1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14827,7 +15263,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="G1" sqref="G1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -14840,10 +15276,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14868,9 +15304,41 @@
         <v>309</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>309</v>
+      </c>
+    </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -14878,7 +15346,7 @@
       <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>

</xml_diff>

<commit_message>
Ananth - Added sparchscript and SNX files inside project structure Updated Test data Excel
</commit_message>
<xml_diff>
--- a/Basic Test Suite/TestData/TestData.xlsx
+++ b/Basic Test Suite/TestData/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7155"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7755" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="SparcsN4Login" sheetId="1" r:id="rId1"/>
@@ -26,15 +26,15 @@
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="ITL-USER - Personal View" guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1380" windowHeight="744" activeSheetId="10"/>
+    <customWorkbookView name="itluser - Personal View" guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="5"/>
     <customWorkbookView name="ITLAdmin - Personal View" guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1362" windowHeight="503" activeSheetId="11"/>
-    <customWorkbookView name="itluser - Personal View" guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="5"/>
-    <customWorkbookView name="ITL-USER - Personal View" guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1380" windowHeight="744" activeSheetId="10"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="349">
   <si>
     <t>Flow Name</t>
   </si>
@@ -84,9 +84,6 @@
     <t>YRD1111</t>
   </si>
   <si>
-    <t>WorkMode</t>
-  </si>
-  <si>
     <t>PointID</t>
   </si>
   <si>
@@ -432,9 +429,6 @@
     <t>LineInsuranceExpiration</t>
   </si>
   <si>
-    <t>Operations</t>
-  </si>
-  <si>
     <t>ERONumber</t>
   </si>
   <si>
@@ -810,9 +804,6 @@
     <t>Standard</t>
   </si>
   <si>
-    <t>Configuration</t>
-  </si>
-  <si>
     <t>ReleaseNumber</t>
   </si>
   <si>
@@ -963,9 +954,6 @@
     <t>YINV_101</t>
   </si>
   <si>
-    <t>SBSU1234570</t>
-  </si>
-  <si>
     <t>n4YinvQueryContainerSeal2</t>
   </si>
   <si>
@@ -1078,6 +1066,21 @@
   </si>
   <si>
     <t>YINV_102</t>
+  </si>
+  <si>
+    <t>EquipmentToBeAttached</t>
+  </si>
+  <si>
+    <t>EquipmentRole</t>
+  </si>
+  <si>
+    <t>ASWU2705190</t>
+  </si>
+  <si>
+    <t>CHSASW</t>
+  </si>
+  <si>
+    <t>CARRIAGE</t>
   </si>
 </sst>
 </file>
@@ -1119,7 +1122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1134,7 +1137,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1154,7 +1156,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{34246483-AB61-4467-BA99-A34781EAEA0F}" diskRevisions="1" revisionId="738" version="172">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{82F04F4E-022D-4926-A8A5-D79C201A90FA}" diskRevisions="1" revisionId="769" version="174">
   <header guid="{0C6C8E69-ABD3-4A89-B740-FE71B52466B3}" dateTime="2018-04-13T11:32:52" maxSheetId="9" userName="itluser" r:id="rId1">
     <sheetIdMap count="8">
       <sheetId val="1"/>
@@ -3506,6 +3508,36 @@
     </sheetIdMap>
   </header>
   <header guid="{34246483-AB61-4467-BA99-A34781EAEA0F}" dateTime="2018-05-11T12:29:57" maxSheetId="12" userName="ITL-USER" r:id="rId172" minRId="719" maxRId="738">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{CE6373AA-7A1D-49D9-80D0-06E398DFAE9D}" dateTime="2018-05-22T11:32:10" maxSheetId="12" userName="ITL-USER" r:id="rId173" minRId="739" maxRId="757">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{82F04F4E-022D-4926-A8A5-D79C201A90FA}" dateTime="2018-05-22T11:32:37" maxSheetId="12" userName="ITL-USER" r:id="rId174" minRId="758" maxRId="769">
     <sheetIdMap count="11">
       <sheetId val="1"/>
       <sheetId val="9"/>
@@ -10598,6 +10630,432 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog173.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="739" sId="1" ref="H1:H1048576" action="deleteCol">
+    <rfmt sheetId="1" xfDxf="1" sqref="H1:H1048576" start="0" length="0"/>
+    <rcc rId="0" sId="1">
+      <nc r="H1" t="inlineStr">
+        <is>
+          <t>WorkMode</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="1">
+      <nc r="H2" t="inlineStr">
+        <is>
+          <t>Operations</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="1">
+      <nc r="H4" t="inlineStr">
+        <is>
+          <t>Operations</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="1">
+      <nc r="H5" t="inlineStr">
+        <is>
+          <t>Configuration</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="1">
+      <nc r="H6" t="inlineStr">
+        <is>
+          <t>Configuration</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="1">
+      <nc r="H7" t="inlineStr">
+        <is>
+          <t>Configuration</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="1">
+      <nc r="H8" t="inlineStr">
+        <is>
+          <t>Operations</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="1">
+      <nc r="H9" t="inlineStr">
+        <is>
+          <t>Operations</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="1">
+      <nc r="H10" t="inlineStr">
+        <is>
+          <t>Configuration</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="1">
+      <nc r="H11" t="inlineStr">
+        <is>
+          <t>Operations</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="1">
+      <nc r="H12" t="inlineStr">
+        <is>
+          <t>Operations</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="1">
+      <nc r="H13" t="inlineStr">
+        <is>
+          <t>Operations</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="1">
+      <nc r="H14" t="inlineStr">
+        <is>
+          <t>Operations</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="1">
+      <nc r="H15" t="inlineStr">
+        <is>
+          <t>Operations</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="1">
+      <nc r="H16" t="inlineStr">
+        <is>
+          <t>Operations</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="1">
+      <nc r="H17" t="inlineStr">
+        <is>
+          <t>Operations</t>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+  <rcc rId="740" sId="8" odxf="1">
+    <nc r="C1" t="inlineStr">
+      <is>
+        <t>EquipmentToBeAttached</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="741" sId="8" odxf="1">
+    <nc r="D1" t="inlineStr">
+      <is>
+        <t>EquipmentRole</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="742" sId="8">
+    <oc r="A2" t="inlineStr">
+      <is>
+        <t>YINV_103</t>
+      </is>
+    </oc>
+    <nc r="A2" t="inlineStr">
+      <is>
+        <t>YINV_101</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="743" sId="8">
+    <oc r="B2" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </oc>
+    <nc r="B2" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="744" sId="8">
+    <oc r="A3" t="inlineStr">
+      <is>
+        <t>YINV_104</t>
+      </is>
+    </oc>
+    <nc r="A3" t="inlineStr">
+      <is>
+        <t>YINV_102</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="745" sId="8">
+    <oc r="B3" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </oc>
+    <nc r="B3" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="746" sId="8" odxf="1">
+    <nc r="C3" t="inlineStr">
+      <is>
+        <t>CHSASW</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="747" sId="8" odxf="1">
+    <nc r="D3" t="inlineStr">
+      <is>
+        <t>CARRIAGE</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="748" sId="8">
+    <oc r="A4" t="inlineStr">
+      <is>
+        <t>YINV_105</t>
+      </is>
+    </oc>
+    <nc r="A4" t="inlineStr">
+      <is>
+        <t>YINV_103</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="749" sId="8">
+    <oc r="B4" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </oc>
+    <nc r="B4" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="750" sId="8">
+    <oc r="A5" t="inlineStr">
+      <is>
+        <t>YINV_106</t>
+      </is>
+    </oc>
+    <nc r="A5" t="inlineStr">
+      <is>
+        <t>YINV_104</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="751" sId="8">
+    <oc r="B5" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </oc>
+    <nc r="B5" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="752" sId="8">
+    <oc r="A6" t="inlineStr">
+      <is>
+        <t>YINV_107</t>
+      </is>
+    </oc>
+    <nc r="A6" t="inlineStr">
+      <is>
+        <t>YINV_105</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="753" sId="8">
+    <oc r="B6" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </oc>
+    <nc r="B6" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="754" sId="8">
+    <nc r="A7" t="inlineStr">
+      <is>
+        <t>YINV_106</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="755" sId="8">
+    <nc r="B7" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="756" sId="8">
+    <nc r="A8" t="inlineStr">
+      <is>
+        <t>YINV_107</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="757" sId="8">
+    <nc r="B8" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog174.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="758" sId="10" odxf="1">
+    <nc r="J2" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="759" sId="10">
+    <nc r="K2" t="inlineStr">
+      <is>
+        <t>S1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="760" sId="10">
+    <nc r="L2" t="inlineStr">
+      <is>
+        <t>S2</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="761" sId="10">
+    <nc r="M2" t="inlineStr">
+      <is>
+        <t>S3</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="762" sId="10" odxf="1">
+    <nc r="N2" t="inlineStr">
+      <is>
+        <t>S4</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="763" sId="10">
+    <oc r="J3" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </oc>
+    <nc r="J3" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="764" sId="10">
+    <oc r="J4" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </oc>
+    <nc r="J4" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="765" sId="10">
+    <oc r="J5" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </oc>
+    <nc r="J5" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="766" sId="10">
+    <oc r="J6" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </oc>
+    <nc r="J6" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="767" sId="10">
+    <oc r="J7" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </oc>
+    <nc r="J7" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="768" sId="10">
+    <oc r="J8" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </oc>
+    <nc r="J8" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="769" sId="10">
+    <oc r="J9" t="inlineStr">
+      <is>
+        <t>SBSU1234570</t>
+      </is>
+    </oc>
+    <nc r="J9" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog18.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcv guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" action="delete"/>
@@ -12366,7 +12824,7 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="7">
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="8">
   <userInfo guid="{0FC3EEC7-1253-40C9-80FE-72015618EED8}" name="ITLAdmin" id="-2068730528" dateTime="2018-04-13T11:51:21"/>
   <userInfo guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" name="itluser" id="-446795219" dateTime="2018-04-13T11:51:26"/>
   <userInfo guid="{44866337-4EB8-44FB-BDBC-D3FE257C9028}" name="ITLAdmin" id="-2068734883" dateTime="2018-04-26T11:22:09"/>
@@ -12374,6 +12832,7 @@
   <userInfo guid="{643B5170-02EC-4179-A42E-444C0001D79C}" name="itluser" id="-446801440" dateTime="2018-04-26T12:21:33"/>
   <userInfo guid="{D364C1FA-D153-48D2-90E8-4A2B95349BD8}" name="itluser" id="-446801266" dateTime="2018-05-08T15:56:31"/>
   <userInfo guid="{34246483-AB61-4467-BA99-A34781EAEA0F}" name="ITL-USER" id="-1580131676" dateTime="2018-05-11T12:28:00"/>
+  <userInfo guid="{82F04F4E-022D-4926-A8A5-D79C201A90FA}" name="ITL-USER" id="-1580134292" dateTime="2018-05-22T11:31:15"/>
 </users>
 </file>
 
@@ -12640,10 +13099,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12652,10 +13111,9 @@
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="9.42578125" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12677,13 +13135,10 @@
       <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -12703,18 +13158,15 @@
       <c r="G2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
-        <v>132</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -12722,13 +13174,10 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
-      <c r="H4" s="10" t="s">
-        <v>132</v>
-      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -12736,13 +13185,10 @@
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
-      <c r="H5" s="10" t="s">
-        <v>258</v>
-      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -12750,13 +13196,10 @@
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
-      <c r="H6" s="10" t="s">
-        <v>258</v>
-      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -12764,13 +13207,10 @@
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-      <c r="H7" s="10" t="s">
-        <v>258</v>
-      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -12778,13 +13218,10 @@
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
-      <c r="H8" s="10" t="s">
-        <v>132</v>
-      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -12792,222 +13229,195 @@
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
-      <c r="H9" s="10" t="s">
-        <v>132</v>
-      </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="15" t="s">
-        <v>303</v>
-      </c>
-      <c r="B10" s="15" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>300</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="15" t="s">
-        <v>258</v>
-      </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="B11" s="15" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="15" t="s">
-        <v>132</v>
-      </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>347</v>
-      </c>
-      <c r="B12" s="15" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="15" t="s">
-        <v>132</v>
-      </c>
     </row>
-    <row r="13" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
+    <row r="13" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
         <v>341</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B16" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C16" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D16" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E16" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F16" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G16" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="15" t="s">
-        <v>132</v>
-      </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="B14" s="15" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D17" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E17" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F17" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G17" s="14" t="s">
         <v>15</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>344</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>345</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
-        <v>346</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
-      <selection activeCell="A2" sqref="A2"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="G9" sqref="G9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -13016,8 +13426,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="G9" sqref="G9"/>
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+      <selection activeCell="A2" sqref="A2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -13031,43 +13441,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="26.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="39.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="34.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="37.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="37.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="36" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="32" style="15" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="29" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="30" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="26.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="39.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="37.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="37.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="37.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="35.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="36" style="14" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="34.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="32" style="14" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29" style="14" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="25.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="31.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="31.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="29.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="30.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="30" style="14" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="28.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="26.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="32.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
@@ -13075,108 +13485,108 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>296</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>297</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>298</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>299</v>
       </c>
-      <c r="H1" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>301</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="L1" s="14" t="s">
         <v>306</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="M1" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="N1" s="14" t="s">
         <v>310</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="O1" s="14" t="s">
         <v>312</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q1" s="14" t="s">
         <v>314</v>
       </c>
-      <c r="O1" s="15" t="s">
-        <v>316</v>
-      </c>
-      <c r="P1" s="15" t="s">
-        <v>317</v>
-      </c>
-      <c r="Q1" s="15" t="s">
+      <c r="R1" s="14" t="s">
         <v>318</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="T1" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="U1" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="V1" s="14" t="s">
         <v>322</v>
       </c>
-      <c r="S1" t="s">
+      <c r="W1" s="14" t="s">
         <v>323</v>
       </c>
-      <c r="T1" t="s">
+      <c r="X1" s="14" t="s">
         <v>324</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Y1" s="14" t="s">
         <v>325</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Z1" s="14" t="s">
         <v>326</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="AA1" s="14" t="s">
         <v>327</v>
       </c>
-      <c r="X1" s="15" t="s">
+      <c r="AB1" s="14" t="s">
         <v>328</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AC1" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AD1" s="14" t="s">
         <v>330</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AE1" s="14" t="s">
         <v>331</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AF1" s="14" t="s">
         <v>332</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AG1" s="14" t="s">
         <v>333</v>
       </c>
-      <c r="AD1" t="s">
-        <v>334</v>
-      </c>
-      <c r="AE1" t="s">
+      <c r="AH1" s="14" t="s">
         <v>335</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>336</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>337</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>3</v>
@@ -13197,396 +13607,380 @@
         <v>15</v>
       </c>
       <c r="H2" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="K2" s="14" t="s">
         <v>304</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="L2" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="W2" s="14">
+        <v>26000</v>
+      </c>
+      <c r="X2" s="14">
+        <v>2000</v>
+      </c>
+      <c r="AB2" s="14">
+        <v>10</v>
+      </c>
+      <c r="AC2" s="14">
+        <v>10</v>
+      </c>
+      <c r="AD2" s="14">
+        <v>12</v>
+      </c>
+      <c r="AE2" s="14">
+        <v>11</v>
+      </c>
+      <c r="AF2" s="14">
+        <v>10</v>
+      </c>
+      <c r="AG2" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="AH2" s="14" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>305</v>
       </c>
-      <c r="J2" s="14"/>
-      <c r="O2" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>320</v>
-      </c>
-      <c r="Q2" s="15" t="s">
-        <v>321</v>
-      </c>
-      <c r="W2" s="15">
-        <v>26000</v>
-      </c>
-      <c r="X2" s="15">
-        <v>2000</v>
-      </c>
-      <c r="AB2">
-        <v>10</v>
-      </c>
-      <c r="AC2">
-        <v>10</v>
-      </c>
-      <c r="AD2">
-        <v>12</v>
-      </c>
-      <c r="AE2">
+      <c r="B3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="AF2">
-        <v>10</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>338</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>340</v>
+      <c r="F3" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>317</v>
       </c>
     </row>
-    <row r="3" spans="1:34" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="B3" s="15" t="s">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H4" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="K5" s="14" t="s">
         <v>304</v>
       </c>
-      <c r="I3" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="J3" s="15" t="s">
+      <c r="L5" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="M5" s="14" t="s">
         <v>309</v>
       </c>
-      <c r="K3" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="L3" s="15" t="s">
+      <c r="N5" s="14" t="s">
         <v>311</v>
-      </c>
-      <c r="M3" s="15" t="s">
-        <v>313</v>
-      </c>
-      <c r="N3" s="15" t="s">
-        <v>315</v>
-      </c>
-      <c r="O3" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="P3" s="15" t="s">
-        <v>320</v>
-      </c>
-      <c r="Q3" s="15" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>347</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>304</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>341</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>304</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>311</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>313</v>
-      </c>
-      <c r="N5" s="15" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="K6" s="14" t="s">
         <v>304</v>
       </c>
-      <c r="I6" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="J6" s="15" t="s">
+      <c r="L6" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="M6" s="14" t="s">
         <v>309</v>
       </c>
-      <c r="K6" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="L6" s="15" t="s">
+      <c r="N6" s="14" t="s">
         <v>311</v>
       </c>
-      <c r="M6" s="15" t="s">
-        <v>313</v>
-      </c>
-      <c r="N6" s="15" t="s">
+      <c r="O6" s="14" t="s">
         <v>315</v>
       </c>
-      <c r="O6" s="15" t="s">
-        <v>319</v>
-      </c>
-      <c r="P6" s="15" t="s">
-        <v>320</v>
-      </c>
-      <c r="Q6" s="15" t="s">
-        <v>321</v>
+      <c r="P6" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="Q6" s="14" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>344</v>
-      </c>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="B7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="15" t="s">
-        <v>304</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="J7" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="N7" s="15"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="15">
+      <c r="H7" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="W7" s="14">
         <v>26000</v>
       </c>
-      <c r="X7" s="15">
+      <c r="X7" s="14">
         <v>2000</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
-        <v>345</v>
-      </c>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="15" t="s">
-        <v>304</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="J8" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="N8" s="15"/>
-      <c r="R8" s="15"/>
-      <c r="S8" s="15"/>
-      <c r="T8" s="15"/>
-      <c r="U8" s="15"/>
-      <c r="V8" s="15"/>
-      <c r="Y8" s="15"/>
-      <c r="Z8" s="15"/>
-      <c r="AA8" s="15"/>
-      <c r="AB8" s="15">
+      <c r="H8" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="AB8" s="14">
         <v>10</v>
       </c>
-      <c r="AC8" s="15">
+      <c r="AC8" s="14">
         <v>11</v>
       </c>
-      <c r="AD8" s="15">
+      <c r="AD8" s="14">
         <v>12</v>
       </c>
-      <c r="AE8" s="15">
+      <c r="AE8" s="14">
         <v>13</v>
       </c>
-      <c r="AF8" s="15">
+      <c r="AF8" s="14">
         <v>10</v>
       </c>
-      <c r="AG8" s="15" t="s">
-        <v>338</v>
+      <c r="AG8" s="14" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="J9" s="14" t="s">
         <v>346</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>304</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="N9" s="15"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
-      <c r="U9" s="15"/>
-      <c r="V9" s="15"/>
-      <c r="Y9" s="15"/>
-      <c r="Z9" s="15"/>
-      <c r="AA9" s="15"/>
-      <c r="AB9" s="15"/>
-      <c r="AC9" s="15"/>
-      <c r="AD9" s="15"/>
-      <c r="AE9" s="15"/>
-      <c r="AF9" s="15"/>
-      <c r="AG9" s="15"/>
-      <c r="AH9" s="15" t="s">
-        <v>340</v>
+      <c r="AH9" s="14" t="s">
+        <v>336</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
-      <selection activeCell="E11" sqref="E11"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="AC1">
+      <selection activeCell="AH2" sqref="AH2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="D11" sqref="D11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="AC1">
-      <selection activeCell="AH2" sqref="AH2"/>
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+      <selection activeCell="E11" sqref="E11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -13612,46 +14006,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>183</v>
+      <c r="B1" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="C2" s="15" t="s">
+      <c r="A2" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>184</v>
+      <c r="E2" s="14" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -13675,44 +14069,44 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D1" t="s">
+        <v>203</v>
+      </c>
+      <c r="E1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" t="s">
         <v>205</v>
-      </c>
-      <c r="E1" t="s">
-        <v>206</v>
-      </c>
-      <c r="F1" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E2" t="s">
         <v>208</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>209</v>
-      </c>
-      <c r="E2" t="s">
-        <v>210</v>
-      </c>
-      <c r="F2" t="s">
-        <v>211</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="K12" sqref="K12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -13720,7 +14114,7 @@
       <selection activeCell="K12" sqref="K12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="K12" sqref="K12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -13767,113 +14161,113 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
       <c r="D1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F1" t="s">
         <v>188</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>189</v>
+      </c>
+      <c r="H1" t="s">
         <v>190</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>191</v>
       </c>
-      <c r="H1" t="s">
-        <v>192</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>193</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>194</v>
+      </c>
+      <c r="L1" t="s">
         <v>195</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>196</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>197</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>198</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>200</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>202</v>
-      </c>
       <c r="R1" t="s">
+        <v>210</v>
+      </c>
+      <c r="S1" t="s">
         <v>212</v>
       </c>
-      <c r="S1" t="s">
-        <v>214</v>
-      </c>
       <c r="T1" t="s">
+        <v>252</v>
+      </c>
+      <c r="U1" t="s">
+        <v>253</v>
+      </c>
+      <c r="V1" t="s">
         <v>254</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>255</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>256</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>257</v>
-      </c>
-      <c r="X1" t="s">
-        <v>259</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="I2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="S2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="O1">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="O1">
       <selection activeCell="Y1" sqref="Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -13881,7 +14275,7 @@
       <selection activeCell="D2" sqref="D2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="O1">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="O1">
       <selection activeCell="Y1" sqref="Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -13960,278 +14354,278 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" t="s">
         <v>60</v>
       </c>
-      <c r="D1" t="s">
-        <v>61</v>
-      </c>
       <c r="E1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" t="s">
         <v>63</v>
       </c>
-      <c r="F1" t="s">
-        <v>64</v>
-      </c>
       <c r="G1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" t="s">
         <v>70</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>71</v>
       </c>
-      <c r="K1" t="s">
-        <v>72</v>
-      </c>
       <c r="L1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" t="s">
         <v>77</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>78</v>
       </c>
-      <c r="O1" t="s">
-        <v>79</v>
-      </c>
       <c r="P1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q1" t="s">
         <v>81</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
+        <v>97</v>
+      </c>
+      <c r="S1" t="s">
         <v>82</v>
       </c>
-      <c r="R1" t="s">
-        <v>98</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>83</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>84</v>
       </c>
-      <c r="U1" t="s">
-        <v>85</v>
-      </c>
       <c r="V1" t="s">
+        <v>88</v>
+      </c>
+      <c r="W1" t="s">
         <v>89</v>
       </c>
-      <c r="W1" t="s">
-        <v>90</v>
-      </c>
       <c r="X1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y1" t="s">
         <v>92</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>93</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>94</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>95</v>
       </c>
-      <c r="AB1" t="s">
-        <v>96</v>
-      </c>
       <c r="AC1" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD1" t="s">
         <v>101</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>102</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>103</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>104</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>105</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>106</v>
       </c>
-      <c r="AI1" t="s">
-        <v>107</v>
-      </c>
       <c r="AJ1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK1" t="s">
         <v>110</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>111</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>112</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>113</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>114</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>115</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>116</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>117</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>118</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>119</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>120</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>121</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>122</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>123</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>124</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>125</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>126</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>127</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>128</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>129</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>130</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2">
         <v>18811</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N2" s="6">
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P2" s="6">
         <v>1</v>
       </c>
       <c r="Q2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="T2" s="7">
         <v>30753</v>
       </c>
       <c r="U2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="W2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Z2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AA2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AC2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AD2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE2" t="s">
         <v>108</v>
       </c>
-      <c r="AE2" t="s">
-        <v>109</v>
-      </c>
       <c r="AG2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AI2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AZ2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="BA2" t="s">
         <v>5</v>
       </c>
       <c r="BD2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="V1">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="V1">
       <selection activeCell="AA1" sqref="AA1:AA1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14241,7 +14635,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="V1">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="V1">
       <selection activeCell="AA1" sqref="AA1:AA1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -14275,153 +14669,153 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
-        <v>25</v>
-      </c>
       <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
-        <v>28</v>
-      </c>
       <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
         <v>30</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>31</v>
       </c>
-      <c r="L1" t="s">
-        <v>32</v>
-      </c>
       <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
         <v>34</v>
       </c>
-      <c r="N1" t="s">
-        <v>35</v>
-      </c>
       <c r="O1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="S1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T1" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="V1" s="11" t="s">
+        <v>269</v>
+      </c>
+      <c r="W1" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="X1" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y1" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="Z1" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="AA1" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="AB1" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="AC1" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="AD1" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="AE1" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="AF1" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="X1" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="Y1" s="11" t="s">
+      <c r="AG1" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="Z1" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="AA1" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="AB1" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="AC1" s="11" t="s">
-        <v>237</v>
-      </c>
-      <c r="AD1" s="11" t="s">
+      <c r="AH1" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="AE1" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="AF1" s="11" t="s">
+      <c r="AI1" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="AG1" s="11" t="s">
+      <c r="AJ1" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="AH1" s="11" t="s">
+      <c r="AK1" s="11" t="s">
         <v>278</v>
       </c>
-      <c r="AI1" s="11" t="s">
+      <c r="AL1" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="AJ1" s="11" t="s">
+      <c r="AM1" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="AK1" s="11" t="s">
+      <c r="AN1" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="AL1" s="11" t="s">
+      <c r="AO1" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="AM1" s="11" t="s">
+      <c r="AP1" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="AN1" s="11" t="s">
+      <c r="AQ1" s="11" t="s">
         <v>284</v>
       </c>
-      <c r="AO1" s="11" t="s">
+      <c r="AR1" s="11" t="s">
         <v>285</v>
       </c>
-      <c r="AP1" s="11" t="s">
+      <c r="AS1" s="11" t="s">
         <v>286</v>
       </c>
-      <c r="AQ1" s="11" t="s">
-        <v>287</v>
-      </c>
-      <c r="AR1" s="11" t="s">
-        <v>288</v>
-      </c>
-      <c r="AS1" s="11" t="s">
-        <v>289</v>
-      </c>
       <c r="AT1" s="11" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E2" s="3">
         <v>231</v>
@@ -14430,40 +14824,40 @@
         <v>232</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="T2" s="11"/>
       <c r="U2" s="11"/>
@@ -14497,37 +14891,37 @@
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>237</v>
+      </c>
+      <c r="R3" t="s">
+        <v>248</v>
+      </c>
+      <c r="S3" t="s">
+        <v>248</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>238</v>
+      </c>
+      <c r="V3" s="11" t="s">
         <v>239</v>
       </c>
-      <c r="R3" t="s">
-        <v>250</v>
-      </c>
-      <c r="S3" t="s">
-        <v>250</v>
-      </c>
-      <c r="T3" s="11" t="s">
+      <c r="W3" s="11" t="s">
         <v>240</v>
       </c>
-      <c r="U3" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="V3" s="11" t="s">
+      <c r="X3" s="11" t="s">
         <v>241</v>
-      </c>
-      <c r="W3" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="X3" s="11" t="s">
-        <v>243</v>
       </c>
       <c r="Y3" s="11">
         <v>10012</v>
       </c>
       <c r="Z3" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="AA3" s="11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="AB3" s="11"/>
       <c r="AC3" s="11"/>
@@ -14551,14 +14945,14 @@
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="S4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="T4" s="11"/>
       <c r="U4" s="11" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="V4" s="11"/>
       <c r="W4" s="11"/>
@@ -14573,13 +14967,13 @@
         <v>55</v>
       </c>
       <c r="AD4" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="AE4" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="AF4" s="11" t="s">
         <v>248</v>
-      </c>
-      <c r="AE4" s="11" t="s">
-        <v>249</v>
-      </c>
-      <c r="AF4" s="11" t="s">
-        <v>250</v>
       </c>
       <c r="AG4" s="11"/>
       <c r="AH4" s="11"/>
@@ -14594,17 +14988,17 @@
       <c r="AQ4" s="11"/>
       <c r="AR4" s="11"/>
       <c r="AS4" s="11" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="AT4" s="11"/>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="T5" s="11"/>
       <c r="U5" s="11" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="V5" s="11"/>
       <c r="W5" s="11"/>
@@ -14617,46 +15011,46 @@
       <c r="AD5" s="11"/>
       <c r="AE5" s="11"/>
       <c r="AF5" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AG5" s="12" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AH5" s="13">
         <v>0.54166666666666663</v>
       </c>
       <c r="AI5" s="12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AJ5" s="13">
         <v>0.58680555555555558</v>
       </c>
       <c r="AK5" s="12" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="AL5" s="13">
         <v>0.33680555555555558</v>
       </c>
       <c r="AM5" s="12" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="AN5" s="13">
         <v>0.70486111111111116</v>
       </c>
       <c r="AO5" s="12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AP5" s="13">
         <v>0.2951388888888889</v>
       </c>
       <c r="AQ5" s="12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AR5" s="13">
         <v>0.67083333333333339</v>
       </c>
       <c r="AS5" s="11" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="AT5" s="11"/>
     </row>
@@ -14674,62 +15068,62 @@
       <c r="AD6" s="11"/>
       <c r="AE6" s="11"/>
       <c r="AF6" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AG6" s="12" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="AH6" s="13">
         <v>0.54166666666666663</v>
       </c>
       <c r="AI6" s="12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AJ6" s="13">
         <v>0.58680555555555558</v>
       </c>
       <c r="AK6" s="12" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="AL6" s="13">
         <v>0.33680555555555558</v>
       </c>
       <c r="AM6" s="12" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="AN6" s="13">
         <v>0.70486111111111116</v>
       </c>
       <c r="AO6" s="12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AP6" s="13">
         <v>0.2951388888888889</v>
       </c>
       <c r="AQ6" s="12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="AR6" s="13">
         <v>0.52361111111111114</v>
       </c>
       <c r="AS6" s="11"/>
       <c r="AT6" s="11" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="22" spans="40:41" x14ac:dyDescent="0.25">
       <c r="AO22" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="40:41" x14ac:dyDescent="0.25">
       <c r="AN25" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="A3" sqref="A3:XFD3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -14737,7 +15131,7 @@
       <selection activeCell="A3" sqref="A3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="A3" sqref="A3:XFD3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -14764,37 +15158,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="H1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>265</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>267</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>268</v>
       </c>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
@@ -14803,20 +15197,20 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="I2" s="8">
         <v>155</v>
@@ -14835,32 +15229,32 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="F3" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>226</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>228</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -14869,7 +15263,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -14879,10 +15273,10 @@
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
@@ -14893,7 +15287,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -14913,7 +15307,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="Q1" sqref="Q1:Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -14921,7 +15315,7 @@
       <selection activeCell="Q1" sqref="Q1:Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="Q1" sqref="Q1:Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -14970,165 +15364,165 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" t="s">
         <v>133</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" t="s">
         <v>135</v>
       </c>
-      <c r="D1" t="s">
-        <v>136</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>137</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" t="s">
         <v>139</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>140</v>
       </c>
-      <c r="H1" t="s">
-        <v>141</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>142</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>143</v>
+      </c>
+      <c r="L1" t="s">
         <v>144</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>145</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>146</v>
       </c>
-      <c r="M1" t="s">
-        <v>147</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>148</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>149</v>
+      </c>
+      <c r="Q1" t="s">
         <v>150</v>
       </c>
-      <c r="P1" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>152</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
+        <v>153</v>
+      </c>
+      <c r="T1" t="s">
         <v>154</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>155</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>156</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>157</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>158</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>159</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>160</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>161</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>162</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>163</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>164</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>165</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>166</v>
       </c>
-      <c r="AE1" t="s">
-        <v>167</v>
-      </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>168</v>
       </c>
-      <c r="AG1" t="s">
-        <v>170</v>
-      </c>
       <c r="AH1" t="s">
+        <v>169</v>
+      </c>
+      <c r="AI1" t="s">
         <v>171</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J2" t="s">
         <v>5</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="Q2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S2" t="s">
         <v>13</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Z2">
         <v>10</v>
@@ -15146,21 +15540,21 @@
         <v>2200</v>
       </c>
       <c r="AF2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AG2" t="s">
         <v>5</v>
       </c>
       <c r="AH2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI2" t="s">
         <v>172</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="W1">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="W1">
       <selection activeCell="AI2" sqref="AI2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15169,7 +15563,7 @@
       <selection activeCell="AI2" sqref="AI2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="W1">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="W1">
       <selection activeCell="AI2" sqref="AI2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -15198,48 +15592,48 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
         <v>51</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>52</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>53</v>
-      </c>
-      <c r="I1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G2">
         <v>1900</v>
@@ -15248,12 +15642,12 @@
         <v>25000</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="G1" sqref="G1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15263,7 +15657,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="G1" sqref="G1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -15276,69 +15670,100 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
+        <v>338</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>341</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>344</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>345</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
+      <c r="B8" s="14" t="s">
         <v>346</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>309</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -15346,7 +15771,7 @@
       <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>

</xml_diff>

<commit_message>
Aswini - Updated TestData
</commit_message>
<xml_diff>
--- a/Basic Test Suite/TestData/TestData.xlsx
+++ b/Basic Test Suite/TestData/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TestComplete\TestN4\Basic Test Suite\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ITL-USER\Desktop\TestComplete\Basic Test Suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="SparcsN4Login" sheetId="1" r:id="rId1"/>
@@ -23,18 +23,20 @@
     <sheet name="UnitFacilityVisit" sheetId="8" r:id="rId9"/>
     <sheet name="N4MobileCommonRoutines" sheetId="10" r:id="rId10"/>
     <sheet name="SparcsN4CommonRoutines" sheetId="11" r:id="rId11"/>
+    <sheet name="YardInventoryQuery" sheetId="12" r:id="rId12"/>
+    <sheet name="YardInspection" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="ITL-USER - Personal View" guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1380" windowHeight="744" activeSheetId="13"/>
     <customWorkbookView name="itluser - Personal View" guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="9"/>
     <customWorkbookView name="ITLAdmin - Personal View" guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1362" windowHeight="503" activeSheetId="11"/>
-    <customWorkbookView name="ITL-USER - Personal View" guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1380" windowHeight="744" activeSheetId="10"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="383">
   <si>
     <t>Flow Name</t>
   </si>
@@ -579,12 +581,6 @@
     <t>Vessel</t>
   </si>
   <si>
-    <t>FileName</t>
-  </si>
-  <si>
-    <t>ICY_Commodity.xml</t>
-  </si>
-  <si>
     <t>MailBoxName</t>
   </si>
   <si>
@@ -1084,6 +1080,111 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>WebRequest</t>
+  </si>
+  <si>
+    <t>\PurgeUnit.txt</t>
+  </si>
+  <si>
+    <t>n4YinvQueryBundleContainer1</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerHasPlacard</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerPlacard1</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerDoorDirection</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerEvent</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerLineOperator</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerEqType</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerTankRails</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerChassis</t>
+  </si>
+  <si>
+    <t>n4YinvQueryContainerNotes</t>
+  </si>
+  <si>
+    <t>SBSU1234590</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>CLASS 1.4</t>
+  </si>
+  <si>
+    <t>Aft</t>
+  </si>
+  <si>
+    <t>TEST-CTR-LOAD-EDI</t>
+  </si>
+  <si>
+    <t>Top</t>
+  </si>
+  <si>
+    <t>CHS1</t>
+  </si>
+  <si>
+    <t>DAS</t>
+  </si>
+  <si>
+    <t>n4YInspEnterContainer</t>
+  </si>
+  <si>
+    <t>n4YInspEnterSeal</t>
+  </si>
+  <si>
+    <t>n4YInspDamageComponent</t>
+  </si>
+  <si>
+    <t>n4YInspDamageType</t>
+  </si>
+  <si>
+    <t>n4YInspDamageSeverity</t>
+  </si>
+  <si>
+    <t>n4YInspDamageLocation</t>
+  </si>
+  <si>
+    <t>n4YInspDamageWidth</t>
+  </si>
+  <si>
+    <t>n4YInspDamageLength</t>
+  </si>
+  <si>
+    <t>n4YInspDamageDepth</t>
+  </si>
+  <si>
+    <t>n4YInspOOGH</t>
+  </si>
+  <si>
+    <t>n4YInspOOGL</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>n4YInspOOGR</t>
+  </si>
+  <si>
+    <t>n4YInspOOGF</t>
+  </si>
+  <si>
+    <t>n4YInspOOGA</t>
   </si>
 </sst>
 </file>
@@ -1159,7 +1260,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{3CB01C14-B4BF-415E-BFBE-7D62CFDE3729}" diskRevisions="1" revisionId="770" version="175">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{2E1BFB99-DAAF-481E-A4ED-F5C2B2B48C90}" diskRevisions="1" revisionId="942" version="183">
   <header guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" dateTime="2018-04-13T11:49:43" maxSheetId="10" userName="itluser" r:id="rId7" minRId="7">
     <sheetIdMap count="9">
       <sheetId val="1"/>
@@ -3495,7 +3596,178 @@
       <sheetId val="11"/>
     </sheetIdMap>
   </header>
+  <header guid="{1D851247-D27D-4079-842F-E8BEE56F43FC}" dateTime="2018-06-04T15:26:40" maxSheetId="12" userName="ITL-USER" r:id="rId176" minRId="771" maxRId="773">
+    <sheetIdMap count="11">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6B3D7986-4CED-4793-B218-11ABE0F4EAE7}" dateTime="2018-06-04T15:41:30" maxSheetId="13" userName="ITL-USER" r:id="rId177" minRId="774" maxRId="838">
+    <sheetIdMap count="12">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{CFA85622-56D2-4E0E-8BF5-66A87AAB6A23}" dateTime="2018-06-04T15:41:44" maxSheetId="14" userName="ITL-USER" r:id="rId178" minRId="839" maxRId="859">
+    <sheetIdMap count="13">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{438B3F62-5B92-4823-A34F-6E8218219287}" dateTime="2018-06-04T16:02:08" maxSheetId="14" userName="ITL-USER" r:id="rId179" minRId="860" maxRId="861">
+    <sheetIdMap count="13">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{D74FD33A-6044-4171-A03D-67805D516CFB}" dateTime="2018-06-04T16:09:52" maxSheetId="14" userName="ITL-USER" r:id="rId180" minRId="862" maxRId="863">
+    <sheetIdMap count="13">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{060CB6DC-B053-4558-A308-6B6B10B75484}" dateTime="2018-06-04T16:17:46" maxSheetId="14" userName="ITL-USER" r:id="rId181" minRId="864" maxRId="939">
+    <sheetIdMap count="13">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{60E0AFCF-AC01-48CF-AA9F-9600287AE28C}" dateTime="2018-06-04T16:23:05" maxSheetId="14" userName="ITL-USER" r:id="rId182" minRId="940" maxRId="941">
+    <sheetIdMap count="13">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{2E1BFB99-DAAF-481E-A4ED-F5C2B2B48C90}" dateTime="2018-06-04T16:24:09" maxSheetId="14" userName="ITL-USER" r:id="rId183" minRId="942">
+    <sheetIdMap count="13">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
 </headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="771" sId="11" ref="E1:E1048576" action="deleteCol">
+    <rfmt sheetId="11" xfDxf="1" sqref="E1:E1048576" start="0" length="0"/>
+    <rcc rId="0" sId="11">
+      <nc r="E1" t="inlineStr">
+        <is>
+          <t>FileName</t>
+        </is>
+      </nc>
+    </rcc>
+    <rcc rId="0" sId="11">
+      <nc r="E2" t="inlineStr">
+        <is>
+          <t>ICY_Commodity.xml</t>
+        </is>
+      </nc>
+    </rcc>
+  </rrc>
+  <rcc rId="772" sId="11">
+    <nc r="E1" t="inlineStr">
+      <is>
+        <t>WebRequest</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="773" sId="11">
+    <nc r="E2" t="inlineStr">
+      <is>
+        <t>\PurgeUnit.txt</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11009,6 +11281,40 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog176.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="940" sId="13">
+    <nc r="O1" t="inlineStr">
+      <is>
+        <t>n4YInspOOGR</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="941" sId="13">
+    <nc r="O2">
+      <v>10</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog177.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="942" sId="13">
+    <oc r="O1" t="inlineStr">
+      <is>
+        <t>n4YInspOOGR</t>
+      </is>
+    </oc>
+    <nc r="O1" t="inlineStr">
+      <is>
+        <t>n4YInspOOGA</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog18.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcv guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" action="delete"/>
@@ -11038,6 +11344,510 @@
       <numFmt numFmtId="166" formatCode="\+\1"/>
     </dxf>
   </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <ris rId="774" sheetId="12" name="[TestData.xlsx]YardInventoryQuery" sheetPosition="11"/>
+  <rcc rId="775" sId="12" odxf="1">
+    <nc r="A1" t="inlineStr">
+      <is>
+        <t>Flow Name</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="776" sId="12" odxf="1">
+    <nc r="B1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainer</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="777" sId="12" odxf="1">
+    <nc r="C1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerSeal1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="778" sId="12" odxf="1">
+    <nc r="D1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerSeal2</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="779" sId="12" odxf="1">
+    <nc r="E1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerSeal3</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="780" sId="12" odxf="1">
+    <nc r="F1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerSeal4</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="781" sId="12" odxf="1">
+    <nc r="G1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageComponent1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="782" sId="12" odxf="1">
+    <nc r="H1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageType1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="783" sId="12" odxf="1">
+    <nc r="I1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageSeverity1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="784" sId="12" odxf="1">
+    <nc r="J1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageLocation1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="785" sId="12" odxf="1">
+    <nc r="K1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageQuantity1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="786" sId="12" odxf="1">
+    <nc r="L1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageWidth1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="787" sId="12" odxf="1">
+    <nc r="M1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageLength1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="788" sId="12" odxf="1">
+    <nc r="N1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageDeep1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="789" sId="12" odxf="1">
+    <nc r="O1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerSafeWeight</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="790" sId="12" odxf="1">
+    <nc r="P1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerTareWeight</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="791" sId="12" odxf="1">
+    <nc r="Q1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerCSCDate</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="792" sId="12" odxf="1">
+    <nc r="R1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerMNF</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="793" sId="12" odxf="1">
+    <nc r="S1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerMNRStatus</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="794" sId="12" odxf="1">
+    <nc r="T1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerOverHeight</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="795" sId="12" odxf="1">
+    <nc r="U1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerOverLeft</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="796" sId="12" odxf="1">
+    <nc r="V1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerOverRight</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="797" sId="12" odxf="1">
+    <nc r="W1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerOverFore</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="798" sId="12" odxf="1">
+    <nc r="X1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerOverAft</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="799" sId="12" odxf="1">
+    <nc r="Y1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerUnits</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="800" sId="12" odxf="1">
+    <nc r="Z1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerGradeValue</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="801" sId="12" odxf="1">
+    <nc r="AA1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryBundleContainer1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="802" sId="12" odxf="1">
+    <nc r="AB1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerHasPlacard</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="803" sId="12" odxf="1">
+    <nc r="AC1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerPlacard1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="804" sId="12" odxf="1">
+    <nc r="AD1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDoorDirection</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="805" sId="12" odxf="1">
+    <nc r="AE1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerEvent</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="806" sId="12" odxf="1">
+    <nc r="AF1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerLineOperator</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="807" sId="12" odxf="1">
+    <nc r="AG1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerEqType</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="808" sId="12" odxf="1">
+    <nc r="AH1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerTankRails</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="809" sId="12" odxf="1">
+    <nc r="AI1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerChassis</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="810" sId="12" odxf="1">
+    <nc r="AJ1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerNotes</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="811" sId="12" odxf="1">
+    <nc r="A2" t="inlineStr">
+      <is>
+        <t>N4MobileCommonRoutines</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="812" sId="12" odxf="1">
+    <nc r="B2" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="813" sId="12" odxf="1">
+    <nc r="C2" t="inlineStr">
+      <is>
+        <t>S1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="814" sId="12" odxf="1">
+    <nc r="D2" t="inlineStr">
+      <is>
+        <t>S2</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="815" sId="12" odxf="1">
+    <nc r="E2" t="inlineStr">
+      <is>
+        <t>S3</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="816" sId="12" odxf="1">
+    <nc r="F2" t="inlineStr">
+      <is>
+        <t>S4</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="817" sId="12" odxf="1">
+    <nc r="G2" t="inlineStr">
+      <is>
+        <t>DOOR</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="818" sId="12" odxf="1">
+    <nc r="H2" t="inlineStr">
+      <is>
+        <t>DAT</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="819" sId="12" odxf="1">
+    <nc r="I2" t="inlineStr">
+      <is>
+        <t>Major</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="820" sId="12" odxf="1">
+    <nc r="O2">
+      <v>26000</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="821" sId="12" odxf="1">
+    <nc r="P2">
+      <v>2000</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="822" sId="12" odxf="1">
+    <nc r="T2">
+      <v>10</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="823" sId="12" odxf="1">
+    <nc r="U2">
+      <v>10</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="824" sId="12" odxf="1">
+    <nc r="V2">
+      <v>12</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="825" sId="12" odxf="1">
+    <nc r="W2">
+      <v>11</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="826" sId="12" odxf="1">
+    <nc r="X2">
+      <v>10</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="827" sId="12" odxf="1">
+    <nc r="Y2" t="inlineStr">
+      <is>
+        <t>cm</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="828" sId="12" odxf="1">
+    <nc r="Z2" t="inlineStr">
+      <is>
+        <t>FOOD</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="829" sId="12" odxf="1">
+    <nc r="AA2" t="inlineStr">
+      <is>
+        <t>SBSU1234590</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="830" sId="12" odxf="1">
+    <nc r="AB2" t="inlineStr">
+      <is>
+        <t>Yes</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="831" sId="12" odxf="1">
+    <nc r="AC2" t="inlineStr">
+      <is>
+        <t>CLASS 1.4</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="832" sId="12" odxf="1">
+    <nc r="AD2" t="inlineStr">
+      <is>
+        <t>Aft</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="833" sId="12" odxf="1">
+    <nc r="AE2" t="inlineStr">
+      <is>
+        <t>TEST-CTR-LOAD-EDI</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="834" sId="12" odxf="1">
+    <nc r="AF2" t="inlineStr">
+      <is>
+        <t>ASW</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="835" sId="12" odxf="1">
+    <nc r="AG2">
+      <v>2200</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="836" sId="12" odxf="1">
+    <nc r="AH2" t="inlineStr">
+      <is>
+        <t>Top</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="837" sId="12" odxf="1">
+    <nc r="AI2" t="inlineStr">
+      <is>
+        <t>CHS1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="838" sId="12" odxf="1">
+    <nc r="AJ2" t="inlineStr">
+      <is>
+        <t>DAS</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
 </revisions>
 </file>
 
@@ -11349,6 +12159,170 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <ris rId="839" sheetId="13" name="[TestData.xlsx]Sheet2" sheetPosition="12"/>
+  <rcc rId="840" sId="13" odxf="1">
+    <nc r="A1" t="inlineStr">
+      <is>
+        <t>Flow Name</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="841" sId="13" odxf="1">
+    <nc r="B1" t="inlineStr">
+      <is>
+        <t>n4YInspEnterContainer</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="842" sId="13" odxf="1">
+    <nc r="C1" t="inlineStr">
+      <is>
+        <t>n4YInspEnterSeal</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="843" sId="13" odxf="1">
+    <nc r="D1" t="inlineStr">
+      <is>
+        <t>n4YInspDamageComponent</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="844" sId="13" odxf="1">
+    <nc r="E1" t="inlineStr">
+      <is>
+        <t>n4YInspDamageType</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="845" sId="13" odxf="1">
+    <nc r="F1" t="inlineStr">
+      <is>
+        <t>n4YInspDamageSeverity</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="846" sId="13" odxf="1">
+    <nc r="G1" t="inlineStr">
+      <is>
+        <t>n4YInspDamageLocation</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="847" sId="13" odxf="1">
+    <nc r="H1" t="inlineStr">
+      <is>
+        <t>n4YInspDamageWidth</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="848" sId="13" odxf="1">
+    <nc r="I1" t="inlineStr">
+      <is>
+        <t>n4YInspDamageLength</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="849" sId="13" odxf="1">
+    <nc r="J1" t="inlineStr">
+      <is>
+        <t>n4YInspDamageDepth</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="850" sId="13" odxf="1">
+    <nc r="K1" t="inlineStr">
+      <is>
+        <t>n4YInspOOGH</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="851" sId="13" odxf="1">
+    <nc r="L1" t="inlineStr">
+      <is>
+        <t>n4YInspOOGL</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="852" sId="13" odxf="1">
+    <nc r="A2" t="inlineStr">
+      <is>
+        <t>N4MobileCommonRoutines</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="853" sId="13" odxf="1">
+    <nc r="B2" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="854" sId="13" odxf="1">
+    <nc r="C2" t="inlineStr">
+      <is>
+        <t>S1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="855" sId="13" odxf="1">
+    <nc r="D2" t="inlineStr">
+      <is>
+        <t>DOOR</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="856" sId="13" odxf="1">
+    <nc r="E2" t="inlineStr">
+      <is>
+        <t>DAT</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="857" sId="13" odxf="1">
+    <nc r="F2" t="inlineStr">
+      <is>
+        <t>Minor</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="858" sId="13" odxf="1">
+    <nc r="K2">
+      <v>10</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="859" sId="13" odxf="1">
+    <nc r="L2">
+      <v>10</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog30.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="53" sId="3" xfDxf="1" dxf="1">
@@ -11477,6 +12451,25 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="860" sId="13">
+    <nc r="M1" t="inlineStr">
+      <is>
+        <t>n4YInspOOGR</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="861" sId="13">
+    <nc r="M2">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog40.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="62" sId="3" xfDxf="1" dxf="1">
@@ -11637,6 +12630,25 @@
   </rcc>
   <rcv guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" action="delete"/>
   <rcv guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="862" sId="13">
+    <nc r="N1" t="inlineStr">
+      <is>
+        <t>n4YInspOOGF</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="863" sId="13">
+    <nc r="N2">
+      <v>10</v>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
 </revisions>
 </file>
 
@@ -11876,6 +12888,591 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="864" sId="10">
+    <oc r="J1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainer</t>
+      </is>
+    </oc>
+    <nc r="J1"/>
+  </rcc>
+  <rcc rId="865" sId="10">
+    <oc r="K1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerSeal1</t>
+      </is>
+    </oc>
+    <nc r="K1"/>
+  </rcc>
+  <rcc rId="866" sId="10">
+    <oc r="L1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerSeal2</t>
+      </is>
+    </oc>
+    <nc r="L1"/>
+  </rcc>
+  <rcc rId="867" sId="10">
+    <oc r="M1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerSeal3</t>
+      </is>
+    </oc>
+    <nc r="M1"/>
+  </rcc>
+  <rcc rId="868" sId="10">
+    <oc r="N1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerSeal4</t>
+      </is>
+    </oc>
+    <nc r="N1"/>
+  </rcc>
+  <rcc rId="869" sId="10">
+    <oc r="O1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageComponent1</t>
+      </is>
+    </oc>
+    <nc r="O1"/>
+  </rcc>
+  <rcc rId="870" sId="10">
+    <oc r="P1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageType1</t>
+      </is>
+    </oc>
+    <nc r="P1"/>
+  </rcc>
+  <rcc rId="871" sId="10">
+    <oc r="Q1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageSeverity1</t>
+      </is>
+    </oc>
+    <nc r="Q1"/>
+  </rcc>
+  <rcc rId="872" sId="10">
+    <oc r="R1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageLocation1</t>
+      </is>
+    </oc>
+    <nc r="R1"/>
+  </rcc>
+  <rcc rId="873" sId="10">
+    <oc r="S1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageQuantity1</t>
+      </is>
+    </oc>
+    <nc r="S1"/>
+  </rcc>
+  <rcc rId="874" sId="10">
+    <oc r="T1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageWidth1</t>
+      </is>
+    </oc>
+    <nc r="T1"/>
+  </rcc>
+  <rcc rId="875" sId="10">
+    <oc r="U1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageLength1</t>
+      </is>
+    </oc>
+    <nc r="U1"/>
+  </rcc>
+  <rcc rId="876" sId="10">
+    <oc r="V1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerDamageDeep1</t>
+      </is>
+    </oc>
+    <nc r="V1"/>
+  </rcc>
+  <rcc rId="877" sId="10">
+    <oc r="W1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerSafeWeight</t>
+      </is>
+    </oc>
+    <nc r="W1"/>
+  </rcc>
+  <rcc rId="878" sId="10">
+    <oc r="X1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerTareWeight</t>
+      </is>
+    </oc>
+    <nc r="X1"/>
+  </rcc>
+  <rcc rId="879" sId="10">
+    <oc r="Y1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerCSCDate</t>
+      </is>
+    </oc>
+    <nc r="Y1"/>
+  </rcc>
+  <rcc rId="880" sId="10">
+    <oc r="Z1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerMNF</t>
+      </is>
+    </oc>
+    <nc r="Z1"/>
+  </rcc>
+  <rcc rId="881" sId="10">
+    <oc r="AA1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerMNRStatus</t>
+      </is>
+    </oc>
+    <nc r="AA1"/>
+  </rcc>
+  <rcc rId="882" sId="10">
+    <oc r="AB1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerOverHeight</t>
+      </is>
+    </oc>
+    <nc r="AB1"/>
+  </rcc>
+  <rcc rId="883" sId="10">
+    <oc r="AC1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerOverLeft</t>
+      </is>
+    </oc>
+    <nc r="AC1"/>
+  </rcc>
+  <rcc rId="884" sId="10">
+    <oc r="AD1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerOverRight</t>
+      </is>
+    </oc>
+    <nc r="AD1"/>
+  </rcc>
+  <rcc rId="885" sId="10">
+    <oc r="AE1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerOverFore</t>
+      </is>
+    </oc>
+    <nc r="AE1"/>
+  </rcc>
+  <rcc rId="886" sId="10">
+    <oc r="AF1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerOverAft</t>
+      </is>
+    </oc>
+    <nc r="AF1"/>
+  </rcc>
+  <rcc rId="887" sId="10">
+    <oc r="AG1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerUnits</t>
+      </is>
+    </oc>
+    <nc r="AG1"/>
+  </rcc>
+  <rcc rId="888" sId="10">
+    <oc r="AH1" t="inlineStr">
+      <is>
+        <t>n4YinvQueryContainerGradeValue</t>
+      </is>
+    </oc>
+    <nc r="AH1"/>
+  </rcc>
+  <rcc rId="889" sId="10">
+    <oc r="J2" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </oc>
+    <nc r="J2"/>
+  </rcc>
+  <rcc rId="890" sId="10">
+    <oc r="K2" t="inlineStr">
+      <is>
+        <t>S1</t>
+      </is>
+    </oc>
+    <nc r="K2"/>
+  </rcc>
+  <rcc rId="891" sId="10">
+    <oc r="L2" t="inlineStr">
+      <is>
+        <t>S2</t>
+      </is>
+    </oc>
+    <nc r="L2"/>
+  </rcc>
+  <rcc rId="892" sId="10">
+    <oc r="M2" t="inlineStr">
+      <is>
+        <t>S3</t>
+      </is>
+    </oc>
+    <nc r="M2"/>
+  </rcc>
+  <rcc rId="893" sId="10">
+    <oc r="N2" t="inlineStr">
+      <is>
+        <t>S4</t>
+      </is>
+    </oc>
+    <nc r="N2"/>
+  </rcc>
+  <rcc rId="894" sId="10">
+    <oc r="O2" t="inlineStr">
+      <is>
+        <t>DOOR</t>
+      </is>
+    </oc>
+    <nc r="O2"/>
+  </rcc>
+  <rcc rId="895" sId="10">
+    <oc r="P2" t="inlineStr">
+      <is>
+        <t>DAT</t>
+      </is>
+    </oc>
+    <nc r="P2"/>
+  </rcc>
+  <rcc rId="896" sId="10">
+    <oc r="Q2" t="inlineStr">
+      <is>
+        <t>Major</t>
+      </is>
+    </oc>
+    <nc r="Q2"/>
+  </rcc>
+  <rcc rId="897" sId="10">
+    <oc r="W2">
+      <v>26000</v>
+    </oc>
+    <nc r="W2"/>
+  </rcc>
+  <rcc rId="898" sId="10">
+    <oc r="X2">
+      <v>2000</v>
+    </oc>
+    <nc r="X2"/>
+  </rcc>
+  <rcc rId="899" sId="10">
+    <oc r="AB2">
+      <v>10</v>
+    </oc>
+    <nc r="AB2"/>
+  </rcc>
+  <rcc rId="900" sId="10">
+    <oc r="AC2">
+      <v>10</v>
+    </oc>
+    <nc r="AC2"/>
+  </rcc>
+  <rcc rId="901" sId="10">
+    <oc r="AD2">
+      <v>12</v>
+    </oc>
+    <nc r="AD2"/>
+  </rcc>
+  <rcc rId="902" sId="10">
+    <oc r="AE2">
+      <v>11</v>
+    </oc>
+    <nc r="AE2"/>
+  </rcc>
+  <rcc rId="903" sId="10">
+    <oc r="AF2">
+      <v>10</v>
+    </oc>
+    <nc r="AF2"/>
+  </rcc>
+  <rcc rId="904" sId="10">
+    <oc r="AG2" t="inlineStr">
+      <is>
+        <t>cm</t>
+      </is>
+    </oc>
+    <nc r="AG2"/>
+  </rcc>
+  <rcc rId="905" sId="10">
+    <oc r="AH2" t="inlineStr">
+      <is>
+        <t>FOOD</t>
+      </is>
+    </oc>
+    <nc r="AH2"/>
+  </rcc>
+  <rcc rId="906" sId="10">
+    <oc r="J3" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </oc>
+    <nc r="J3"/>
+  </rcc>
+  <rcc rId="907" sId="10">
+    <oc r="K3" t="inlineStr">
+      <is>
+        <t>S1</t>
+      </is>
+    </oc>
+    <nc r="K3"/>
+  </rcc>
+  <rcc rId="908" sId="10">
+    <oc r="L3" t="inlineStr">
+      <is>
+        <t>S2</t>
+      </is>
+    </oc>
+    <nc r="L3"/>
+  </rcc>
+  <rcc rId="909" sId="10">
+    <oc r="M3" t="inlineStr">
+      <is>
+        <t>S3</t>
+      </is>
+    </oc>
+    <nc r="M3"/>
+  </rcc>
+  <rcc rId="910" sId="10">
+    <oc r="N3" t="inlineStr">
+      <is>
+        <t>S4</t>
+      </is>
+    </oc>
+    <nc r="N3"/>
+  </rcc>
+  <rcc rId="911" sId="10">
+    <oc r="O3" t="inlineStr">
+      <is>
+        <t>DOOR</t>
+      </is>
+    </oc>
+    <nc r="O3"/>
+  </rcc>
+  <rcc rId="912" sId="10">
+    <oc r="P3" t="inlineStr">
+      <is>
+        <t>DAT</t>
+      </is>
+    </oc>
+    <nc r="P3"/>
+  </rcc>
+  <rcc rId="913" sId="10">
+    <oc r="Q3" t="inlineStr">
+      <is>
+        <t>Major</t>
+      </is>
+    </oc>
+    <nc r="Q3"/>
+  </rcc>
+  <rcc rId="914" sId="10">
+    <oc r="J4" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </oc>
+    <nc r="J4"/>
+  </rcc>
+  <rcc rId="915" sId="10">
+    <oc r="J5" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </oc>
+    <nc r="J5"/>
+  </rcc>
+  <rcc rId="916" sId="10">
+    <oc r="K5" t="inlineStr">
+      <is>
+        <t>S1</t>
+      </is>
+    </oc>
+    <nc r="K5"/>
+  </rcc>
+  <rcc rId="917" sId="10">
+    <oc r="L5" t="inlineStr">
+      <is>
+        <t>S2</t>
+      </is>
+    </oc>
+    <nc r="L5"/>
+  </rcc>
+  <rcc rId="918" sId="10">
+    <oc r="M5" t="inlineStr">
+      <is>
+        <t>S3</t>
+      </is>
+    </oc>
+    <nc r="M5"/>
+  </rcc>
+  <rcc rId="919" sId="10">
+    <oc r="N5" t="inlineStr">
+      <is>
+        <t>S4</t>
+      </is>
+    </oc>
+    <nc r="N5"/>
+  </rcc>
+  <rcc rId="920" sId="10">
+    <oc r="J6" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </oc>
+    <nc r="J6"/>
+  </rcc>
+  <rcc rId="921" sId="10">
+    <oc r="K6" t="inlineStr">
+      <is>
+        <t>S1</t>
+      </is>
+    </oc>
+    <nc r="K6"/>
+  </rcc>
+  <rcc rId="922" sId="10">
+    <oc r="L6" t="inlineStr">
+      <is>
+        <t>S2</t>
+      </is>
+    </oc>
+    <nc r="L6"/>
+  </rcc>
+  <rcc rId="923" sId="10">
+    <oc r="M6" t="inlineStr">
+      <is>
+        <t>S3</t>
+      </is>
+    </oc>
+    <nc r="M6"/>
+  </rcc>
+  <rcc rId="924" sId="10">
+    <oc r="N6" t="inlineStr">
+      <is>
+        <t>S4</t>
+      </is>
+    </oc>
+    <nc r="N6"/>
+  </rcc>
+  <rcc rId="925" sId="10">
+    <oc r="O6" t="inlineStr">
+      <is>
+        <t>DOOR</t>
+      </is>
+    </oc>
+    <nc r="O6"/>
+  </rcc>
+  <rcc rId="926" sId="10">
+    <oc r="P6" t="inlineStr">
+      <is>
+        <t>DAT</t>
+      </is>
+    </oc>
+    <nc r="P6"/>
+  </rcc>
+  <rcc rId="927" sId="10">
+    <oc r="Q6" t="inlineStr">
+      <is>
+        <t>Major</t>
+      </is>
+    </oc>
+    <nc r="Q6"/>
+  </rcc>
+  <rcc rId="928" sId="10">
+    <oc r="J7" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </oc>
+    <nc r="J7"/>
+  </rcc>
+  <rcc rId="929" sId="10">
+    <oc r="W7">
+      <v>26000</v>
+    </oc>
+    <nc r="W7"/>
+  </rcc>
+  <rcc rId="930" sId="10">
+    <oc r="X7">
+      <v>2000</v>
+    </oc>
+    <nc r="X7"/>
+  </rcc>
+  <rcc rId="931" sId="10">
+    <oc r="J8" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </oc>
+    <nc r="J8"/>
+  </rcc>
+  <rcc rId="932" sId="10">
+    <oc r="AB8">
+      <v>10</v>
+    </oc>
+    <nc r="AB8"/>
+  </rcc>
+  <rcc rId="933" sId="10">
+    <oc r="AC8">
+      <v>11</v>
+    </oc>
+    <nc r="AC8"/>
+  </rcc>
+  <rcc rId="934" sId="10">
+    <oc r="AD8">
+      <v>12</v>
+    </oc>
+    <nc r="AD8"/>
+  </rcc>
+  <rcc rId="935" sId="10">
+    <oc r="AE8">
+      <v>13</v>
+    </oc>
+    <nc r="AE8"/>
+  </rcc>
+  <rcc rId="936" sId="10">
+    <oc r="AF8">
+      <v>10</v>
+    </oc>
+    <nc r="AF8"/>
+  </rcc>
+  <rcc rId="937" sId="10">
+    <oc r="AG8" t="inlineStr">
+      <is>
+        <t>cm</t>
+      </is>
+    </oc>
+    <nc r="AG8"/>
+  </rcc>
+  <rcc rId="938" sId="10">
+    <oc r="J9" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </oc>
+    <nc r="J9"/>
+  </rcc>
+  <rcc rId="939" sId="10">
+    <oc r="AH9" t="inlineStr">
+      <is>
+        <t>FOOD</t>
+      </is>
+    </oc>
+    <nc r="AH9"/>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog60.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="98" sId="6" xfDxf="1" dxf="1">
@@ -12713,8 +14310,8 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="8">
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="9">
   <userInfo guid="{0FC3EEC7-1253-40C9-80FE-72015618EED8}" name="ITLAdmin" id="-2068730528" dateTime="2018-04-13T11:51:21"/>
   <userInfo guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" name="itluser" id="-446795219" dateTime="2018-04-13T11:51:26"/>
   <userInfo guid="{44866337-4EB8-44FB-BDBC-D3FE257C9028}" name="ITLAdmin" id="-2068734883" dateTime="2018-04-26T11:22:09"/>
@@ -12723,6 +14320,7 @@
   <userInfo guid="{D364C1FA-D153-48D2-90E8-4A2B95349BD8}" name="itluser" id="-446801266" dateTime="2018-05-08T15:56:31"/>
   <userInfo guid="{34246483-AB61-4467-BA99-A34781EAEA0F}" name="ITL-USER" id="-1580131676" dateTime="2018-05-11T12:28:00"/>
   <userInfo guid="{82F04F4E-022D-4926-A8A5-D79C201A90FA}" name="ITL-USER" id="-1580134292" dateTime="2018-05-22T11:31:15"/>
+  <userInfo guid="{2E1BFB99-DAAF-481E-A4ED-F5C2B2B48C90}" name="ITL-USER" id="-1580073728" dateTime="2018-06-04T15:40:39"/>
 </users>
 </file>
 
@@ -12992,7 +14590,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13051,12 +14649,12 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -13067,7 +14665,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -13078,7 +14676,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B6" s="10"/>
       <c r="C6" s="10"/>
@@ -13089,7 +14687,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
@@ -13100,7 +14698,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -13111,7 +14709,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
@@ -13122,7 +14720,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>3</v>
@@ -13145,7 +14743,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>3</v>
@@ -13168,7 +14766,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>3</v>
@@ -13191,7 +14789,7 @@
     </row>
     <row r="13" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>3</v>
@@ -13214,7 +14812,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>3</v>
@@ -13237,7 +14835,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>3</v>
@@ -13260,7 +14858,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>3</v>
@@ -13283,7 +14881,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>3</v>
@@ -13306,18 +14904,18 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="G9" sqref="G9"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="A3" sqref="A3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="A2" sqref="A2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="G9" sqref="G9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -13329,10 +14927,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:AP1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13370,113 +14968,38 @@
     <col min="35" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>291</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>292</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="F1" s="14" t="s">
         <v>293</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>295</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="I1" s="14" t="s">
         <v>296</v>
       </c>
-      <c r="H1" s="14" t="s">
-        <v>297</v>
-      </c>
-      <c r="I1" s="14" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>298</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>299</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>303</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>306</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>308</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>310</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>312</v>
-      </c>
-      <c r="P1" s="14" t="s">
-        <v>313</v>
-      </c>
-      <c r="Q1" s="14" t="s">
-        <v>314</v>
-      </c>
-      <c r="R1" s="14" t="s">
-        <v>318</v>
-      </c>
-      <c r="S1" s="14" t="s">
-        <v>319</v>
-      </c>
-      <c r="T1" s="14" t="s">
-        <v>320</v>
-      </c>
-      <c r="U1" s="14" t="s">
-        <v>321</v>
-      </c>
-      <c r="V1" s="14" t="s">
-        <v>322</v>
-      </c>
-      <c r="W1" s="14" t="s">
-        <v>323</v>
-      </c>
-      <c r="X1" s="14" t="s">
-        <v>324</v>
-      </c>
-      <c r="Y1" s="14" t="s">
-        <v>325</v>
-      </c>
-      <c r="Z1" s="14" t="s">
-        <v>326</v>
-      </c>
-      <c r="AA1" s="14" t="s">
-        <v>327</v>
-      </c>
-      <c r="AB1" s="14" t="s">
-        <v>328</v>
-      </c>
-      <c r="AC1" s="14" t="s">
-        <v>329</v>
-      </c>
-      <c r="AD1" s="14" t="s">
-        <v>330</v>
-      </c>
-      <c r="AE1" s="14" t="s">
-        <v>331</v>
-      </c>
-      <c r="AF1" s="14" t="s">
-        <v>332</v>
-      </c>
-      <c r="AG1" s="14" t="s">
-        <v>333</v>
-      </c>
-      <c r="AH1" s="14" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>300</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>3</v>
@@ -13497,66 +15020,15 @@
         <v>15</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>304</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>307</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>309</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>311</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>315</v>
-      </c>
-      <c r="P2" s="14" t="s">
-        <v>316</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>317</v>
-      </c>
-      <c r="W2" s="14">
-        <v>26000</v>
-      </c>
-      <c r="X2" s="14">
-        <v>2000</v>
-      </c>
-      <c r="AB2" s="14">
-        <v>10</v>
-      </c>
-      <c r="AC2" s="14">
-        <v>10</v>
-      </c>
-      <c r="AD2" s="14">
-        <v>12</v>
-      </c>
-      <c r="AE2" s="14">
-        <v>11</v>
-      </c>
-      <c r="AF2" s="14">
-        <v>10</v>
-      </c>
-      <c r="AG2" s="14" t="s">
-        <v>334</v>
-      </c>
-      <c r="AH2" s="14" t="s">
-        <v>336</v>
+        <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>3</v>
@@ -13577,39 +15049,15 @@
         <v>15</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="J3" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="K3" s="14" t="s">
-        <v>304</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>307</v>
-      </c>
-      <c r="M3" s="14" t="s">
-        <v>309</v>
-      </c>
-      <c r="N3" s="14" t="s">
-        <v>311</v>
-      </c>
-      <c r="O3" s="14" t="s">
-        <v>315</v>
-      </c>
-      <c r="P3" s="14" t="s">
-        <v>316</v>
-      </c>
-      <c r="Q3" s="14" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>3</v>
@@ -13630,18 +15078,15 @@
         <v>15</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>346</v>
+        <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>3</v>
@@ -13662,30 +15107,15 @@
         <v>15</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>304</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>307</v>
-      </c>
-      <c r="M5" s="14" t="s">
-        <v>309</v>
-      </c>
-      <c r="N5" s="14" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>3</v>
@@ -13706,39 +15136,15 @@
         <v>15</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>304</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>307</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>309</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>311</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>315</v>
-      </c>
-      <c r="P6" s="14" t="s">
-        <v>316</v>
-      </c>
-      <c r="Q6" s="14" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>3</v>
@@ -13759,24 +15165,15 @@
         <v>15</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="W7" s="14">
-        <v>26000</v>
-      </c>
-      <c r="X7" s="14">
-        <v>2000</v>
+        <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>3</v>
@@ -13797,36 +15194,15 @@
         <v>15</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="AB8" s="14">
-        <v>10</v>
-      </c>
-      <c r="AC8" s="14">
-        <v>11</v>
-      </c>
-      <c r="AD8" s="14">
-        <v>12</v>
-      </c>
-      <c r="AE8" s="14">
-        <v>13</v>
-      </c>
-      <c r="AF8" s="14">
-        <v>10</v>
-      </c>
-      <c r="AG8" s="14" t="s">
-        <v>334</v>
+        <v>300</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>3</v>
@@ -13847,20 +15223,18 @@
         <v>15</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="AH9" s="14" t="s">
-        <v>336</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="AH2" sqref="AH2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="AC1" sqref="AC1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13869,10 +15243,6 @@
       <selection activeCell="E11" sqref="E11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="AC1">
-      <selection activeCell="AH2" sqref="AH2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13883,7 +15253,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13892,7 +15262,7 @@
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -13908,8 +15278,8 @@
       <c r="D1" s="14" t="s">
         <v>177</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>181</v>
+      <c r="E1" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -13925,12 +15295,16 @@
       <c r="D2" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>182</v>
+      <c r="E2" t="s">
+        <v>349</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="E3" sqref="E3"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13939,8 +15313,256 @@
       <selection activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
+  </customSheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AJ2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="26.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="35.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="32" style="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="31.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="31.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="30" style="14" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="28.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="26.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="32.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="28.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="31.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="29" style="14" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="34.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="26.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="33.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="28" style="14" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="30" style="14" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="28" style="14" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="26.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>306</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>310</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>316</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>317</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>318</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>319</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>320</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>321</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>322</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>323</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="T1" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="U1" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="V1" s="14" t="s">
+        <v>328</v>
+      </c>
+      <c r="W1" s="14" t="s">
+        <v>329</v>
+      </c>
+      <c r="X1" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="Y1" s="14" t="s">
+        <v>331</v>
+      </c>
+      <c r="Z1" s="14" t="s">
+        <v>333</v>
+      </c>
+      <c r="AA1" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="AB1" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="AC1" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="AD1" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="AE1" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="AF1" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="AG1" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="AH1" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="AI1" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="AJ1" s="14" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>305</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>309</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="O2" s="14">
+        <v>26000</v>
+      </c>
+      <c r="P2" s="14">
+        <v>2000</v>
+      </c>
+      <c r="T2" s="14">
+        <v>10</v>
+      </c>
+      <c r="U2" s="14">
+        <v>10</v>
+      </c>
+      <c r="V2" s="14">
+        <v>12</v>
+      </c>
+      <c r="W2" s="14">
+        <v>11</v>
+      </c>
+      <c r="X2" s="14">
+        <v>10</v>
+      </c>
+      <c r="Y2" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="Z2" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="AA2" s="14" t="s">
+        <v>360</v>
+      </c>
+      <c r="AB2" s="14" t="s">
+        <v>361</v>
+      </c>
+      <c r="AC2" s="14" t="s">
+        <v>362</v>
+      </c>
+      <c r="AD2" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="AE2" s="14" t="s">
+        <v>364</v>
+      </c>
+      <c r="AF2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG2" s="14">
+        <v>2200</v>
+      </c>
+      <c r="AH2" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="AI2" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="AJ2" s="14" t="s">
+        <v>367</v>
+      </c>
+    </row>
+  </sheetData>
+  <customSheetViews>
     <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D15" sqref="D15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -13948,12 +15570,132 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>376</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>378</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>381</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>314</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="K2" s="14">
+        <v>10</v>
+      </c>
+      <c r="L2" s="14">
+        <v>10</v>
+      </c>
+      <c r="M2" s="14">
+        <v>10</v>
+      </c>
+      <c r="N2" s="14">
+        <v>10</v>
+      </c>
+      <c r="O2" s="14">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="E1">
+      <selection activeCell="N2" sqref="N2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13971,46 +15713,50 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E1" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" t="s">
         <v>203</v>
       </c>
-      <c r="E1" t="s">
-        <v>204</v>
-      </c>
-      <c r="F1" t="s">
-        <v>205</v>
-      </c>
       <c r="G1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D2" t="s">
+        <v>205</v>
+      </c>
+      <c r="E2" t="s">
         <v>206</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>207</v>
-      </c>
-      <c r="E2" t="s">
-        <v>208</v>
-      </c>
-      <c r="F2" t="s">
-        <v>209</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="K12" sqref="K12"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="H1" sqref="H1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14019,10 +15765,6 @@
       <selection activeCell="K12" sqref="K12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="K12" sqref="K12"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14032,8 +15774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14072,70 +15814,70 @@
         <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" t="s">
         <v>186</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>187</v>
+      </c>
+      <c r="H1" t="s">
         <v>188</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>189</v>
       </c>
-      <c r="H1" t="s">
-        <v>190</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>191</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>192</v>
+      </c>
+      <c r="L1" t="s">
         <v>193</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>194</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>195</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>196</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>198</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>200</v>
-      </c>
       <c r="R1" t="s">
+        <v>208</v>
+      </c>
+      <c r="S1" t="s">
         <v>210</v>
       </c>
-      <c r="S1" t="s">
-        <v>212</v>
-      </c>
       <c r="T1" t="s">
+        <v>250</v>
+      </c>
+      <c r="U1" t="s">
+        <v>251</v>
+      </c>
+      <c r="V1" t="s">
         <v>252</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>253</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>254</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>255</v>
-      </c>
-      <c r="X1" t="s">
-        <v>256</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -14143,35 +15885,39 @@
         <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>28</v>
       </c>
       <c r="R2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="S2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="O1">
+      <selection activeCell="Y1" sqref="Y1"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="D2" sqref="D2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14180,10 +15926,6 @@
       <selection activeCell="Y1" sqref="Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="O1">
-      <selection activeCell="Y1" sqref="Y1"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14193,8 +15935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE2"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14530,17 +16272,17 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="V1">
+      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="J1">
       <selection activeCell="U3" sqref="U3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="V1">
-      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="V1">
       <selection activeCell="AA1" sqref="AA1:AA1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -14556,7 +16298,7 @@
   <dimension ref="A1:AT25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14628,85 +16370,85 @@
         <v>86</v>
       </c>
       <c r="T1" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="U1" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="V1" s="11" t="s">
         <v>267</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="W1" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="X1" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="Y1" s="11" t="s">
         <v>269</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="Z1" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="AA1" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="AB1" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC1" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="AD1" s="11" t="s">
         <v>270</v>
       </c>
-      <c r="X1" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="Y1" s="11" t="s">
+      <c r="AE1" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="AF1" s="11" t="s">
         <v>271</v>
       </c>
-      <c r="Z1" s="11" t="s">
-        <v>232</v>
-      </c>
-      <c r="AA1" s="11" t="s">
-        <v>233</v>
-      </c>
-      <c r="AB1" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="AC1" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="AD1" s="11" t="s">
+      <c r="AG1" s="11" t="s">
         <v>272</v>
       </c>
-      <c r="AE1" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="AF1" s="11" t="s">
+      <c r="AH1" s="11" t="s">
         <v>273</v>
       </c>
-      <c r="AG1" s="11" t="s">
+      <c r="AI1" s="11" t="s">
         <v>274</v>
       </c>
-      <c r="AH1" s="11" t="s">
+      <c r="AJ1" s="11" t="s">
         <v>275</v>
       </c>
-      <c r="AI1" s="11" t="s">
+      <c r="AK1" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="AJ1" s="11" t="s">
+      <c r="AL1" s="11" t="s">
         <v>277</v>
       </c>
-      <c r="AK1" s="11" t="s">
+      <c r="AM1" s="11" t="s">
         <v>278</v>
       </c>
-      <c r="AL1" s="11" t="s">
+      <c r="AN1" s="11" t="s">
         <v>279</v>
       </c>
-      <c r="AM1" s="11" t="s">
+      <c r="AO1" s="11" t="s">
         <v>280</v>
       </c>
-      <c r="AN1" s="11" t="s">
+      <c r="AP1" s="11" t="s">
         <v>281</v>
       </c>
-      <c r="AO1" s="11" t="s">
+      <c r="AQ1" s="11" t="s">
         <v>282</v>
       </c>
-      <c r="AP1" s="11" t="s">
+      <c r="AR1" s="11" t="s">
         <v>283</v>
       </c>
-      <c r="AQ1" s="11" t="s">
+      <c r="AS1" s="11" t="s">
         <v>284</v>
       </c>
-      <c r="AR1" s="11" t="s">
-        <v>285</v>
-      </c>
-      <c r="AS1" s="11" t="s">
-        <v>286</v>
-      </c>
       <c r="AT1" s="11" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
@@ -14796,37 +16538,37 @@
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>235</v>
+      </c>
+      <c r="R3" t="s">
+        <v>246</v>
+      </c>
+      <c r="S3" t="s">
+        <v>246</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="V3" s="11" t="s">
         <v>237</v>
       </c>
-      <c r="R3" t="s">
-        <v>248</v>
-      </c>
-      <c r="S3" t="s">
-        <v>248</v>
-      </c>
-      <c r="T3" s="11" t="s">
+      <c r="W3" s="11" t="s">
         <v>238</v>
       </c>
-      <c r="U3" s="11" t="s">
-        <v>238</v>
-      </c>
-      <c r="V3" s="11" t="s">
+      <c r="X3" s="11" t="s">
         <v>239</v>
-      </c>
-      <c r="W3" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="X3" s="11" t="s">
-        <v>241</v>
       </c>
       <c r="Y3" s="11">
         <v>10012</v>
       </c>
       <c r="Z3" s="11" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="AA3" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="AB3" s="11"/>
       <c r="AC3" s="11"/>
@@ -14850,14 +16592,14 @@
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="S4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="T4" s="11"/>
       <c r="U4" s="11" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="V4" s="11"/>
       <c r="W4" s="11"/>
@@ -14872,13 +16614,13 @@
         <v>55</v>
       </c>
       <c r="AD4" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="AE4" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="AF4" s="11" t="s">
         <v>246</v>
-      </c>
-      <c r="AE4" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="AF4" s="11" t="s">
-        <v>248</v>
       </c>
       <c r="AG4" s="11"/>
       <c r="AH4" s="11"/>
@@ -14893,17 +16635,17 @@
       <c r="AQ4" s="11"/>
       <c r="AR4" s="11"/>
       <c r="AS4" s="11" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="AT4" s="11"/>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="T5" s="11"/>
       <c r="U5" s="11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="V5" s="11"/>
       <c r="W5" s="11"/>
@@ -14919,43 +16661,43 @@
         <v>87</v>
       </c>
       <c r="AG5" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AH5" s="13">
         <v>0.54166666666666663</v>
       </c>
       <c r="AI5" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="AJ5" s="13">
         <v>0.58680555555555558</v>
       </c>
       <c r="AK5" s="12" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="AL5" s="13">
         <v>0.33680555555555558</v>
       </c>
       <c r="AM5" s="12" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="AN5" s="13">
         <v>0.70486111111111116</v>
       </c>
       <c r="AO5" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="AP5" s="13">
         <v>0.2951388888888889</v>
       </c>
       <c r="AQ5" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="AR5" s="13">
         <v>0.67083333333333339</v>
       </c>
       <c r="AS5" s="11" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="AT5" s="11"/>
     </row>
@@ -14976,67 +16718,67 @@
         <v>87</v>
       </c>
       <c r="AG6" s="12" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="AH6" s="13">
         <v>0.54166666666666663</v>
       </c>
       <c r="AI6" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="AJ6" s="13">
         <v>0.58680555555555558</v>
       </c>
       <c r="AK6" s="12" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="AL6" s="13">
         <v>0.33680555555555558</v>
       </c>
       <c r="AM6" s="12" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="AN6" s="13">
         <v>0.70486111111111116</v>
       </c>
       <c r="AO6" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="AP6" s="13">
         <v>0.2951388888888889</v>
       </c>
       <c r="AQ6" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="AR6" s="13">
         <v>0.52361111111111114</v>
       </c>
       <c r="AS6" s="11"/>
       <c r="AT6" s="11" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="22" spans="40:41" x14ac:dyDescent="0.25">
       <c r="AO22" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="25" spans="40:41" x14ac:dyDescent="0.25">
       <c r="AN25" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="A3" sqref="A3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="A3" sqref="A3:XFD3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -15063,37 +16805,37 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>258</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="E1" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="E1" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>217</v>
-      </c>
-      <c r="H1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>261</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>263</v>
-      </c>
-      <c r="K1" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>265</v>
       </c>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
@@ -15102,20 +16844,20 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="I2" s="8">
         <v>155</v>
@@ -15134,32 +16876,32 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="F3" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>224</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>226</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
       <c r="L3" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -15168,7 +16910,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -15178,10 +16920,10 @@
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K4" s="8"/>
       <c r="L4" s="8"/>
@@ -15192,7 +16934,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -15212,6 +16954,10 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="Q1" sqref="Q1:Y1"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="Q1" sqref="Q1:Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15220,10 +16966,6 @@
       <selection activeCell="Q1" sqref="Q1:Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="Q1" sqref="Q1:Y1"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15233,7 +16975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="W1" workbookViewId="0">
       <selection activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
@@ -15459,6 +17201,11 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="W1">
+      <selection activeCell="AI2" sqref="AI2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="AI2" sqref="AI2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15466,15 +17213,11 @@
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="W1">
       <selection activeCell="AI2" sqref="AI2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
-    </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="W1">
-      <selection activeCell="AI2" sqref="AI2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -15551,17 +17294,17 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="G1" sqref="G1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="G1" sqref="G1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="G1" sqref="G1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -15594,79 +17337,83 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B3" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>346</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>347</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="B1" sqref="B1"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15675,10 +17422,6 @@
       <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="B1" sqref="B1"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Dinesh - Updated ReeferMonitor test data
</commit_message>
<xml_diff>
--- a/Basic Test Suite/TestData/TestData.xlsx
+++ b/Basic Test Suite/TestData/TestData.xlsx
@@ -5,38 +5,40 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ITL-USER\Desktop\TestComplete\Basic Test Suite\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itluser\Desktop\TestCompleteLatest\Basic Test Suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="9" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="SparcsN4Login" sheetId="1" r:id="rId1"/>
-    <sheet name="XPS" sheetId="9" r:id="rId2"/>
-    <sheet name="EDI" sheetId="2" r:id="rId3"/>
-    <sheet name="Gate" sheetId="3" r:id="rId4"/>
-    <sheet name="Vessel" sheetId="4" r:id="rId5"/>
-    <sheet name="Rail" sheetId="5" r:id="rId6"/>
-    <sheet name="Orders" sheetId="6" r:id="rId7"/>
-    <sheet name="Inventory" sheetId="7" r:id="rId8"/>
-    <sheet name="UnitFacilityVisit" sheetId="8" r:id="rId9"/>
-    <sheet name="N4MobileCommonRoutines" sheetId="10" r:id="rId10"/>
-    <sheet name="SparcsN4CommonRoutines" sheetId="11" r:id="rId11"/>
-    <sheet name="YardInventoryQuery" sheetId="12" r:id="rId12"/>
-    <sheet name="YardInspection" sheetId="13" r:id="rId13"/>
+    <sheet name="cdsds" sheetId="14" state="hidden" r:id="rId1"/>
+    <sheet name="SparcsN4Login" sheetId="1" r:id="rId2"/>
+    <sheet name="XPS" sheetId="9" r:id="rId3"/>
+    <sheet name="EDI" sheetId="2" r:id="rId4"/>
+    <sheet name="Gate" sheetId="3" r:id="rId5"/>
+    <sheet name="Vessel" sheetId="4" r:id="rId6"/>
+    <sheet name="Rail" sheetId="5" r:id="rId7"/>
+    <sheet name="Orders" sheetId="6" r:id="rId8"/>
+    <sheet name="Inventory" sheetId="7" r:id="rId9"/>
+    <sheet name="UnitFacilityVisit" sheetId="8" r:id="rId10"/>
+    <sheet name="N4MobileCommonRoutines" sheetId="10" r:id="rId11"/>
+    <sheet name="SparcsN4CommonRoutines" sheetId="11" r:id="rId12"/>
+    <sheet name="YardInventoryQuery" sheetId="12" r:id="rId13"/>
+    <sheet name="ReeferMonitor" sheetId="15" r:id="rId14"/>
+    <sheet name="YardInspection" sheetId="13" r:id="rId15"/>
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="itluser - Personal View" guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="1"/>
+    <customWorkbookView name="ITLAdmin - Personal View" guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1362" windowHeight="503" activeSheetId="11"/>
     <customWorkbookView name="ITL-USER - Personal View" guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1380" windowHeight="744" activeSheetId="13"/>
-    <customWorkbookView name="itluser - Personal View" guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" activeSheetId="9"/>
-    <customWorkbookView name="ITLAdmin - Personal View" guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1362" windowHeight="503" activeSheetId="11"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="418">
   <si>
     <t>Flow Name</t>
   </si>
@@ -1233,6 +1235,63 @@
   </si>
   <si>
     <t>Yard Inspection</t>
+  </si>
+  <si>
+    <t>dfbdx fd fd</t>
+  </si>
+  <si>
+    <t>n4Wheeled Unit</t>
+  </si>
+  <si>
+    <t>n4ReturnTemp</t>
+  </si>
+  <si>
+    <t>n4SupplyTemp</t>
+  </si>
+  <si>
+    <t>n4notes</t>
+  </si>
+  <si>
+    <t>n4FaultCode</t>
+  </si>
+  <si>
+    <t>n4Vent</t>
+  </si>
+  <si>
+    <t>n4VentUnit</t>
+  </si>
+  <si>
+    <t>n4Humidity</t>
+  </si>
+  <si>
+    <t>n4Co2</t>
+  </si>
+  <si>
+    <t>n4Oxygen</t>
+  </si>
+  <si>
+    <t>n4TemperatureSetPoint</t>
+  </si>
+  <si>
+    <t>n4GenSetid</t>
+  </si>
+  <si>
+    <t>n4Fuelevel</t>
+  </si>
+  <si>
+    <t>N4MobileReeferMonitor</t>
+  </si>
+  <si>
+    <t>Reefer Monitor</t>
+  </si>
+  <si>
+    <t>SBSU12345690</t>
+  </si>
+  <si>
+    <t>s1</t>
+  </si>
+  <si>
+    <t>Percentage</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1289,6 +1348,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1308,7 +1369,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C5987485-93A6-4D54-8156-0B4DA73E93EF}" diskRevisions="1" revisionId="1178" version="208">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B811EF09-604A-4F66-AA58-B7F52E2BFBC7}" diskRevisions="1" revisionId="1224" version="211">
   <header guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" dateTime="2018-04-13T11:49:43" maxSheetId="10" userName="itluser" r:id="rId7" minRId="7">
     <sheetIdMap count="9">
       <sheetId val="1"/>
@@ -4202,6 +4263,63 @@
       <sheetId val="13"/>
     </sheetIdMap>
   </header>
+  <header guid="{62C13622-6051-4D43-AB3A-4313F48755D8}" dateTime="2018-06-05T18:09:26" maxSheetId="16" userName="itluser" r:id="rId209" minRId="1179" maxRId="1182">
+    <sheetIdMap count="15">
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="14"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5E9307BE-C8FF-489A-A353-020DEE10E1B7}" dateTime="2018-06-05T18:11:05" maxSheetId="16" userName="itluser" r:id="rId210" minRId="1183" maxRId="1222">
+    <sheetIdMap count="15">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B811EF09-604A-4F66-AA58-B7F52E2BFBC7}" dateTime="2018-06-05T18:11:37" maxSheetId="16" userName="itluser" r:id="rId211" minRId="1223" maxRId="1224">
+    <sheetIdMap count="15">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -13997,6 +14115,331 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog203.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <ris rId="1179" sheetId="14" name="[TestData.xlsx]Sheet1" sheetPosition="2"/>
+  <ris rId="1180" sheetId="15" name="[TestData.xlsx]Sheet2" sheetPosition="13"/>
+  <rrc rId="1181" sId="14" eol="1" ref="A7:XFD7" action="insertRow"/>
+  <rcc rId="1182" sId="14">
+    <nc r="C7" t="inlineStr">
+      <is>
+        <t>dfbdx fd fd</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" action="delete"/>
+  <rcv guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog204.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1183" sId="15" xfDxf="1" dxf="1">
+    <nc r="A1" t="inlineStr">
+      <is>
+        <t>Flow Name</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1184" sId="15" xfDxf="1" dxf="1">
+    <nc r="B1" t="inlineStr">
+      <is>
+        <t>n4MobileUserName</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1185" sId="15" xfDxf="1" dxf="1">
+    <nc r="C1" t="inlineStr">
+      <is>
+        <t>n4MobilePassword</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1186" sId="15" xfDxf="1" dxf="1">
+    <nc r="D1" t="inlineStr">
+      <is>
+        <t>n4MobileOperator</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1187" sId="15" xfDxf="1" dxf="1">
+    <nc r="E1" t="inlineStr">
+      <is>
+        <t>n4MobileComplex</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1188" sId="15" xfDxf="1" dxf="1">
+    <nc r="F1" t="inlineStr">
+      <is>
+        <t>n4MobileFacility</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1189" sId="15" xfDxf="1" dxf="1">
+    <nc r="G1" t="inlineStr">
+      <is>
+        <t>n4MobileYard</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1190" sId="15" xfDxf="1" dxf="1">
+    <nc r="H1" t="inlineStr">
+      <is>
+        <t>n4MobileProgram</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1191" sId="15" xfDxf="1" dxf="1">
+    <nc r="I1" t="inlineStr">
+      <is>
+        <t>n4Wheeled Unit</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1192" sId="15" xfDxf="1" dxf="1">
+    <nc r="J1" t="inlineStr">
+      <is>
+        <t>n4ReturnTemp</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1193" sId="15" xfDxf="1" dxf="1">
+    <nc r="K1" t="inlineStr">
+      <is>
+        <t>n4SupplyTemp</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1194" sId="15" xfDxf="1" dxf="1">
+    <nc r="L1" t="inlineStr">
+      <is>
+        <t>n4notes</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1195" sId="15" xfDxf="1" dxf="1">
+    <nc r="M1" t="inlineStr">
+      <is>
+        <t>n4FaultCode</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1196" sId="15" xfDxf="1" dxf="1">
+    <nc r="N1" t="inlineStr">
+      <is>
+        <t>n4Vent</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1197" sId="15" xfDxf="1" dxf="1">
+    <nc r="O1" t="inlineStr">
+      <is>
+        <t>n4VentUnit</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1198" sId="15" xfDxf="1" dxf="1">
+    <nc r="P1" t="inlineStr">
+      <is>
+        <t>n4Humidity</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1199" sId="15" xfDxf="1" dxf="1">
+    <nc r="Q1" t="inlineStr">
+      <is>
+        <t>n4Co2</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1200" sId="15" xfDxf="1" dxf="1">
+    <nc r="R1" t="inlineStr">
+      <is>
+        <t>n4Oxygen</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1201" sId="15" xfDxf="1" dxf="1">
+    <nc r="S1" t="inlineStr">
+      <is>
+        <t>n4TemperatureSetPoint</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1202" sId="15" xfDxf="1" dxf="1">
+    <nc r="T1" t="inlineStr">
+      <is>
+        <t>n4GenSetid</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1203" sId="15" xfDxf="1" dxf="1">
+    <nc r="U1" t="inlineStr">
+      <is>
+        <t>n4Fuelevel</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1204" sId="15" xfDxf="1" dxf="1">
+    <nc r="A2" t="inlineStr">
+      <is>
+        <t>N4MobileReeferMonitor</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1205" sId="15" xfDxf="1" dxf="1">
+    <nc r="B2" t="inlineStr">
+      <is>
+        <t>admin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1206" sId="15" xfDxf="1" dxf="1">
+    <nc r="C2" t="inlineStr">
+      <is>
+        <t>Admin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1207" sId="15" xfDxf="1" dxf="1">
+    <nc r="D2" t="inlineStr">
+      <is>
+        <t>OPR1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1208" sId="15" xfDxf="1" dxf="1">
+    <nc r="E2" t="inlineStr">
+      <is>
+        <t>CPX11</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1209" sId="15" xfDxf="1" dxf="1">
+    <nc r="F2" t="inlineStr">
+      <is>
+        <t>FCY111</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1210" sId="15" xfDxf="1" dxf="1">
+    <nc r="G2" t="inlineStr">
+      <is>
+        <t>YRD1111</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1211" sId="15" xfDxf="1" dxf="1">
+    <nc r="H2" t="inlineStr">
+      <is>
+        <t>Reefer Monitor</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1212" sId="15" xfDxf="1" dxf="1">
+    <nc r="I2" t="inlineStr">
+      <is>
+        <t>SBSU12345690</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1213" sId="15" xfDxf="1" dxf="1">
+    <nc r="J2">
+      <v>22</v>
+    </nc>
+  </rcc>
+  <rcc rId="1214" sId="15" xfDxf="1" dxf="1">
+    <nc r="K2">
+      <v>15</v>
+    </nc>
+  </rcc>
+  <rcc rId="1215" sId="15" xfDxf="1" dxf="1">
+    <nc r="L2" t="inlineStr">
+      <is>
+        <t>s1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="15" xfDxf="1" sqref="M2" start="0" length="0"/>
+  <rfmt sheetId="15" xfDxf="1" sqref="N2" start="0" length="0"/>
+  <rcc rId="1216" sId="15" xfDxf="1" dxf="1">
+    <nc r="O2" t="inlineStr">
+      <is>
+        <t>Percentage</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1217" sId="15" xfDxf="1" dxf="1">
+    <nc r="P2">
+      <v>0.255</v>
+    </nc>
+  </rcc>
+  <rfmt sheetId="15" xfDxf="1" sqref="Q2" start="0" length="0"/>
+  <rfmt sheetId="15" xfDxf="1" sqref="R2" start="0" length="0"/>
+  <rfmt sheetId="15" xfDxf="1" sqref="S2" start="0" length="0"/>
+  <rfmt sheetId="15" xfDxf="1" sqref="T2" start="0" length="0"/>
+  <rcc rId="1218" sId="15" xfDxf="1" dxf="1">
+    <nc r="U2">
+      <v>75</v>
+    </nc>
+  </rcc>
+  <rcc rId="1219" sId="1" odxf="1">
+    <oc r="A18" t="inlineStr">
+      <is>
+        <t>Play</t>
+      </is>
+    </oc>
+    <nc r="A18" t="inlineStr">
+      <is>
+        <t>N4MobileReeferMonitor</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1220" sId="1">
+    <nc r="A19" t="inlineStr">
+      <is>
+        <t xml:space="preserve"> </t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" action="delete"/>
+  <rcv guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" action="add"/>
+  <rsnm rId="1221" sheetId="14" oldName="[TestData.xlsx]Sheet1" newName="[TestData.xlsx]cdsds"/>
+  <rsnm rId="1222" sheetId="15" oldName="[TestData.xlsx]Sheet2" newName="[TestData.xlsx]ReeferMonitor"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog205.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1223" sId="1">
+    <oc r="A18" t="inlineStr">
+      <is>
+        <t>N4MobileReeferMonitor</t>
+      </is>
+    </oc>
+    <nc r="A18" t="inlineStr">
+      <is>
+        <t>Play</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1224" sId="1" xfDxf="1" dxf="1">
+    <oc r="A19" t="inlineStr">
+      <is>
+        <t xml:space="preserve"> </t>
+      </is>
+    </oc>
+    <nc r="A19" t="inlineStr">
+      <is>
+        <t>N4MobileReeferMonitor</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog21.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="25" sId="3">
@@ -16437,7 +16880,7 @@
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="9">
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="10">
   <userInfo guid="{0FC3EEC7-1253-40C9-80FE-72015618EED8}" name="ITLAdmin" id="-2068730528" dateTime="2018-04-13T11:51:21"/>
   <userInfo guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" name="itluser" id="-446795219" dateTime="2018-04-13T11:51:26"/>
   <userInfo guid="{44866337-4EB8-44FB-BDBC-D3FE257C9028}" name="ITLAdmin" id="-2068734883" dateTime="2018-04-26T11:22:09"/>
@@ -16447,6 +16890,7 @@
   <userInfo guid="{34246483-AB61-4467-BA99-A34781EAEA0F}" name="ITL-USER" id="-1580131676" dateTime="2018-05-11T12:28:00"/>
   <userInfo guid="{82F04F4E-022D-4926-A8A5-D79C201A90FA}" name="ITL-USER" id="-1580134292" dateTime="2018-05-22T11:31:15"/>
   <userInfo guid="{C5987485-93A6-4D54-8156-0B4DA73E93EF}" name="ITL-USER" id="-1580073728" dateTime="2018-06-04T15:40:39"/>
+  <userInfo guid="{B811EF09-604A-4F66-AA58-B7F52E2BFBC7}" name="itluser" id="-446809699" dateTime="2018-06-05T18:12:58"/>
 </users>
 </file>
 
@@ -16713,355 +17157,148 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="7" spans="3:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="14" t="s">
+        <v>399</v>
+      </c>
+    </row>
+  </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" state="hidden">
+      <selection activeCell="H18" sqref="H18"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
+      <c r="B1" s="14" t="s">
+        <v>336</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>343</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>344</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>200</v>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>344</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>345</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>346</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>335</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>344</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>344</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>338</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>344</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>344</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>298</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>303</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>341</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>335</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>337</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>338</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>339</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>340</v>
       </c>
-      <c r="B17" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>397</v>
+      <c r="B8" s="14" t="s">
+        <v>344</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="G9" sqref="G9"/>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId1"/>
-    </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="A3" sqref="A3"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup orientation="portrait" r:id="rId3"/>
+    </customSheetView>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="B1" sqref="B1"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17388,29 +17625,29 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="A3" sqref="A3:A9"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="AC1" sqref="AC1"/>
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="E11" sqref="E11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="A3" sqref="A3:A9"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17458,29 +17695,29 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="E2" sqref="E2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="E2" sqref="E2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ9"/>
   <sheetViews>
     <sheetView topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AL6" sqref="AL6"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18263,6 +18500,10 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="AG1">
+      <selection activeCell="G15" sqref="G15"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="AG1">
       <selection activeCell="AL6" sqref="AL6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18272,12 +18513,151 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>290</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>400</v>
+      </c>
+      <c r="J1" s="15" t="s">
+        <v>401</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>402</v>
+      </c>
+      <c r="L1" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>404</v>
+      </c>
+      <c r="N1" s="15" t="s">
+        <v>405</v>
+      </c>
+      <c r="O1" s="15" t="s">
+        <v>406</v>
+      </c>
+      <c r="P1" s="15" t="s">
+        <v>407</v>
+      </c>
+      <c r="Q1" s="15" t="s">
+        <v>408</v>
+      </c>
+      <c r="R1" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="S1" s="15" t="s">
+        <v>410</v>
+      </c>
+      <c r="T1" s="15" t="s">
+        <v>411</v>
+      </c>
+      <c r="U1" s="15" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>414</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>415</v>
+      </c>
+      <c r="J2" s="15">
+        <v>22</v>
+      </c>
+      <c r="K2" s="15">
+        <v>15</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>416</v>
+      </c>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15" t="s">
+        <v>417</v>
+      </c>
+      <c r="P2" s="15">
+        <v>0.255</v>
+      </c>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="A2" sqref="A2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+  </customSheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:AA3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18523,6 +18903,10 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="D1">
+      <selection activeCell="G15" sqref="G15"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="O1">
       <selection activeCell="Z2" sqref="Z2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18534,10 +18918,360 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="9.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>303</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>335</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>337</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>338</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>413</v>
+      </c>
+    </row>
+  </sheetData>
+  <customSheetViews>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="A19" sqref="A19"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+      <selection activeCell="A2" sqref="A2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId2"/>
+    </customSheetView>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="G9" sqref="G9"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup orientation="portrait" r:id="rId3"/>
+    </customSheetView>
+  </customSheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18595,29 +19329,29 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="K12" sqref="K12"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="K12" sqref="K12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="K12" sqref="K12"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18756,29 +19490,29 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="O1">
-      <selection activeCell="Y1" sqref="Y1"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="O1">
       <selection activeCell="Y1" sqref="Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="O1">
+      <selection activeCell="Y1" sqref="Y1"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE2"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19114,17 +19848,17 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="V1">
-      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="J1">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="J1">
-      <selection activeCell="U3" sqref="U3"/>
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="V1">
+      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="V1">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="V1">
       <selection activeCell="AA1" sqref="AA1:AA1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -19135,12 +19869,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19612,29 +20346,29 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="A3" sqref="A3:XFD3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Y1"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19796,29 +20530,29 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="Q1" sqref="Q1:Y1"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="Q1" sqref="Q1:Y1"/>
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="Q1" sqref="Q1:Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="Q1" sqref="Q1:Y1"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AI2" sqref="AI2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20043,32 +20777,31 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="W1">
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="W1">
       <selection activeCell="AI2" sqref="AI2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="AI2" sqref="AI2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="W1">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="W1">
       <selection activeCell="AI2" sqref="AI2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20136,17 +20869,17 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="G1" sqref="G1"/>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="G1" sqref="G1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="G1" sqref="G1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
@@ -20155,116 +20888,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="14"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>336</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>342</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>303</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>341</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>344</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
-        <v>335</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>337</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>338</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>339</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>340</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>344</v>
-      </c>
-    </row>
-  </sheetData>
-  <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="B1" sqref="B1"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="B1" sqref="B1"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
-      <selection activeCell="B1" sqref="B1"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-  </customSheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Dinesh - Updated rail inventory cases and test data
</commit_message>
<xml_diff>
--- a/Basic Test Suite/TestData/TestData.xlsx
+++ b/Basic Test Suite/TestData/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itluser\Desktop\TestCompleteLatest\Test Complete\Basic Test Suite\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itluser\Desktop\TestCompleteLatest\Basic Test Suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="10" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="cdsds" sheetId="14" state="hidden" r:id="rId1"/>
@@ -32,15 +32,15 @@
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="ITLAdmin - Personal View" guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1362" windowHeight="503" activeSheetId="11"/>
     <customWorkbookView name="ITL-USER - Personal View" guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1380" windowHeight="744" activeSheetId="16"/>
-    <customWorkbookView name="ITLAdmin - Personal View" guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1362" windowHeight="503" activeSheetId="11"/>
     <customWorkbookView name="itluser - Personal View" guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1380" windowHeight="744" activeSheetId="17"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="452">
   <si>
     <t>Flow Name</t>
   </si>
@@ -1372,6 +1372,30 @@
   </si>
   <si>
     <t>STD</t>
+  </si>
+  <si>
+    <t>n4Track</t>
+  </si>
+  <si>
+    <t>n4Position</t>
+  </si>
+  <si>
+    <t>n4TransferPoint</t>
+  </si>
+  <si>
+    <t>n4Metermark</t>
+  </si>
+  <si>
+    <t>Rail Inventory</t>
+  </si>
+  <si>
+    <t>Reefer Monitor</t>
+  </si>
+  <si>
+    <t>n4ClickEditSegBreak</t>
+  </si>
+  <si>
+    <t>n4AddContainer1</t>
   </si>
 </sst>
 </file>
@@ -1449,7 +1473,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{EC6B99F2-BAFB-4F81-BF30-4ACACEB126F7}" diskRevisions="1" revisionId="1303" version="232">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{0C6D09E4-075A-4EDD-B3D4-023B29F5DABC}" diskRevisions="1" revisionId="1315" version="241">
   <header guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" dateTime="2018-04-13T11:49:43" maxSheetId="10" userName="itluser" r:id="rId7" minRId="7">
     <sheetIdMap count="9">
       <sheetId val="1"/>
@@ -4791,6 +4815,195 @@
     </sheetIdMap>
   </header>
   <header guid="{EC6B99F2-BAFB-4F81-BF30-4ACACEB126F7}" dateTime="2018-06-08T17:40:12" maxSheetId="18" userName="itluser" r:id="rId232" minRId="1303">
+    <sheetIdMap count="17">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{DD3A6473-9C21-414D-A18E-459A6285470C}" dateTime="2018-06-11T12:46:08" maxSheetId="18" userName="itluser" r:id="rId233" minRId="1304" maxRId="1305">
+    <sheetIdMap count="17">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{0D209139-831C-4689-928A-2628EDA819F0}" dateTime="2018-06-11T12:54:21" maxSheetId="18" userName="itluser" r:id="rId234" minRId="1306">
+    <sheetIdMap count="17">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{15739E69-FFE7-4C46-A217-ADEEF8E59BF1}" dateTime="2018-06-11T12:56:46" maxSheetId="18" userName="itluser" r:id="rId235" minRId="1307">
+    <sheetIdMap count="17">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{C471B8BC-D5C2-4D57-9853-9FFB1714C58B}" dateTime="2018-06-11T13:09:41" maxSheetId="18" userName="itluser" r:id="rId236" minRId="1308">
+    <sheetIdMap count="17">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A1AD0CC5-0532-47CD-A12D-5BA541E2F212}" dateTime="2018-06-11T13:26:28" maxSheetId="18" userName="itluser" r:id="rId237" minRId="1309">
+    <sheetIdMap count="17">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{3488DC1C-EAC7-4464-9DD0-BB50F5AD6F48}" dateTime="2018-06-11T14:33:47" maxSheetId="18" userName="itluser" r:id="rId238" minRId="1310" maxRId="1313">
+    <sheetIdMap count="17">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{38F60545-2FB9-456E-B8C0-7E0EC486F7A2}" dateTime="2018-06-11T14:45:10" maxSheetId="18" userName="itluser" r:id="rId239">
+    <sheetIdMap count="17">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{84F50593-E0B7-4A66-BC8A-81F7B4483911}" dateTime="2018-06-11T14:52:14" maxSheetId="18" userName="itluser" r:id="rId240" minRId="1314">
+    <sheetIdMap count="17">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{0C6D09E4-075A-4EDD-B3D4-023B29F5DABC}" dateTime="2018-06-11T18:04:42" maxSheetId="18" userName="itluser" r:id="rId241" minRId="1315">
     <sheetIdMap count="17">
       <sheetId val="14"/>
       <sheetId val="1"/>
@@ -15732,6 +15945,51 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog227.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1304" sId="17">
+    <nc r="G1" t="inlineStr">
+      <is>
+        <t>n4Track</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1305" sId="17" xfDxf="1" dxf="1">
+    <nc r="H1" t="inlineStr">
+      <is>
+        <t>n4Position</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" action="delete"/>
+  <rcv guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog228.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1306" sId="17" xfDxf="1" dxf="1">
+    <nc r="I1" t="inlineStr">
+      <is>
+        <t>n4TransferPoint</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog229.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1307" sId="17" xfDxf="1" dxf="1">
+    <nc r="J1" t="inlineStr">
+      <is>
+        <t>n4Metermark</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog23.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="28" sId="3">
@@ -15909,6 +16167,103 @@
   </rcc>
   <rcv guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" action="delete"/>
   <rcv guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog230.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="17" xfDxf="1" sqref="K1" start="0" length="0"/>
+  <rcc rId="1308" sId="17">
+    <nc r="K1" t="inlineStr">
+      <is>
+        <t>n4AddEditSegBreak</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog231.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1309" sId="17">
+    <nc r="K2" t="inlineStr">
+      <is>
+        <t>Yes</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog232.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1310" sId="10" odxf="1">
+    <nc r="A11" t="inlineStr">
+      <is>
+        <t>N4MobileRailInventory</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1311" sId="10" xfDxf="1" dxf="1">
+    <nc r="H11" t="inlineStr">
+      <is>
+        <t>Rail Inventory</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1312" sId="10" odxf="1">
+    <nc r="A12" t="inlineStr">
+      <is>
+        <t>N4MobileReeferMonitor</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1313" sId="10" xfDxf="1" dxf="1">
+    <nc r="H12" t="inlineStr">
+      <is>
+        <t>Reefer Monitor</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog233.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rfmt sheetId="17" xfDxf="1" sqref="K2" start="0" length="0"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog234.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1314" sId="17" xfDxf="1" dxf="1">
+    <oc r="K1" t="inlineStr">
+      <is>
+        <t>n4AddEditSegBreak</t>
+      </is>
+    </oc>
+    <nc r="K1" t="inlineStr">
+      <is>
+        <t>n4ClickEditSegBreak</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" action="delete"/>
+  <rcv guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog235.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1315" sId="17" xfDxf="1" dxf="1">
+    <nc r="L1" t="inlineStr">
+      <is>
+        <t>n4AddContainer1</t>
+      </is>
+    </nc>
+  </rcc>
 </revisions>
 </file>
 
@@ -18135,8 +18490,8 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="11">
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="12">
   <userInfo guid="{0FC3EEC7-1253-40C9-80FE-72015618EED8}" name="ITLAdmin" id="-2068730528" dateTime="2018-04-13T11:51:21"/>
   <userInfo guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" name="itluser" id="-446795219" dateTime="2018-04-13T11:51:26"/>
   <userInfo guid="{44866337-4EB8-44FB-BDBC-D3FE257C9028}" name="ITLAdmin" id="-2068734883" dateTime="2018-04-26T11:22:09"/>
@@ -18148,6 +18503,7 @@
   <userInfo guid="{C5987485-93A6-4D54-8156-0B4DA73E93EF}" name="ITL-USER" id="-1580073728" dateTime="2018-06-04T15:40:39"/>
   <userInfo guid="{B811EF09-604A-4F66-AA58-B7F52E2BFBC7}" name="itluser" id="-446809699" dateTime="2018-06-05T18:12:58"/>
   <userInfo guid="{EC6B99F2-BAFB-4F81-BF30-4ACACEB126F7}" name="itluser" id="-446781240" dateTime="2018-06-08T17:40:00"/>
+  <userInfo guid="{0C6D09E4-075A-4EDD-B3D4-023B29F5DABC}" name="itluser" id="-446797799" dateTime="2018-06-11T15:43:40"/>
 </users>
 </file>
 
@@ -18537,11 +18893,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -18556,7 +18912,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
@@ -18884,14 +19240,30 @@
         <v>398</v>
       </c>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>441</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>413</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>449</v>
+      </c>
+    </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+      <selection activeCell="E11" sqref="E11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="B1" sqref="B1"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
-      <selection activeCell="E11" sqref="E11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
@@ -18956,12 +19328,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+      <selection activeCell="B6" sqref="B6"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="E2" sqref="E2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
-      <selection activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
@@ -19855,15 +20227,25 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -19882,8 +20264,26 @@
       <c r="F1" t="s">
         <v>440</v>
       </c>
+      <c r="G1" t="s">
+        <v>444</v>
+      </c>
+      <c r="H1" t="s">
+        <v>445</v>
+      </c>
+      <c r="I1" t="s">
+        <v>446</v>
+      </c>
+      <c r="J1" t="s">
+        <v>447</v>
+      </c>
+      <c r="K1" t="s">
+        <v>450</v>
+      </c>
+      <c r="L1" t="s">
+        <v>451</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>441</v>
       </c>
@@ -19897,13 +20297,16 @@
         <v>360</v>
       </c>
       <c r="F2" t="s">
+        <v>360</v>
+      </c>
+      <c r="K2" t="s">
         <v>360</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="I14" sqref="I14"/>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="B1">
+      <selection activeCell="K1" sqref="K1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -20418,8 +20821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20748,13 +21151,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="G9" sqref="G9"/>
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+      <selection activeCell="A2" sqref="A2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
-      <selection activeCell="A2" sqref="A2"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="G9" sqref="G9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -20832,11 +21235,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="K12" sqref="K12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="K12" sqref="K12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -20993,11 +21396,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="O1">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="O1">
       <selection activeCell="Y1" sqref="Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="O1">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="O1">
       <selection activeCell="Y1" sqref="Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -21351,12 +21754,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="V1">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="V1">
       <selection activeCell="AA1" sqref="AA1:AA1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="V1">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="V1">
       <selection activeCell="AA1" sqref="AA1:AA1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -21849,11 +22252,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="A3" sqref="A3:XFD3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="A3" sqref="A3:XFD3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -22033,11 +22436,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="Q1" sqref="Q1:Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="Q1" sqref="Q1:Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -22280,12 +22683,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="W1">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="W1">
       <selection activeCell="AI2" sqref="AI2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="W1">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="W1">
       <selection activeCell="AI2" sqref="AI2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
@@ -22372,12 +22775,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="G1" sqref="G1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="G1" sqref="G1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Aswini - Updated Test Data and Script file N4MobileYardInventoryGroundedCommonRoutines
</commit_message>
<xml_diff>
--- a/Basic Test Suite/TestData/TestData.xlsx
+++ b/Basic Test Suite/TestData/TestData.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="464">
   <si>
     <t>Flow Name</t>
   </si>
@@ -1395,9 +1395,6 @@
     <t>n4AddContainer1</t>
   </si>
   <si>
-    <t>F10L</t>
-  </si>
-  <si>
     <t>n4YinvGroundTier</t>
   </si>
   <si>
@@ -1408,6 +1405,33 @@
   </si>
   <si>
     <t>n4YinvGroundTier3Container</t>
+  </si>
+  <si>
+    <t>n4YinvGroundTier1RemoveContainer</t>
+  </si>
+  <si>
+    <t>n4YinvGroundTier2RemoveContainer</t>
+  </si>
+  <si>
+    <t>n4YinvGroundTier3RemoveContainer</t>
+  </si>
+  <si>
+    <t>F10M</t>
+  </si>
+  <si>
+    <t>n4YinvGroundTier1BundleMasterContainer</t>
+  </si>
+  <si>
+    <t>n4YinvGroundTier1BundleSlaveContainer</t>
+  </si>
+  <si>
+    <t>ASWU2705180</t>
+  </si>
+  <si>
+    <t>n4YinvGroundTier2BundleMasterContainer</t>
+  </si>
+  <si>
+    <t>n4YinvGroundTier3BundleMasterContainer</t>
   </si>
 </sst>
 </file>
@@ -1485,7 +1509,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{ED6CE125-9591-4FAE-ADD5-B2299A65314E}" diskRevisions="1" revisionId="1325" version="247">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C8F755ED-221C-45B0-9557-1C03AB2567AF}" diskRevisions="1" revisionId="1341" version="257">
   <header guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" dateTime="2018-04-13T11:49:43" maxSheetId="10" userName="itluser" r:id="rId7" minRId="7">
     <sheetIdMap count="9">
       <sheetId val="1"/>
@@ -5142,6 +5166,216 @@
     </sheetIdMap>
   </header>
   <header guid="{ED6CE125-9591-4FAE-ADD5-B2299A65314E}" dateTime="2018-06-12T15:51:41" maxSheetId="18" userName="ITL-USER" r:id="rId247" minRId="1325">
+    <sheetIdMap count="17">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{8826F43F-A4AF-483A-BAF3-02E202088E24}" dateTime="2018-06-12T16:03:12" maxSheetId="18" userName="ITL-USER" r:id="rId248" minRId="1326" maxRId="1327">
+    <sheetIdMap count="17">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{EBFAFA1A-D84C-41A8-8CED-6507A5C2AF8C}" dateTime="2018-06-12T16:03:24" maxSheetId="18" userName="ITL-USER" r:id="rId249" minRId="1328">
+    <sheetIdMap count="17">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B6B37134-BC17-4EEC-A914-9A7AE28A75C1}" dateTime="2018-06-12T16:24:19" maxSheetId="18" userName="ITL-USER" r:id="rId250" minRId="1329">
+    <sheetIdMap count="17">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5FAE2148-AAF2-4BE9-90AD-43455A149156}" dateTime="2018-06-13T10:14:31" maxSheetId="18" userName="ITL-USER" r:id="rId251" minRId="1330">
+    <sheetIdMap count="17">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{DD22640A-A27E-42A0-B3B1-8CA006806E99}" dateTime="2018-06-13T11:08:41" maxSheetId="18" userName="ITL-USER" r:id="rId252" minRId="1331">
+    <sheetIdMap count="17">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B56BF2B8-C73F-4994-8110-6DBFE0D3586E}" dateTime="2018-06-13T11:12:35" maxSheetId="18" userName="ITL-USER" r:id="rId253" minRId="1332">
+    <sheetIdMap count="17">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{00CBAC07-BABA-47B5-AA6B-0581855E09A8}" dateTime="2018-06-13T12:11:05" maxSheetId="18" userName="ITL-USER" r:id="rId254" minRId="1333" maxRId="1334">
+    <sheetIdMap count="17">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{E59CABBA-2B8A-4258-B4F5-8A33915669E5}" dateTime="2018-06-13T12:13:01" maxSheetId="18" userName="ITL-USER" r:id="rId255" minRId="1335">
+    <sheetIdMap count="17">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{41290385-A8BD-4F25-9C90-178B23920B14}" dateTime="2018-06-13T12:18:42" maxSheetId="18" userName="ITL-USER" r:id="rId256" minRId="1336" maxRId="1337">
+    <sheetIdMap count="17">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{C8F755ED-221C-45B0-9557-1C03AB2567AF}" dateTime="2018-06-13T12:34:00" maxSheetId="18" userName="ITL-USER" r:id="rId257" minRId="1338" maxRId="1341">
     <sheetIdMap count="17">
       <sheetId val="14"/>
       <sheetId val="1"/>
@@ -16530,6 +16764,137 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog242.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1326" sId="16">
+    <nc r="J1" t="inlineStr">
+      <is>
+        <t>n4YinvGroundTier1RemoveContainer</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1327" sId="16">
+    <nc r="K1" t="inlineStr">
+      <is>
+        <t>n4YinvGroundTier2RemoveContainer</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog243.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1328" sId="16">
+    <nc r="L1" t="inlineStr">
+      <is>
+        <t>n4YinvGroundTier3RemoveContainer</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog244.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1329" sId="16">
+    <oc r="F2">
+      <v>2</v>
+    </oc>
+    <nc r="F2">
+      <v>3</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog245.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1330" sId="16">
+    <oc r="B2" t="inlineStr">
+      <is>
+        <t>F10L</t>
+      </is>
+    </oc>
+    <nc r="B2" t="inlineStr">
+      <is>
+        <t>F10M</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog246.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1331" sId="16">
+    <oc r="F2">
+      <v>3</v>
+    </oc>
+    <nc r="F2">
+      <v>2</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog247.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1332" sId="16">
+    <oc r="F2">
+      <v>2</v>
+    </oc>
+    <nc r="F2">
+      <v>3</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog248.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1333" sId="16">
+    <nc r="M1" t="inlineStr">
+      <is>
+        <t>n4YinvGroundTier1BundleContainer</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1334" sId="16">
+    <nc r="M2" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog249.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1335" sId="16">
+    <oc r="M1" t="inlineStr">
+      <is>
+        <t>n4YinvGroundTier1BundleContainer</t>
+      </is>
+    </oc>
+    <nc r="M1" t="inlineStr">
+      <is>
+        <t>n4YinvGroundTier1BundleMasterContainer</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog25.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="48" sId="3" xfDxf="1" dxf="1">
@@ -16539,6 +16904,64 @@
       </is>
     </nc>
   </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog250.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1336" sId="16">
+    <nc r="N1" t="inlineStr">
+      <is>
+        <t>n4YinvGroundTier1BundleSlaveContainer</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1337" sId="16">
+    <nc r="N2" t="inlineStr">
+      <is>
+        <t>ASWU2705180</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog251.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1338" sId="16">
+    <nc r="O1" t="inlineStr">
+      <is>
+        <t>n4YinvGroundTier2BundleMasterContainer</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1339" sId="16" odxf="1">
+    <nc r="O2" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1340" sId="16">
+    <nc r="P1" t="inlineStr">
+      <is>
+        <t>n4YinvGroundTier3BundleMasterContainer</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1341" sId="16" odxf="1">
+    <nc r="P2" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
 </revisions>
 </file>
 
@@ -18755,7 +19178,7 @@
   <userInfo guid="{B811EF09-604A-4F66-AA58-B7F52E2BFBC7}" name="itluser" id="-446809699" dateTime="2018-06-05T18:12:58"/>
   <userInfo guid="{EC6B99F2-BAFB-4F81-BF30-4ACACEB126F7}" name="itluser" id="-446781240" dateTime="2018-06-08T17:40:00"/>
   <userInfo guid="{0C6D09E4-075A-4EDD-B3D4-023B29F5DABC}" name="itluser" id="-446797799" dateTime="2018-06-11T15:43:40"/>
-  <userInfo guid="{ED6CE125-9591-4FAE-ADD5-B2299A65314E}" name="ITL-USER" id="-1580105203" dateTime="2018-06-12T15:40:21"/>
+  <userInfo guid="{C8F755ED-221C-45B0-9557-1C03AB2567AF}" name="ITL-USER" id="-1580079401" dateTime="2018-06-13T12:10:34"/>
 </users>
 </file>
 
@@ -20572,10 +20995,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20587,9 +21010,13 @@
     <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -20606,30 +21033,51 @@
         <v>434</v>
       </c>
       <c r="F1" t="s">
+        <v>451</v>
+      </c>
+      <c r="G1" t="s">
         <v>452</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>453</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>454</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>455</v>
       </c>
+      <c r="K1" t="s">
+        <v>456</v>
+      </c>
+      <c r="L1" t="s">
+        <v>457</v>
+      </c>
+      <c r="M1" t="s">
+        <v>459</v>
+      </c>
+      <c r="N1" t="s">
+        <v>460</v>
+      </c>
+      <c r="O1" t="s">
+        <v>462</v>
+      </c>
+      <c r="P1" t="s">
+        <v>463</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>298</v>
       </c>
       <c r="B2" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="E2" t="s">
         <v>344</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
         <v>344</v>
@@ -20638,13 +21086,25 @@
         <v>344</v>
       </c>
       <c r="I2" t="s">
+        <v>344</v>
+      </c>
+      <c r="M2" t="s">
+        <v>344</v>
+      </c>
+      <c r="N2" t="s">
+        <v>461</v>
+      </c>
+      <c r="O2" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="P2" s="16" t="s">
         <v>344</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="D1">
-      <selection activeCell="I2" sqref="I2"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="M1">
+      <selection activeCell="P2" sqref="P2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">

</xml_diff>

<commit_message>
Aswini - Updated N4MobileGateInspectionCommonRoutines
</commit_message>
<xml_diff>
--- a/Basic Test Suite/TestData/TestData.xlsx
+++ b/Basic Test Suite/TestData/TestData.xlsx
@@ -34,14 +34,14 @@
   <calcPr calcId="145621"/>
   <customWorkbookViews>
     <customWorkbookView name="ITL-USER - Personal View" guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1380" windowHeight="744" activeSheetId="18"/>
+    <customWorkbookView name="itluser - Personal View" guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1380" windowHeight="744" activeSheetId="17"/>
     <customWorkbookView name="ITLAdmin - Personal View" guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1362" windowHeight="503" activeSheetId="11"/>
-    <customWorkbookView name="itluser - Personal View" guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1380" windowHeight="744" activeSheetId="17"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="493">
   <si>
     <t>Flow Name</t>
   </si>
@@ -1475,6 +1475,51 @@
   </si>
   <si>
     <t>n4GInspDamageDepth</t>
+  </si>
+  <si>
+    <t>n4GInspTemperature</t>
+  </si>
+  <si>
+    <t>n4GInspTempUnit</t>
+  </si>
+  <si>
+    <t>n4GInspIsGenset</t>
+  </si>
+  <si>
+    <t>n4GInspGensetType</t>
+  </si>
+  <si>
+    <t>n4GInspGensetDamageComponent</t>
+  </si>
+  <si>
+    <t>n4GInspGensetDamageLocation</t>
+  </si>
+  <si>
+    <t>n4GInspGensetDamageType</t>
+  </si>
+  <si>
+    <t>n4GInspGensetDamageSeverity</t>
+  </si>
+  <si>
+    <t>n4GInspGensetDamageQuantity</t>
+  </si>
+  <si>
+    <t>n4GInspGensetDamageWidth</t>
+  </si>
+  <si>
+    <t>n4GInspGensetDamageLength</t>
+  </si>
+  <si>
+    <t>n4GInspGensetDamageDepth</t>
+  </si>
+  <si>
+    <t>n4GInspOOGTop</t>
+  </si>
+  <si>
+    <t>n4GInspOOGLeft</t>
+  </si>
+  <si>
+    <t>n4GInspOOGRight</t>
   </si>
 </sst>
 </file>
@@ -1552,7 +1597,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{21020E91-DEEE-4F51-9240-3827FDED4377}" diskRevisions="1" revisionId="1370" version="272">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{D1C04910-AD23-4127-92A6-F91493935D47}" diskRevisions="1" revisionId="1392" version="282">
   <header guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" dateTime="2018-04-13T11:49:43" maxSheetId="10" userName="itluser" r:id="rId7" minRId="7">
     <sheetIdMap count="9">
       <sheetId val="1"/>
@@ -5748,6 +5793,226 @@
     </sheetIdMap>
   </header>
   <header guid="{21020E91-DEEE-4F51-9240-3827FDED4377}" dateTime="2018-06-14T12:36:45" maxSheetId="19" userName="ITL-USER" r:id="rId272" minRId="1369" maxRId="1370">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{FD18459B-F42A-4E52-86F2-BA9B794E8CFA}" dateTime="2018-06-14T15:06:14" maxSheetId="19" userName="ITL-USER" r:id="rId273" minRId="1371" maxRId="1372">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{59A7DF98-1DA3-4A03-ADE2-3474AA7D97C3}" dateTime="2018-06-14T15:08:28" maxSheetId="19" userName="ITL-USER" r:id="rId274" minRId="1373" maxRId="1374">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{0DBF59CD-6673-4CAF-A9C8-9ECC5B6E849C}" dateTime="2018-06-14T15:10:12" maxSheetId="19" userName="ITL-USER" r:id="rId275" minRId="1375" maxRId="1376">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{19A378A4-4E9A-4A88-836C-EC9939D673E0}" dateTime="2018-06-14T15:10:34" maxSheetId="19" userName="ITL-USER" r:id="rId276" minRId="1377">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{339EB71B-1055-4094-AE89-7FBCD95D41C1}" dateTime="2018-06-14T15:14:36" maxSheetId="19" userName="ITL-USER" r:id="rId277" minRId="1378">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{9BF74820-0848-4F92-9688-074DE4D30DC9}" dateTime="2018-06-14T15:30:20" maxSheetId="19" userName="ITL-USER" r:id="rId278" minRId="1379" maxRId="1382">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6955F332-D62F-45DC-874E-3532B0332922}" dateTime="2018-06-14T15:31:28" maxSheetId="19" userName="ITL-USER" r:id="rId279" minRId="1383" maxRId="1386">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{3CEF21D2-8F8D-456B-989D-31E573D884B8}" dateTime="2018-06-14T17:23:30" maxSheetId="19" userName="ITL-USER" r:id="rId280" minRId="1387" maxRId="1388">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{E5F99182-E821-4435-9AD0-81F79F8DB119}" dateTime="2018-06-14T17:28:44" maxSheetId="19" userName="ITL-USER" r:id="rId281" minRId="1389" maxRId="1390">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{D1C04910-AD23-4127-92A6-F91493935D47}" dateTime="2018-06-14T17:40:28" maxSheetId="19" userName="ITL-USER" r:id="rId282" minRId="1391" maxRId="1392">
     <sheetIdMap count="18">
       <sheetId val="14"/>
       <sheetId val="1"/>
@@ -17648,6 +17913,65 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog267.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1371" sId="18">
+    <nc r="M1" t="inlineStr">
+      <is>
+        <t>n4GInspTemperature</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1372" sId="18">
+    <nc r="M2">
+      <v>15</v>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog268.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1373" sId="18">
+    <nc r="N1" t="inlineStr">
+      <is>
+        <t>n4GInspTempUnit</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1374" sId="18">
+    <nc r="N2" t="inlineStr">
+      <is>
+        <t>C</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog269.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1375" sId="18">
+    <nc r="O1" t="inlineStr">
+      <is>
+        <t>n4GInspIsGenset</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1376" sId="18">
+    <nc r="O2" t="inlineStr">
+      <is>
+        <t>No</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog27.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="50" sId="3" xfDxf="1" dxf="1">
@@ -17657,6 +17981,160 @@
       </is>
     </nc>
   </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog270.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1377" sId="18">
+    <oc r="O2" t="inlineStr">
+      <is>
+        <t>No</t>
+      </is>
+    </oc>
+    <nc r="O2"/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog271.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1378" sId="18">
+    <nc r="P1" t="inlineStr">
+      <is>
+        <t>n4GInspGensetType</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog272.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1379" sId="18">
+    <nc r="Q1" t="inlineStr">
+      <is>
+        <t>n4GInspGensetDamageComponent</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1380" sId="18">
+    <nc r="R1" t="inlineStr">
+      <is>
+        <t>n4GInspGensetDamageLocation</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1381" sId="18">
+    <nc r="S1" t="inlineStr">
+      <is>
+        <t>n4GInspGensetDamageType</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1382" sId="18">
+    <nc r="T1" t="inlineStr">
+      <is>
+        <t>n4GInspGensetDamageSeverity</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog273.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1383" sId="18">
+    <nc r="U1" t="inlineStr">
+      <is>
+        <t>n4GInspGensetDamageQuantity</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1384" sId="18">
+    <nc r="V1" t="inlineStr">
+      <is>
+        <t>n4GInspGensetDamageWidth</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1385" sId="18">
+    <nc r="W1" t="inlineStr">
+      <is>
+        <t>n4GInspGensetDamageLength</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1386" sId="18" xfDxf="1" dxf="1">
+    <nc r="X1" t="inlineStr">
+      <is>
+        <t>n4GInspGensetDamageDepth</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog274.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1387" sId="18">
+    <nc r="Y1" t="inlineStr">
+      <is>
+        <t>n4GInspOOGTop</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1388" sId="18">
+    <nc r="Y2">
+      <v>5</v>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog275.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1389" sId="18">
+    <nc r="Z1" t="inlineStr">
+      <is>
+        <t>n4GInspOOGLeft</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1390" sId="18">
+    <nc r="Z2">
+      <v>4</v>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog276.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1391" sId="18">
+    <nc r="AA1" t="inlineStr">
+      <is>
+        <t>n4GInspOOGRight</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1392" sId="18">
+    <nc r="AA2">
+      <v>3</v>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
 </revisions>
 </file>
 
@@ -19849,7 +20327,7 @@
   <userInfo guid="{B811EF09-604A-4F66-AA58-B7F52E2BFBC7}" name="itluser" id="-446809699" dateTime="2018-06-05T18:12:58"/>
   <userInfo guid="{EC6B99F2-BAFB-4F81-BF30-4ACACEB126F7}" name="itluser" id="-446781240" dateTime="2018-06-08T17:40:00"/>
   <userInfo guid="{0C6D09E4-075A-4EDD-B3D4-023B29F5DABC}" name="itluser" id="-446797799" dateTime="2018-06-11T15:43:40"/>
-  <userInfo guid="{21020E91-DEEE-4F51-9240-3827FDED4377}" name="ITL-USER" id="-1580105824" dateTime="2018-06-14T12:01:46"/>
+  <userInfo guid="{D1C04910-AD23-4127-92A6-F91493935D47}" name="ITL-USER" id="-1580119968" dateTime="2018-06-14T15:05:55"/>
 </users>
 </file>
 
@@ -20243,12 +20721,12 @@
       <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="B1" sqref="B1"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -20608,12 +21086,12 @@
       <selection activeCell="H2" sqref="H2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="E11" sqref="E11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -20678,12 +21156,12 @@
       <selection activeCell="E2" sqref="E2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="B6" sqref="B6"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -21663,10 +22141,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21683,9 +22161,24 @@
     <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -21722,8 +22215,53 @@
       <c r="L1" t="s">
         <v>477</v>
       </c>
+      <c r="M1" t="s">
+        <v>478</v>
+      </c>
+      <c r="N1" t="s">
+        <v>479</v>
+      </c>
+      <c r="O1" t="s">
+        <v>480</v>
+      </c>
+      <c r="P1" t="s">
+        <v>481</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>482</v>
+      </c>
+      <c r="R1" t="s">
+        <v>483</v>
+      </c>
+      <c r="S1" t="s">
+        <v>484</v>
+      </c>
+      <c r="T1" t="s">
+        <v>485</v>
+      </c>
+      <c r="U1" t="s">
+        <v>486</v>
+      </c>
+      <c r="V1" t="s">
+        <v>487</v>
+      </c>
+      <c r="W1" t="s">
+        <v>488</v>
+      </c>
+      <c r="X1" t="s">
+        <v>489</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>490</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>491</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>492</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>298</v>
       </c>
@@ -21758,13 +22296,28 @@
         <v>4</v>
       </c>
       <c r="L2" s="16">
+        <v>3</v>
+      </c>
+      <c r="M2" s="16">
+        <v>15</v>
+      </c>
+      <c r="N2" s="16" t="s">
+        <v>419</v>
+      </c>
+      <c r="Y2" s="16">
+        <v>5</v>
+      </c>
+      <c r="Z2" s="16">
+        <v>4</v>
+      </c>
+      <c r="AA2" s="16">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="G1">
-      <selection activeCell="L2" sqref="L2"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="U1">
+      <selection activeCell="AA2" sqref="AA2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -22677,13 +23230,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
-      <selection activeCell="A2" sqref="A2"/>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="A19" sqref="A19"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="A19" sqref="A19"/>
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+      <selection activeCell="A2" sqref="A2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -22760,12 +23313,12 @@
       <selection activeCell="K12" sqref="K12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="K12" sqref="K12"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -22921,12 +23474,12 @@
       <selection activeCell="Y1" sqref="Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="O1">
       <selection activeCell="Y1" sqref="Y1"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -23280,13 +23833,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="V1">
-      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="J1">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="J1">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="V1">
+      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -23777,12 +24330,12 @@
       <selection activeCell="A3" sqref="A3:XFD3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="A3" sqref="A3:XFD3"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -23961,12 +24514,12 @@
       <selection activeCell="Q1" sqref="Q1:Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="Q1" sqref="Q1:Y1"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -24209,14 +24762,14 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="W1">
       <selection activeCell="AI2" sqref="AI2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
-    </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="G15" sqref="G15"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24302,13 +24855,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
-      <selection activeCell="G1" sqref="G1"/>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
+      <selection activeCell="G1" sqref="G1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>

</xml_diff>

<commit_message>
Aswini - Updated TestData and Script file N4MobileGateInspectionCommonRoutines
</commit_message>
<xml_diff>
--- a/Basic Test Suite/TestData/TestData.xlsx
+++ b/Basic Test Suite/TestData/TestData.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="515">
   <si>
     <t>Flow Name</t>
   </si>
@@ -1550,6 +1550,42 @@
   </si>
   <si>
     <t>n4GInspSlaveUnit</t>
+  </si>
+  <si>
+    <t>n4GInspPositionOnTruck</t>
+  </si>
+  <si>
+    <t>n4GInspDoorDirection</t>
+  </si>
+  <si>
+    <t>n4GInspCSC</t>
+  </si>
+  <si>
+    <t>n4GInspMnf</t>
+  </si>
+  <si>
+    <t>n4GInspSafeWeight</t>
+  </si>
+  <si>
+    <t>n4GInspTareWeight</t>
+  </si>
+  <si>
+    <t>n4GInspSeal1</t>
+  </si>
+  <si>
+    <t>n4GInspSeal2</t>
+  </si>
+  <si>
+    <t>n4GInspSeal3</t>
+  </si>
+  <si>
+    <t>n4GInspSeal4</t>
+  </si>
+  <si>
+    <t>n4GInspSeal5</t>
+  </si>
+  <si>
+    <t>S5</t>
   </si>
 </sst>
 </file>
@@ -1627,7 +1663,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{65AF415F-CF80-4375-9BD5-D7BFDD3D9813}" diskRevisions="1" revisionId="1412" version="294">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{FA76DEB1-9A8B-4A73-A1DF-F512395FA091}" diskRevisions="1" revisionId="1432" version="304">
   <header guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" dateTime="2018-04-13T11:49:43" maxSheetId="10" userName="itluser" r:id="rId7" minRId="7">
     <sheetIdMap count="9">
       <sheetId val="1"/>
@@ -6307,6 +6343,226 @@
     </sheetIdMap>
   </header>
   <header guid="{65AF415F-CF80-4375-9BD5-D7BFDD3D9813}" dateTime="2018-06-15T12:07:53" maxSheetId="19" userName="ITL-USER" r:id="rId294" minRId="1412">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6714CB33-4610-4BE7-B48E-9576FA571B58}" dateTime="2018-06-15T12:19:53" maxSheetId="19" userName="ITL-USER" r:id="rId295" minRId="1413" maxRId="1414">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{374FCE6B-9C4A-41F5-93A5-75A6999F7089}" dateTime="2018-06-15T12:31:37" maxSheetId="19" userName="ITL-USER" r:id="rId296" minRId="1415" maxRId="1416">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{997C981F-98FA-4980-A113-82AF9F19CDB9}" dateTime="2018-06-15T12:34:52" maxSheetId="19" userName="ITL-USER" r:id="rId297" minRId="1417" maxRId="1418">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{D45A8E0C-6E4C-4FB5-BF85-92F48B7035BC}" dateTime="2018-06-15T12:35:46" maxSheetId="19" userName="ITL-USER" r:id="rId298" minRId="1419" maxRId="1420">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{D5865CE7-D104-4786-AECB-DBEEF36347D3}" dateTime="2018-06-15T12:37:43" maxSheetId="19" userName="ITL-USER" r:id="rId299" minRId="1421" maxRId="1422">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A72401AC-AFC8-4E7D-A9FE-E6FA2927312C}" dateTime="2018-06-15T12:52:23" maxSheetId="19" userName="ITL-USER" r:id="rId300" minRId="1423" maxRId="1424">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{288E56C7-423D-4941-BD04-CD4680AE14BB}" dateTime="2018-06-15T12:54:39" maxSheetId="19" userName="ITL-USER" r:id="rId301" minRId="1425" maxRId="1426">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{F4A3F7E4-F925-4008-994A-AB2B2A891DCF}" dateTime="2018-06-15T12:56:50" maxSheetId="19" userName="ITL-USER" r:id="rId302" minRId="1427" maxRId="1428">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{7EB5D2BC-3FB2-4823-9AF8-9F4C0C6EA710}" dateTime="2018-06-15T12:57:05" maxSheetId="19" userName="ITL-USER" r:id="rId303" minRId="1429" maxRId="1430">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{FA76DEB1-9A8B-4A73-A1DF-F512395FA091}" dateTime="2018-06-15T12:58:38" maxSheetId="19" userName="ITL-USER" r:id="rId304" minRId="1431" maxRId="1432">
     <sheetIdMap count="18">
       <sheetId val="14"/>
       <sheetId val="1"/>
@@ -18675,12 +18931,210 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog289.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1413" sId="18">
+    <nc r="AK1" t="inlineStr">
+      <is>
+        <t>n4GInspPositionOnTruck</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1414" sId="18">
+    <nc r="AK2">
+      <v>1</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog29.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="52" sId="3" xfDxf="1" dxf="1">
     <nc r="AP1" t="inlineStr">
       <is>
         <t>TruckingCoContactState</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog290.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1415" sId="18">
+    <nc r="AL1" t="inlineStr">
+      <is>
+        <t>n4GInspDoorDirection</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1416" sId="18">
+    <nc r="AL2" t="inlineStr">
+      <is>
+        <t>Aft</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog291.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1417" sId="18">
+    <nc r="AM1" t="inlineStr">
+      <is>
+        <t>n4GInspCSC</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1418" sId="18">
+    <nc r="AN1" t="inlineStr">
+      <is>
+        <t>n4GInspMnf</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog292.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1419" sId="18">
+    <nc r="AO1" t="inlineStr">
+      <is>
+        <t>n4GInspSafeWeight</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1420" sId="18">
+    <nc r="AO2">
+      <v>1000</v>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog293.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1421" sId="18">
+    <nc r="AP1" t="inlineStr">
+      <is>
+        <t>n4GInspTareWeight</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1422" sId="18">
+    <nc r="AP2">
+      <v>20000</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog294.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1423" sId="18">
+    <nc r="AQ1" t="inlineStr">
+      <is>
+        <t>n4GInspSeal1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1424" sId="18">
+    <nc r="AQ2" t="inlineStr">
+      <is>
+        <t>S1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog295.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1425" sId="18">
+    <nc r="AR1" t="inlineStr">
+      <is>
+        <t>n4GInspSeal2</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1426" sId="18">
+    <nc r="AR2" t="inlineStr">
+      <is>
+        <t>S2</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog296.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1427" sId="18">
+    <nc r="AS1" t="inlineStr">
+      <is>
+        <t>n4GInspSeal3</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1428" sId="18">
+    <nc r="AS2" t="inlineStr">
+      <is>
+        <t>S3</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog297.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1429" sId="18">
+    <nc r="AT1" t="inlineStr">
+      <is>
+        <t>n4GInspSeal4</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1430" sId="18">
+    <nc r="AT2" t="inlineStr">
+      <is>
+        <t>S4</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog298.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1431" sId="18">
+    <nc r="AU1" t="inlineStr">
+      <is>
+        <t>n4GInspSeal5</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1432" sId="18">
+    <nc r="AU2" t="inlineStr">
+      <is>
+        <t>S5</t>
       </is>
     </nc>
   </rcc>
@@ -20853,7 +21307,7 @@
   <userInfo guid="{EC6B99F2-BAFB-4F81-BF30-4ACACEB126F7}" name="itluser" id="-446781240" dateTime="2018-06-08T17:40:00"/>
   <userInfo guid="{0C6D09E4-075A-4EDD-B3D4-023B29F5DABC}" name="itluser" id="-446797799" dateTime="2018-06-11T15:43:40"/>
   <userInfo guid="{D1C04910-AD23-4127-92A6-F91493935D47}" name="ITL-USER" id="-1580119968" dateTime="2018-06-14T15:05:55"/>
-  <userInfo guid="{65AF415F-CF80-4375-9BD5-D7BFDD3D9813}" name="ITL-USER" id="-1580094246" dateTime="2018-06-15T10:58:52"/>
+  <userInfo guid="{FA76DEB1-9A8B-4A73-A1DF-F512395FA091}" name="ITL-USER" id="-1580094246" dateTime="2018-06-15T10:58:52"/>
 </users>
 </file>
 
@@ -22667,10 +23121,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AU2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AI2" sqref="AI2"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AU2" sqref="AU2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22706,9 +23160,14 @@
     <col min="29" max="34" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="42" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="46" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -22817,8 +23276,41 @@
       <c r="AJ1" t="s">
         <v>502</v>
       </c>
+      <c r="AK1" t="s">
+        <v>503</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>504</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>505</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>506</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>507</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>508</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>509</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>510</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>511</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>512</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>513</v>
+      </c>
     </row>
-    <row r="2" spans="1:36" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>298</v>
       </c>
@@ -22896,12 +23388,39 @@
       </c>
       <c r="AJ2" s="16" t="s">
         <v>461</v>
+      </c>
+      <c r="AK2" s="16">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="16" t="s">
+        <v>362</v>
+      </c>
+      <c r="AO2" s="16">
+        <v>1000</v>
+      </c>
+      <c r="AP2" s="16">
+        <v>20000</v>
+      </c>
+      <c r="AQ2" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="AR2" s="16" t="s">
+        <v>305</v>
+      </c>
+      <c r="AS2" s="16" t="s">
+        <v>307</v>
+      </c>
+      <c r="AT2" s="16" t="s">
+        <v>309</v>
+      </c>
+      <c r="AU2" s="16" t="s">
+        <v>514</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="Z1">
-      <selection activeCell="AJ2" sqref="AJ2"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="AJ1">
+      <selection activeCell="AT2" sqref="AT2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Aswini - Updated TestData and Updated Scriptfile N4MobileGateInspectionCommonRoutines
</commit_message>
<xml_diff>
--- a/Basic Test Suite/TestData/TestData.xlsx
+++ b/Basic Test Suite/TestData/TestData.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="521">
   <si>
     <t>Flow Name</t>
   </si>
@@ -1586,6 +1586,24 @@
   </si>
   <si>
     <t>S5</t>
+  </si>
+  <si>
+    <t>n4GInspChsDamageComponent</t>
+  </si>
+  <si>
+    <t>CORNER</t>
+  </si>
+  <si>
+    <t>n4GInspChsDamageLocation</t>
+  </si>
+  <si>
+    <t>n4GInspChsDamageType</t>
+  </si>
+  <si>
+    <t>n4GInspChsDamageSeverity</t>
+  </si>
+  <si>
+    <t>CHS</t>
   </si>
 </sst>
 </file>
@@ -1663,7 +1681,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{FA76DEB1-9A8B-4A73-A1DF-F512395FA091}" diskRevisions="1" revisionId="1432" version="304">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{BFF01A5A-C4DC-4952-8FF1-D041D354242B}" diskRevisions="1" revisionId="1444" version="311">
   <header guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" dateTime="2018-04-13T11:49:43" maxSheetId="10" userName="itluser" r:id="rId7" minRId="7">
     <sheetIdMap count="9">
       <sheetId val="1"/>
@@ -6563,6 +6581,160 @@
     </sheetIdMap>
   </header>
   <header guid="{FA76DEB1-9A8B-4A73-A1DF-F512395FA091}" dateTime="2018-06-15T12:58:38" maxSheetId="19" userName="ITL-USER" r:id="rId304" minRId="1431" maxRId="1432">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A51B2B8D-8844-464F-9C99-FE735C4DC4C8}" dateTime="2018-06-15T14:36:42" maxSheetId="19" userName="ITL-USER" r:id="rId305" minRId="1433" maxRId="1434">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{594A782C-1E19-47AD-8768-80B30EE86EEA}" dateTime="2018-06-15T14:45:47" maxSheetId="19" userName="ITL-USER" r:id="rId306" minRId="1435" maxRId="1436">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{DF766F13-0399-490D-BB26-38A72CB93AA9}" dateTime="2018-06-15T14:46:03" maxSheetId="19" userName="ITL-USER" r:id="rId307" minRId="1437">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{56B0262C-FF25-4B17-930A-34E0B8166B15}" dateTime="2018-06-15T14:48:19" maxSheetId="19" userName="ITL-USER" r:id="rId308" minRId="1438" maxRId="1439">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{93573324-F57E-4FC4-AB8F-57755B2D1614}" dateTime="2018-06-15T14:59:38" maxSheetId="19" userName="ITL-USER" r:id="rId309" minRId="1440" maxRId="1441">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{ABD0CB41-2248-45BD-BBFC-80C62FFE5A2D}" dateTime="2018-06-15T15:00:11" maxSheetId="19" userName="ITL-USER" r:id="rId310" minRId="1442" maxRId="1443">
+    <sheetIdMap count="18">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{BFF01A5A-C4DC-4952-8FF1-D041D354242B}" dateTime="2018-06-15T15:11:15" maxSheetId="19" userName="ITL-USER" r:id="rId311" minRId="1444">
     <sheetIdMap count="18">
       <sheetId val="14"/>
       <sheetId val="1"/>
@@ -19141,6 +19313,27 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog299.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1433" sId="18">
+    <nc r="AV1" t="inlineStr">
+      <is>
+        <t>n4GInspChsDamageComponent</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1434" sId="18">
+    <nc r="AV2" t="inlineStr">
+      <is>
+        <t>CORNER</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <ris rId="839" sheetId="13" name="[TestData.xlsx]Sheet2" sheetPosition="12"/>
@@ -19311,6 +19504,120 @@
     <nc r="AQ1" t="inlineStr">
       <is>
         <t>TruckingCoContactTelePhone</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog300.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1435" sId="18">
+    <nc r="AW1" t="inlineStr">
+      <is>
+        <t>n4GInspChsDamageLocation</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1436" sId="18">
+    <nc r="AX1" t="inlineStr">
+      <is>
+        <t>n4GInspChsDamageType</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog301.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1437" sId="18" odxf="1" quotePrefix="1">
+    <nc r="AX2" t="inlineStr">
+      <is>
+        <t>----</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog302.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1438" sId="18">
+    <nc r="AY1" t="inlineStr">
+      <is>
+        <t>n4GInspChsDamageSeverity</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1439" sId="18">
+    <nc r="AY2" t="inlineStr">
+      <is>
+        <t>Major</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog303.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1440" sId="18">
+    <nc r="AZ1" t="inlineStr">
+      <is>
+        <t>n4GInspDamageQuantity</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1441" sId="18">
+    <nc r="BA1" t="inlineStr">
+      <is>
+        <t>n4GInspDamageWidth</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog304.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1442" sId="18">
+    <nc r="BB1" t="inlineStr">
+      <is>
+        <t>n4GInspDamageLength</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1443" sId="18">
+    <nc r="BC1" t="inlineStr">
+      <is>
+        <t>n4GInspDamageDepth</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog305.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1444" sId="18" quotePrefix="1">
+    <oc r="AX2" t="inlineStr">
+      <is>
+        <t>----</t>
+      </is>
+    </oc>
+    <nc r="AX2" t="inlineStr">
+      <is>
+        <t>CHS</t>
       </is>
     </nc>
   </rcc>
@@ -21307,7 +21614,7 @@
   <userInfo guid="{EC6B99F2-BAFB-4F81-BF30-4ACACEB126F7}" name="itluser" id="-446781240" dateTime="2018-06-08T17:40:00"/>
   <userInfo guid="{0C6D09E4-075A-4EDD-B3D4-023B29F5DABC}" name="itluser" id="-446797799" dateTime="2018-06-11T15:43:40"/>
   <userInfo guid="{D1C04910-AD23-4127-92A6-F91493935D47}" name="ITL-USER" id="-1580119968" dateTime="2018-06-14T15:05:55"/>
-  <userInfo guid="{FA76DEB1-9A8B-4A73-A1DF-F512395FA091}" name="ITL-USER" id="-1580094246" dateTime="2018-06-15T10:58:52"/>
+  <userInfo guid="{BFF01A5A-C4DC-4952-8FF1-D041D354242B}" name="ITL-USER" id="-1580094246" dateTime="2018-06-15T10:58:52"/>
 </users>
 </file>
 
@@ -23121,10 +23428,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU2"/>
+  <dimension ref="A1:BC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AU2" sqref="AU2"/>
+    <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="AX2" sqref="AX2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23164,10 +23471,17 @@
     <col min="38" max="38" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="41" max="42" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="43" max="46" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="47" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="21" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -23309,8 +23623,32 @@
       <c r="AU1" t="s">
         <v>513</v>
       </c>
+      <c r="AV1" t="s">
+        <v>515</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>517</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>518</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>519</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>474</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>475</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>476</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>477</v>
+      </c>
     </row>
-    <row r="2" spans="1:47" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>298</v>
       </c>
@@ -23415,12 +23753,21 @@
       </c>
       <c r="AU2" s="16" t="s">
         <v>514</v>
+      </c>
+      <c r="AV2" s="16" t="s">
+        <v>516</v>
+      </c>
+      <c r="AX2" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="AY2" s="16" t="s">
+        <v>315</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="AJ1">
-      <selection activeCell="AT2" sqref="AT2"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="AV1">
+      <selection activeCell="BC1" sqref="BC1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Diensh - Updated Test data
</commit_message>
<xml_diff>
--- a/Basic Test Suite/TestData/TestData.xlsx
+++ b/Basic Test Suite/TestData/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ITL-USER\Desktop\TestComplete\Basic Test Suite\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itluser\Desktop\LatestTestComplete\Basic Test Suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="12" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="cdsds" sheetId="14" state="hidden" r:id="rId1"/>
@@ -34,15 +34,15 @@
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="itluser - Personal View" guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1380" windowHeight="744" activeSheetId="17"/>
+    <customWorkbookView name="ITLAdmin - Personal View" guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1362" windowHeight="503" activeSheetId="11"/>
     <customWorkbookView name="ITL-USER - Personal View" guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1380" windowHeight="744" activeSheetId="19"/>
-    <customWorkbookView name="ITLAdmin - Personal View" guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1362" windowHeight="503" activeSheetId="11"/>
-    <customWorkbookView name="itluser - Personal View" guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1380" windowHeight="744" activeSheetId="17"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="586">
   <si>
     <t>Flow Name</t>
   </si>
@@ -1614,6 +1614,192 @@
   </si>
   <si>
     <t>CR1</t>
+  </si>
+  <si>
+    <t>n4OrphanContainer</t>
+  </si>
+  <si>
+    <t>n4OrphanIsocode</t>
+  </si>
+  <si>
+    <t>n4OrphanSlot</t>
+  </si>
+  <si>
+    <t>n4OrphanUnit1</t>
+  </si>
+  <si>
+    <t>n4OrphanUnit2</t>
+  </si>
+  <si>
+    <t>n4Seal</t>
+  </si>
+  <si>
+    <t>n4YardLoc</t>
+  </si>
+  <si>
+    <t>n4Lineoperator</t>
+  </si>
+  <si>
+    <t>n4railFreightKind</t>
+  </si>
+  <si>
+    <t>n4TankRails</t>
+  </si>
+  <si>
+    <t>n4RailDirection</t>
+  </si>
+  <si>
+    <t>n4RailNotes</t>
+  </si>
+  <si>
+    <t>n4DamageComp</t>
+  </si>
+  <si>
+    <t>n4DamageType</t>
+  </si>
+  <si>
+    <t>n4DamageSeverity</t>
+  </si>
+  <si>
+    <t>n4DamageLength</t>
+  </si>
+  <si>
+    <t>n4DamageWidth</t>
+  </si>
+  <si>
+    <t>n4DamageQuatity</t>
+  </si>
+  <si>
+    <t>n4DamageDeep</t>
+  </si>
+  <si>
+    <t>n4DamageLocation</t>
+  </si>
+  <si>
+    <t>n4RailInventoryPowerON</t>
+  </si>
+  <si>
+    <t>n4RailInventoryTemp</t>
+  </si>
+  <si>
+    <t>n4Gensetid</t>
+  </si>
+  <si>
+    <t>n4railtype</t>
+  </si>
+  <si>
+    <t>n4OOGHeigth</t>
+  </si>
+  <si>
+    <t>n4OOGLeft</t>
+  </si>
+  <si>
+    <t>n4OOGRigth</t>
+  </si>
+  <si>
+    <t>n4OOGFlore</t>
+  </si>
+  <si>
+    <t>n4OOGUnits</t>
+  </si>
+  <si>
+    <t>n4RailInventoryPlacard</t>
+  </si>
+  <si>
+    <t>n4Placard1</t>
+  </si>
+  <si>
+    <t>n4Placard2</t>
+  </si>
+  <si>
+    <t>n4Placard3</t>
+  </si>
+  <si>
+    <t>n4Placard4</t>
+  </si>
+  <si>
+    <t>n4Placard5</t>
+  </si>
+  <si>
+    <t>n4Placard6</t>
+  </si>
+  <si>
+    <t>n4RailInventoryGrd</t>
+  </si>
+  <si>
+    <t>n4RailInventorymaterial</t>
+  </si>
+  <si>
+    <t>n4RailInventoryS1</t>
+  </si>
+  <si>
+    <t>n4RailInventoryS2</t>
+  </si>
+  <si>
+    <t>n4RailInventoryS3</t>
+  </si>
+  <si>
+    <t>n4RailInventoryS4</t>
+  </si>
+  <si>
+    <t>n4RailInventoryBundle</t>
+  </si>
+  <si>
+    <t>n4RailInventoryWeight</t>
+  </si>
+  <si>
+    <t>n4RailInventoryunit</t>
+  </si>
+  <si>
+    <t>n4RailInventoryTareWeight</t>
+  </si>
+  <si>
+    <t>n4RailInventorycscDate</t>
+  </si>
+  <si>
+    <t>n4RailInventoryMnf</t>
+  </si>
+  <si>
+    <t>n4RailInventorymrstatus</t>
+  </si>
+  <si>
+    <t>n4RailInventoryGrdFood</t>
+  </si>
+  <si>
+    <t>n4RailInventorymaterialMade</t>
+  </si>
+  <si>
+    <t>DINU17296000</t>
+  </si>
+  <si>
+    <t>DINU1234567</t>
+  </si>
+  <si>
+    <t>DINU1231258</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>FCL</t>
+  </si>
+  <si>
+    <t>Forward</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>S12</t>
+  </si>
+  <si>
+    <t>ID1</t>
+  </si>
+  <si>
+    <t>MnRStatus</t>
   </si>
 </sst>
 </file>
@@ -1691,7 +1877,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{FB08D31F-BDE4-4C92-82F7-5EF44FACB22F}" diskRevisions="1" revisionId="1451" version="314">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{DC5973E4-7BB7-4FF1-B826-D3886C9F80C9}" diskRevisions="1" revisionId="1547" version="315">
   <header guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" dateTime="2018-04-13T11:49:43" maxSheetId="10" userName="itluser" r:id="rId7" minRId="7">
     <sheetIdMap count="9">
       <sheetId val="1"/>
@@ -6813,6 +6999,29 @@
     </sheetIdMap>
   </header>
   <header guid="{FB08D31F-BDE4-4C92-82F7-5EF44FACB22F}" dateTime="2018-06-15T15:45:53" maxSheetId="20" userName="ITL-USER" r:id="rId314" minRId="1450" maxRId="1451">
+    <sheetIdMap count="19">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{DC5973E4-7BB7-4FF1-B826-D3886C9F80C9}" dateTime="2018-06-19T12:13:56" maxSheetId="20" userName="itluser" r:id="rId315" minRId="1452" maxRId="1547">
     <sheetIdMap count="19">
       <sheetId val="14"/>
       <sheetId val="1"/>
@@ -19769,6 +19978,753 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog309.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1452" sId="17" odxf="1">
+    <nc r="M1" t="inlineStr">
+      <is>
+        <t>n4OrphanContainer</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1453" sId="17" odxf="1">
+    <nc r="N1" t="inlineStr">
+      <is>
+        <t>n4OrphanIsocode</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1454" sId="17" odxf="1">
+    <nc r="O1" t="inlineStr">
+      <is>
+        <t>n4OrphanSlot</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1455" sId="17" odxf="1">
+    <nc r="P1" t="inlineStr">
+      <is>
+        <t>n4OrphanUnit1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1456" sId="17" odxf="1">
+    <nc r="Q1" t="inlineStr">
+      <is>
+        <t>n4OrphanUnit2</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1457" sId="17" odxf="1">
+    <nc r="R1" t="inlineStr">
+      <is>
+        <t>n4Seal</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1458" sId="17" odxf="1">
+    <nc r="S1" t="inlineStr">
+      <is>
+        <t>n4YardLoc</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1459" sId="17" odxf="1">
+    <nc r="T1" t="inlineStr">
+      <is>
+        <t>n4Lineoperator</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1460" sId="17" odxf="1">
+    <nc r="U1" t="inlineStr">
+      <is>
+        <t>n4railFreightKind</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1461" sId="17" odxf="1">
+    <nc r="V1" t="inlineStr">
+      <is>
+        <t>n4TankRails</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1462" sId="17" odxf="1">
+    <nc r="W1" t="inlineStr">
+      <is>
+        <t>n4RailDirection</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1463" sId="17" odxf="1">
+    <nc r="X1" t="inlineStr">
+      <is>
+        <t>n4RailNotes</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1464" sId="17" odxf="1">
+    <nc r="Y1" t="inlineStr">
+      <is>
+        <t>n4DamageComp</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1465" sId="17" odxf="1">
+    <nc r="Z1" t="inlineStr">
+      <is>
+        <t>n4DamageType</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1466" sId="17" odxf="1">
+    <nc r="AA1" t="inlineStr">
+      <is>
+        <t>n4DamageSeverity</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1467" sId="17" odxf="1">
+    <nc r="AB1" t="inlineStr">
+      <is>
+        <t>n4DamageLength</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1468" sId="17" odxf="1">
+    <nc r="AC1" t="inlineStr">
+      <is>
+        <t>n4DamageWidth</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1469" sId="17" odxf="1">
+    <nc r="AD1" t="inlineStr">
+      <is>
+        <t>n4DamageQuatity</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1470" sId="17" odxf="1">
+    <nc r="AE1" t="inlineStr">
+      <is>
+        <t>n4DamageDeep</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1471" sId="17" odxf="1">
+    <nc r="AF1" t="inlineStr">
+      <is>
+        <t>n4DamageLocation</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1472" sId="17" odxf="1">
+    <nc r="AG1" t="inlineStr">
+      <is>
+        <t>n4RailInventoryPowerON</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1473" sId="17" odxf="1">
+    <nc r="AH1" t="inlineStr">
+      <is>
+        <t>n4RailInventoryTemp</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1474" sId="17" odxf="1">
+    <nc r="AI1" t="inlineStr">
+      <is>
+        <t>n4Gensetid</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1475" sId="17" odxf="1">
+    <nc r="AJ1" t="inlineStr">
+      <is>
+        <t>n4railtype</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1476" sId="17" odxf="1">
+    <nc r="AK1" t="inlineStr">
+      <is>
+        <t>n4OOGHeigth</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1477" sId="17" odxf="1">
+    <nc r="AL1" t="inlineStr">
+      <is>
+        <t>n4OOGLeft</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1478" sId="17" odxf="1">
+    <nc r="AM1" t="inlineStr">
+      <is>
+        <t>n4OOGRigth</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1479" sId="17" odxf="1">
+    <nc r="AN1" t="inlineStr">
+      <is>
+        <t>n4OOGFlore</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1480" sId="17" odxf="1">
+    <nc r="AO1" t="inlineStr">
+      <is>
+        <t>n4OOGUnits</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1481" sId="17" odxf="1">
+    <nc r="AP1" t="inlineStr">
+      <is>
+        <t>n4RailInventoryPlacard</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1482" sId="17" odxf="1">
+    <nc r="AQ1" t="inlineStr">
+      <is>
+        <t>n4Placard1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1483" sId="17" odxf="1">
+    <nc r="AR1" t="inlineStr">
+      <is>
+        <t>n4Placard2</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1484" sId="17" odxf="1">
+    <nc r="AS1" t="inlineStr">
+      <is>
+        <t>n4Placard3</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1485" sId="17" odxf="1">
+    <nc r="AT1" t="inlineStr">
+      <is>
+        <t>n4Placard4</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1486" sId="17" odxf="1">
+    <nc r="AU1" t="inlineStr">
+      <is>
+        <t>n4Placard5</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1487" sId="17" odxf="1">
+    <nc r="AV1" t="inlineStr">
+      <is>
+        <t>n4Placard6</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1488" sId="17" odxf="1">
+    <nc r="AW1" t="inlineStr">
+      <is>
+        <t>n4RailInventoryGrd</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1489" sId="17" odxf="1">
+    <nc r="AX1" t="inlineStr">
+      <is>
+        <t>n4RailInventorymaterial</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1490" sId="17" odxf="1">
+    <nc r="AY1" t="inlineStr">
+      <is>
+        <t>n4RailInventoryS1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1491" sId="17" odxf="1">
+    <nc r="AZ1" t="inlineStr">
+      <is>
+        <t>n4RailInventoryS2</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1492" sId="17" odxf="1">
+    <nc r="BA1" t="inlineStr">
+      <is>
+        <t>n4RailInventoryS3</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1493" sId="17" odxf="1">
+    <nc r="BB1" t="inlineStr">
+      <is>
+        <t>n4RailInventoryS4</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1494" sId="17" odxf="1">
+    <nc r="BC1" t="inlineStr">
+      <is>
+        <t>n4RailInventoryBundle</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1495" sId="17" odxf="1">
+    <nc r="BD1" t="inlineStr">
+      <is>
+        <t>n4RailInventoryWeight</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1496" sId="17" odxf="1">
+    <nc r="BE1" t="inlineStr">
+      <is>
+        <t>n4RailInventoryunit</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1497" sId="17" odxf="1">
+    <nc r="BF1" t="inlineStr">
+      <is>
+        <t>n4RailInventoryTareWeight</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1498" sId="17" odxf="1">
+    <nc r="BG1" t="inlineStr">
+      <is>
+        <t>n4RailInventorycscDate</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1499" sId="17" odxf="1">
+    <nc r="BH1" t="inlineStr">
+      <is>
+        <t>n4RailInventoryMnf</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1500" sId="17" odxf="1">
+    <nc r="BI1" t="inlineStr">
+      <is>
+        <t>n4RailInventorymrstatus</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1501" sId="17" odxf="1">
+    <nc r="BJ1" t="inlineStr">
+      <is>
+        <t>n4RailInventoryGrdFood</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1502" sId="17" odxf="1">
+    <nc r="BK1" t="inlineStr">
+      <is>
+        <t>n4RailInventorymaterialMade</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1503" sId="17" odxf="1">
+    <nc r="BL1" t="inlineStr">
+      <is>
+        <t xml:space="preserve"> </t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1504" sId="17" odxf="1">
+    <nc r="M2" t="inlineStr">
+      <is>
+        <t>DINU17296000</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1505" sId="17" odxf="1">
+    <nc r="N2">
+      <v>2200</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1506" sId="17" odxf="1">
+    <nc r="O2">
+      <v>2</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1507" sId="17" odxf="1">
+    <nc r="P2" t="inlineStr">
+      <is>
+        <t>DINU1234567</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1508" sId="17" odxf="1">
+    <nc r="Q2" t="inlineStr">
+      <is>
+        <t>DINU1231258</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1509" sId="17" odxf="1">
+    <nc r="R2" t="inlineStr">
+      <is>
+        <t>s1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1510" sId="17" odxf="1">
+    <nc r="S2" t="inlineStr">
+      <is>
+        <t>1A</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1511" sId="17" odxf="1">
+    <nc r="T2" t="inlineStr">
+      <is>
+        <t>ASW</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1512" sId="17" odxf="1">
+    <nc r="U2" t="inlineStr">
+      <is>
+        <t>FCL</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1513" sId="17" odxf="1">
+    <nc r="V2" t="inlineStr">
+      <is>
+        <t>Top</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1514" sId="17" odxf="1">
+    <nc r="W2" t="inlineStr">
+      <is>
+        <t>Forward</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1515" sId="17" odxf="1">
+    <nc r="Y2" t="inlineStr">
+      <is>
+        <t>DOOR</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1516" sId="17" odxf="1">
+    <nc r="Z2" t="inlineStr">
+      <is>
+        <t>DAT</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1517" sId="17" odxf="1">
+    <nc r="AA2" t="inlineStr">
+      <is>
+        <t>Major</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1518" sId="17" odxf="1">
+    <nc r="AB2">
+      <v>44</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1519" sId="17" odxf="1">
+    <nc r="AC2">
+      <v>11</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1520" sId="17" odxf="1">
+    <nc r="AD2">
+      <v>2</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1521" sId="17" odxf="1">
+    <nc r="AE2">
+      <v>15</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1522" sId="17" odxf="1">
+    <nc r="AG2" t="inlineStr">
+      <is>
+        <t>NO</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1523" sId="17" odxf="1">
+    <nc r="AH2" t="inlineStr">
+      <is>
+        <t>F</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1524" sId="17" odxf="1">
+    <nc r="AJ2">
+      <v>9000</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1525" sId="17" odxf="1">
+    <nc r="AK2">
+      <v>11</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1526" sId="17" odxf="1">
+    <nc r="AL2">
+      <v>5</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1527" sId="17" odxf="1">
+    <nc r="AM2">
+      <v>10</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1528" sId="17" odxf="1">
+    <nc r="AP2" t="inlineStr">
+      <is>
+        <t>Yes</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1529" sId="17" odxf="1">
+    <nc r="AQ2" t="inlineStr">
+      <is>
+        <t>CLASS 1.4</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1530" sId="17" odxf="1">
+    <nc r="AR2" t="inlineStr">
+      <is>
+        <t>CLASS 1.4</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1531" sId="17" odxf="1">
+    <nc r="AS2" t="inlineStr">
+      <is>
+        <t>CLASS 1.4</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1532" sId="17" odxf="1">
+    <nc r="AT2" t="inlineStr">
+      <is>
+        <t>CLASS 1.4</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1533" sId="17" odxf="1">
+    <nc r="AU2" t="inlineStr">
+      <is>
+        <t>CLASS 1.4</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1534" sId="17" odxf="1">
+    <nc r="AV2" t="inlineStr">
+      <is>
+        <t>CLASS 1.4</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1535" sId="17" odxf="1">
+    <nc r="AW2" t="inlineStr">
+      <is>
+        <t>FOOD</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1536" sId="17" odxf="1">
+    <nc r="AX2" t="inlineStr">
+      <is>
+        <t>Steel</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1537" sId="17" odxf="1">
+    <nc r="AY2" t="inlineStr">
+      <is>
+        <t>S12</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1538" sId="17" odxf="1">
+    <nc r="AZ2" t="inlineStr">
+      <is>
+        <t>S2</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1539" sId="17" odxf="1">
+    <nc r="BA2" t="inlineStr">
+      <is>
+        <t>S3</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1540" sId="17" odxf="1">
+    <nc r="BB2" t="inlineStr">
+      <is>
+        <t>S4</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1541" sId="17" odxf="1">
+    <nc r="BC2" t="inlineStr">
+      <is>
+        <t>ID1</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1542" sId="17" odxf="1">
+    <nc r="BD2">
+      <v>100</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1543" sId="17" odxf="1">
+    <nc r="BF2">
+      <v>2200</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1544" sId="17" odxf="1">
+    <nc r="BG2">
+      <v>12566</v>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1545" sId="17" odxf="1">
+    <nc r="BI2" t="inlineStr">
+      <is>
+        <t>MnRStatus</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1546" sId="17" odxf="1">
+    <nc r="BJ2" t="inlineStr">
+      <is>
+        <t>FOOD</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1547" sId="17" odxf="1">
+    <nc r="BK2" t="inlineStr">
+      <is>
+        <t>Steel</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog31.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="54" sId="3" xfDxf="1" dxf="1">
@@ -21744,7 +22700,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="14">
   <userInfo guid="{0FC3EEC7-1253-40C9-80FE-72015618EED8}" name="ITLAdmin" id="-2068730528" dateTime="2018-04-13T11:51:21"/>
   <userInfo guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" name="itluser" id="-446795219" dateTime="2018-04-13T11:51:26"/>
@@ -22041,11 +22997,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" state="hidden">
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" state="hidden">
       <selection activeCell="H18" sqref="H18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" state="hidden">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" state="hidden">
       <selection activeCell="H18" sqref="H18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -22059,7 +23015,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22149,16 +23105,16 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="B1" sqref="B1"/>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -22171,7 +23127,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22514,16 +23470,16 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="H2" sqref="H2"/>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="E11" sqref="E11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="H2" sqref="H2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -22536,7 +23492,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22584,16 +23540,16 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="E2" sqref="E2"/>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="E2" sqref="E2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -22605,7 +23561,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -23466,11 +24424,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="AG1">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="AG1">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -23480,90 +24438,382 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:BL2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="19.140625" customWidth="1"/>
+    <col min="1" max="1" width="22" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="9.140625" style="16"/>
+    <col min="11" max="11" width="17" style="16" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" style="16" customWidth="1"/>
+    <col min="13" max="15" width="9.140625" style="16"/>
+    <col min="16" max="17" width="9.5703125" style="16" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="16" t="s">
         <v>435</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="16" t="s">
         <v>436</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="16" t="s">
         <v>437</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="16" t="s">
         <v>438</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="16" t="s">
         <v>439</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="16" t="s">
         <v>443</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="16" t="s">
         <v>444</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="16" t="s">
         <v>445</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="16" t="s">
         <v>446</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="16" t="s">
         <v>449</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="16" t="s">
         <v>450</v>
       </c>
+      <c r="M1" s="16" t="s">
+        <v>524</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>525</v>
+      </c>
+      <c r="O1" s="16" t="s">
+        <v>526</v>
+      </c>
+      <c r="P1" s="16" t="s">
+        <v>527</v>
+      </c>
+      <c r="Q1" s="16" t="s">
+        <v>528</v>
+      </c>
+      <c r="R1" s="16" t="s">
+        <v>529</v>
+      </c>
+      <c r="S1" s="16" t="s">
+        <v>530</v>
+      </c>
+      <c r="T1" s="16" t="s">
+        <v>531</v>
+      </c>
+      <c r="U1" s="16" t="s">
+        <v>532</v>
+      </c>
+      <c r="V1" s="16" t="s">
+        <v>533</v>
+      </c>
+      <c r="W1" s="16" t="s">
+        <v>534</v>
+      </c>
+      <c r="X1" s="16" t="s">
+        <v>535</v>
+      </c>
+      <c r="Y1" s="16" t="s">
+        <v>536</v>
+      </c>
+      <c r="Z1" s="16" t="s">
+        <v>537</v>
+      </c>
+      <c r="AA1" s="16" t="s">
+        <v>538</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>539</v>
+      </c>
+      <c r="AC1" s="16" t="s">
+        <v>540</v>
+      </c>
+      <c r="AD1" s="16" t="s">
+        <v>541</v>
+      </c>
+      <c r="AE1" s="16" t="s">
+        <v>542</v>
+      </c>
+      <c r="AF1" s="16" t="s">
+        <v>543</v>
+      </c>
+      <c r="AG1" s="16" t="s">
+        <v>544</v>
+      </c>
+      <c r="AH1" s="16" t="s">
+        <v>545</v>
+      </c>
+      <c r="AI1" s="16" t="s">
+        <v>546</v>
+      </c>
+      <c r="AJ1" s="16" t="s">
+        <v>547</v>
+      </c>
+      <c r="AK1" s="16" t="s">
+        <v>548</v>
+      </c>
+      <c r="AL1" s="16" t="s">
+        <v>549</v>
+      </c>
+      <c r="AM1" s="16" t="s">
+        <v>550</v>
+      </c>
+      <c r="AN1" s="16" t="s">
+        <v>551</v>
+      </c>
+      <c r="AO1" s="16" t="s">
+        <v>552</v>
+      </c>
+      <c r="AP1" s="16" t="s">
+        <v>553</v>
+      </c>
+      <c r="AQ1" s="16" t="s">
+        <v>554</v>
+      </c>
+      <c r="AR1" s="16" t="s">
+        <v>555</v>
+      </c>
+      <c r="AS1" s="16" t="s">
+        <v>556</v>
+      </c>
+      <c r="AT1" s="16" t="s">
+        <v>557</v>
+      </c>
+      <c r="AU1" s="16" t="s">
+        <v>558</v>
+      </c>
+      <c r="AV1" s="16" t="s">
+        <v>559</v>
+      </c>
+      <c r="AW1" s="16" t="s">
+        <v>560</v>
+      </c>
+      <c r="AX1" s="16" t="s">
+        <v>561</v>
+      </c>
+      <c r="AY1" s="16" t="s">
+        <v>562</v>
+      </c>
+      <c r="AZ1" s="16" t="s">
+        <v>563</v>
+      </c>
+      <c r="BA1" s="16" t="s">
+        <v>564</v>
+      </c>
+      <c r="BB1" s="16" t="s">
+        <v>565</v>
+      </c>
+      <c r="BC1" s="16" t="s">
+        <v>566</v>
+      </c>
+      <c r="BD1" s="16" t="s">
+        <v>567</v>
+      </c>
+      <c r="BE1" s="16" t="s">
+        <v>568</v>
+      </c>
+      <c r="BF1" s="16" t="s">
+        <v>569</v>
+      </c>
+      <c r="BG1" s="16" t="s">
+        <v>570</v>
+      </c>
+      <c r="BH1" s="16" t="s">
+        <v>571</v>
+      </c>
+      <c r="BI1" s="16" t="s">
+        <v>572</v>
+      </c>
+      <c r="BJ1" s="16" t="s">
+        <v>573</v>
+      </c>
+      <c r="BK1" s="16" t="s">
+        <v>574</v>
+      </c>
+      <c r="BL1" s="16" t="s">
+        <v>246</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>440</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="16" t="s">
         <v>441</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="16" t="s">
         <v>442</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="16" t="s">
         <v>360</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="16" t="s">
         <v>360</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="16" t="s">
         <v>360</v>
+      </c>
+      <c r="M2" s="16" t="s">
+        <v>575</v>
+      </c>
+      <c r="N2" s="16">
+        <v>2200</v>
+      </c>
+      <c r="O2" s="16">
+        <v>2</v>
+      </c>
+      <c r="P2" s="16" t="s">
+        <v>576</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>577</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>578</v>
+      </c>
+      <c r="T2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="U2" s="16" t="s">
+        <v>579</v>
+      </c>
+      <c r="V2" s="16" t="s">
+        <v>364</v>
+      </c>
+      <c r="W2" s="16" t="s">
+        <v>580</v>
+      </c>
+      <c r="Y2" s="16" t="s">
+        <v>313</v>
+      </c>
+      <c r="Z2" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="AA2" s="16" t="s">
+        <v>315</v>
+      </c>
+      <c r="AB2" s="16">
+        <v>44</v>
+      </c>
+      <c r="AC2" s="16">
+        <v>11</v>
+      </c>
+      <c r="AD2" s="16">
+        <v>2</v>
+      </c>
+      <c r="AE2" s="16">
+        <v>15</v>
+      </c>
+      <c r="AG2" s="16" t="s">
+        <v>581</v>
+      </c>
+      <c r="AH2" s="16" t="s">
+        <v>582</v>
+      </c>
+      <c r="AJ2" s="16">
+        <v>9000</v>
+      </c>
+      <c r="AK2" s="16">
+        <v>11</v>
+      </c>
+      <c r="AL2" s="16">
+        <v>5</v>
+      </c>
+      <c r="AM2" s="16">
+        <v>10</v>
+      </c>
+      <c r="AP2" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="AQ2" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="AR2" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="AS2" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="AT2" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="AU2" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="AV2" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="AW2" s="16" t="s">
+        <v>334</v>
+      </c>
+      <c r="AX2" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="AY2" s="16" t="s">
+        <v>583</v>
+      </c>
+      <c r="AZ2" s="16" t="s">
+        <v>305</v>
+      </c>
+      <c r="BA2" s="16" t="s">
+        <v>307</v>
+      </c>
+      <c r="BB2" s="16" t="s">
+        <v>309</v>
+      </c>
+      <c r="BC2" s="16" t="s">
+        <v>584</v>
+      </c>
+      <c r="BD2" s="16">
+        <v>100</v>
+      </c>
+      <c r="BF2" s="16">
+        <v>2200</v>
+      </c>
+      <c r="BG2" s="2">
+        <v>12566</v>
+      </c>
+      <c r="BI2" s="16" t="s">
+        <v>585</v>
+      </c>
+      <c r="BJ2" s="16" t="s">
+        <v>334</v>
+      </c>
+      <c r="BK2" s="16" t="s">
+        <v>396</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="B1">
+      <selection activeCell="K1" sqref="K1"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="B1">
       <selection activeCell="F13" sqref="F13"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="B1">
-      <selection activeCell="K1" sqref="K1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -23924,7 +25174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -23972,8 +25222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24078,12 +25328,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="B2" sqref="B2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="M1">
       <selection activeCell="Q1" sqref="Q1"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="B2" sqref="B2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -24096,98 +25346,93 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>400</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>401</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="16" t="s">
         <v>402</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="16" t="s">
         <v>404</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="16" t="s">
         <v>405</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="16" t="s">
         <v>406</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="16" t="s">
         <v>407</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="16" t="s">
         <v>408</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="16" t="s">
         <v>409</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="16" t="s">
         <v>410</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="16" t="s">
         <v>411</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="N1" s="16" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>413</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>414</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="16">
         <v>22</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="16">
         <v>15</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="16" t="s">
         <v>415</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="16" t="s">
         <v>416</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="16">
         <v>0.255</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15">
+      <c r="N2" s="16">
         <v>75</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="A2" sqref="A2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="N9" sqref="N9"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="A2" sqref="A2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -24199,8 +25444,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI3"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" workbookViewId="0">
-      <selection activeCell="AI2" sqref="AI2:AI3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24521,12 +25766,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="D1">
+      <selection activeCell="G15" sqref="G15"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="Z1">
       <selection activeCell="AI2" sqref="AI2:AI3"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="D1">
-      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -24538,8 +25783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24868,8 +26113,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="G9" sqref="G9"/>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="A19" sqref="A19"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -24878,8 +26123,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="A19" sqref="A19"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="G9" sqref="G9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -24894,7 +26139,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24952,16 +26197,16 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="K12" sqref="K12"/>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="K12" sqref="K12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="K12" sqref="K12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -24973,8 +26218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25113,16 +26358,16 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="O1">
-      <selection activeCell="Y1" sqref="Y1"/>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="O1">
       <selection activeCell="Y1" sqref="Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="O1">
+      <selection activeCell="Y1" sqref="Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -25134,8 +26379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE2"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25471,8 +26716,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="V1">
-      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="J1">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -25481,8 +26726,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="J1">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="V1">
+      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>
@@ -25497,7 +26742,7 @@
   <dimension ref="A1:AT25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25969,16 +27214,16 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="A3" sqref="A3:XFD3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -25991,7 +27236,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Y1"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26153,16 +27398,16 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="Q1" sqref="Q1:Y1"/>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
       <selection activeCell="Q1" sqref="Q1:Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="Q1" sqref="Q1:Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -26174,8 +27419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AI2" sqref="AI2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26400,23 +27645,22 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="W1">
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="W1">
       <selection activeCell="AI2" sqref="AI2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="W1">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="W1">
       <selection activeCell="AI2" sqref="AI2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="G15" sqref="G15"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -26425,7 +27669,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26493,8 +27737,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="G1" sqref="G1"/>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
@@ -26503,8 +27747,8 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="G1" sqref="G1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
     </customSheetView>

</xml_diff>

<commit_message>
Aswini - Updated Script files
</commit_message>
<xml_diff>
--- a/Basic Test Suite/TestData/TestData.xlsx
+++ b/Basic Test Suite/TestData/TestData.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="592">
   <si>
     <t>Flow Name</t>
   </si>
@@ -1799,9 +1799,6 @@
     <t>n4DepotOrphanContainerID</t>
   </si>
   <si>
-    <t>ASWU2705130</t>
-  </si>
-  <si>
     <t>n4DepotOrphanContainerLocation</t>
   </si>
   <si>
@@ -1809,6 +1806,18 @@
   </si>
   <si>
     <t>n4DepotHatchClerkOrphanIsoType</t>
+  </si>
+  <si>
+    <t>n4DepotHatchClerkOrphanChassisID</t>
+  </si>
+  <si>
+    <t>n4DepotHatchClerkOrphanChassisSlot</t>
+  </si>
+  <si>
+    <t>n4DepotHatchClerkOrphanContainerDoorDirection</t>
+  </si>
+  <si>
+    <t>ASWU2705120</t>
   </si>
 </sst>
 </file>
@@ -1886,7 +1895,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{23352E82-398F-48E2-AE1D-EBED7D9EDEB5}" diskRevisions="1" revisionId="1555" version="320">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{BDFEF748-9026-4534-A65E-11F22F124BF4}" diskRevisions="1" revisionId="1559" version="322">
   <header guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" dateTime="2018-04-13T11:49:43" maxSheetId="10" userName="itluser" r:id="rId7" minRId="7">
     <sheetIdMap count="9">
       <sheetId val="1"/>
@@ -7146,6 +7155,52 @@
     </sheetIdMap>
   </header>
   <header guid="{23352E82-398F-48E2-AE1D-EBED7D9EDEB5}" dateTime="2018-06-22T14:58:59" maxSheetId="20" userName="ITL-USER" r:id="rId320" minRId="1554" maxRId="1555">
+    <sheetIdMap count="19">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5889B6B4-5C44-49B2-8152-C6F2D660D38D}" dateTime="2018-06-22T15:01:44" maxSheetId="20" userName="ITL-USER" r:id="rId321" minRId="1556">
+    <sheetIdMap count="19">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{BDFEF748-9026-4534-A65E-11F22F124BF4}" dateTime="2018-06-22T15:48:21" maxSheetId="20" userName="ITL-USER" r:id="rId322" minRId="1557" maxRId="1559">
     <sheetIdMap count="19">
       <sheetId val="14"/>
       <sheetId val="1"/>
@@ -21006,6 +21061,51 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog315.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1556" sId="19">
+    <nc r="G1" t="inlineStr">
+      <is>
+        <t>n4DepotHatchClerkOrphanChassisID</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog316.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1557" sId="19">
+    <nc r="H1" t="inlineStr">
+      <is>
+        <t>n4DepotHatchClerkOrphanChassisSlot</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1558" sId="19">
+    <nc r="I1" t="inlineStr">
+      <is>
+        <t>n4DepotHatchClerkOrphanContainerDoorDirection</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1559" sId="19">
+    <oc r="D2" t="inlineStr">
+      <is>
+        <t>ASWU2705130</t>
+      </is>
+    </oc>
+    <nc r="D2" t="inlineStr">
+      <is>
+        <t>ASWU2705120</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog32.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="55" sId="3" xfDxf="1" dxf="1">
@@ -22983,7 +23083,7 @@
   <userInfo guid="{0C6D09E4-075A-4EDD-B3D4-023B29F5DABC}" name="itluser" id="-446797799" dateTime="2018-06-11T15:43:40"/>
   <userInfo guid="{D1C04910-AD23-4127-92A6-F91493935D47}" name="ITL-USER" id="-1580119968" dateTime="2018-06-14T15:05:55"/>
   <userInfo guid="{FB08D31F-BDE4-4C92-82F7-5EF44FACB22F}" name="ITL-USER" id="-1580094246" dateTime="2018-06-15T10:58:52"/>
-  <userInfo guid="{23352E82-398F-48E2-AE1D-EBED7D9EDEB5}" name="ITL-USER" id="-1580112220" dateTime="2018-06-22T14:52:22"/>
+  <userInfo guid="{BDFEF748-9026-4534-A65E-11F22F124BF4}" name="ITL-USER" id="-1580112220" dateTime="2018-06-22T14:52:22"/>
 </users>
 </file>
 
@@ -25415,10 +25515,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25429,9 +25529,12 @@
     <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -25445,13 +25548,22 @@
         <v>584</v>
       </c>
       <c r="E1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F1" t="s">
+        <v>587</v>
+      </c>
+      <c r="G1" t="s">
         <v>588</v>
       </c>
+      <c r="H1" t="s">
+        <v>589</v>
+      </c>
+      <c r="I1" t="s">
+        <v>590</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>298</v>
       </c>
@@ -25462,10 +25574,10 @@
         <v>521</v>
       </c>
       <c r="D2" t="s">
-        <v>585</v>
+        <v>591</v>
       </c>
       <c r="E2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F2">
         <v>2200</v>
@@ -25474,7 +25586,7 @@
   </sheetData>
   <customSheetViews>
     <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>

<commit_message>
Aswini - Updated Test DAta
</commit_message>
<xml_diff>
--- a/Basic Test Suite/TestData/TestData.xlsx
+++ b/Basic Test Suite/TestData/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itluser\Desktop\TestComplete22618\Basic Test Suite\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ITL-USER\Desktop\TestComplete\Basic Test Suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="10" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="8" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="cdsds" sheetId="14" state="hidden" r:id="rId1"/>
@@ -37,15 +37,15 @@
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="ITL-USER - Personal View" guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1380" windowHeight="744" activeSheetId="8"/>
     <customWorkbookView name="itluser - Personal View" guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1380" windowHeight="744" activeSheetId="21"/>
-    <customWorkbookView name="ITL-USER - Personal View" guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1380" windowHeight="744" activeSheetId="19"/>
     <customWorkbookView name="ITLAdmin - Personal View" guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1362" windowHeight="503" activeSheetId="11"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1093" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="634">
   <si>
     <t>Flow Name</t>
   </si>
@@ -1899,6 +1899,54 @@
   </si>
   <si>
     <t>DINU7540155</t>
+  </si>
+  <si>
+    <t>YINV_YINS_101</t>
+  </si>
+  <si>
+    <t>Unit1inSNX</t>
+  </si>
+  <si>
+    <t>ASWU2705190~ASW~F10L.1</t>
+  </si>
+  <si>
+    <t>SnxName</t>
+  </si>
+  <si>
+    <t>ReceiveEmptyUnit2200.xml</t>
+  </si>
+  <si>
+    <t>Unit2inSNX</t>
+  </si>
+  <si>
+    <t>ASWU2705180~ASW~F10K.1</t>
+  </si>
+  <si>
+    <t>Unit3inSNX</t>
+  </si>
+  <si>
+    <t>ASWU2705170~ASW~F10K.2</t>
+  </si>
+  <si>
+    <t>PAYLOAD</t>
+  </si>
+  <si>
+    <t>n4YInspBUndleContainer2</t>
+  </si>
+  <si>
+    <t>ASWU2705170</t>
+  </si>
+  <si>
+    <t>UnitAttached</t>
+  </si>
+  <si>
+    <t>DeleteUnit1</t>
+  </si>
+  <si>
+    <t>DeleteUnit2</t>
+  </si>
+  <si>
+    <t>DeleteUnit3</t>
   </si>
 </sst>
 </file>
@@ -1976,7 +2024,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C12268D6-D807-4CC2-B4A7-ADCD12DC4640}" diskRevisions="1" revisionId="1660" version="362">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{AE37B969-B9E8-407D-AD25-C9352A863F89}" diskRevisions="1" revisionId="1707" version="376">
   <header guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" dateTime="2018-04-13T11:49:43" maxSheetId="10" userName="itluser" r:id="rId7" minRId="7">
     <sheetIdMap count="9">
       <sheetId val="1"/>
@@ -8290,6 +8338,370 @@
     </sheetIdMap>
   </header>
   <header guid="{C12268D6-D807-4CC2-B4A7-ADCD12DC4640}" dateTime="2018-06-29T15:21:34" maxSheetId="23" userName="itluser" r:id="rId362" minRId="1660">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{8C773B0B-2FA1-4FF3-B766-871A088BE6A1}" dateTime="2018-07-03T13:16:49" maxSheetId="23" userName="ITL-USER" r:id="rId363" minRId="1661" maxRId="1668">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{03C81741-09E9-4104-8D87-4B63BF18F63F}" dateTime="2018-07-03T15:33:16" maxSheetId="23" userName="ITL-USER" r:id="rId364" minRId="1669" maxRId="1670">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{E476DA43-89B5-497A-87C3-CDE73A14E497}" dateTime="2018-07-03T15:37:19" maxSheetId="23" userName="ITL-USER" r:id="rId365" minRId="1671" maxRId="1673">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{17114929-C696-43E2-8D1C-0B2E5B92D89D}" dateTime="2018-07-03T15:41:31" maxSheetId="23" userName="ITL-USER" r:id="rId366" minRId="1674" maxRId="1676">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{96BAD32F-AAA0-47CC-817B-80ABDFCB0BF8}" dateTime="2018-07-03T15:42:47" maxSheetId="23" userName="ITL-USER" r:id="rId367" minRId="1677" maxRId="1679">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{CAFFA1CA-FD55-4D72-8882-154FAF1BB1FD}" dateTime="2018-07-03T17:35:35" maxSheetId="23" userName="ITL-USER" r:id="rId368" minRId="1680" maxRId="1684">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{24B93DDD-E49D-4A28-B9AD-67CF1ADC528A}" dateTime="2018-07-03T17:37:27" maxSheetId="23" userName="ITL-USER" r:id="rId369" minRId="1685" maxRId="1693">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B829F8E7-75C1-45DA-852A-72039F31E3E0}" dateTime="2018-07-03T17:40:40" maxSheetId="23" userName="ITL-USER" r:id="rId370" minRId="1694" maxRId="1695">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{31C8ECCA-5E2E-48AC-85B2-C27C925378A2}" dateTime="2018-07-03T17:40:52" maxSheetId="23" userName="ITL-USER" r:id="rId371" minRId="1696">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{AEAD8A2C-9188-465C-A168-BD372590D8B3}" dateTime="2018-07-04T10:59:48" maxSheetId="23" userName="ITL-USER" r:id="rId372" minRId="1697">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{ADC7E201-593B-423F-A49F-C1FEC8F55E72}" dateTime="2018-07-04T11:38:29" maxSheetId="23" userName="ITL-USER" r:id="rId373" minRId="1698" maxRId="1699">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{34714CFD-7AAB-4A67-87E4-3D0FBCDC21E4}" dateTime="2018-07-04T11:41:54" maxSheetId="23" userName="ITL-USER" r:id="rId374" minRId="1700" maxRId="1701">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{AC957541-00B1-47D1-9200-4DED38A46BA4}" dateTime="2018-07-04T11:46:25" maxSheetId="23" userName="ITL-USER" r:id="rId375" minRId="1702" maxRId="1705">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{AE37B969-B9E8-407D-AD25-C9352A863F89}" dateTime="2018-07-04T11:47:42" maxSheetId="23" userName="ITL-USER" r:id="rId376" minRId="1706" maxRId="1707">
     <sheetIdMap count="22">
       <sheetId val="14"/>
       <sheetId val="1"/>
@@ -23289,6 +23701,104 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog357.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="1661" sId="1" eol="1" ref="A25:XFD25" action="insertRow"/>
+  <rcc rId="1662" sId="1">
+    <nc r="A25" t="inlineStr">
+      <is>
+        <t>YINV_YINS_101</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1663" sId="1">
+    <nc r="B25" t="inlineStr">
+      <is>
+        <t>admin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1664" sId="1">
+    <nc r="C25" t="inlineStr">
+      <is>
+        <t>Admin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1665" sId="1">
+    <nc r="D25" t="inlineStr">
+      <is>
+        <t>OPR1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1666" sId="1">
+    <nc r="E25" t="inlineStr">
+      <is>
+        <t>CPX11</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1667" sId="1">
+    <nc r="F25" t="inlineStr">
+      <is>
+        <t>FCY111</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1668" sId="1">
+    <nc r="G25" t="inlineStr">
+      <is>
+        <t>YRD1111</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog358.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1669" sId="1">
+    <nc r="H1" t="inlineStr">
+      <is>
+        <t>Unit1inSNX</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1670" sId="1">
+    <nc r="H25" t="inlineStr">
+      <is>
+        <t>ASWU2705190~ASW~F10L.1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog359.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1671" sId="1">
+    <nc r="I10" t="inlineStr">
+      <is>
+        <t>SnxName</t>
+      </is>
+    </nc>
+  </rcc>
+  <rm rId="1672" sheetId="1" source="I10" destination="I1" sourceSheetId="1"/>
+  <rcc rId="1673" sId="1">
+    <nc r="I25" t="inlineStr">
+      <is>
+        <t>ReceiveEmptyUnit2200.xml</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog36.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="58" sId="3" xfDxf="1" dxf="1">
@@ -23303,6 +23813,271 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog360.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="1674" sId="1" ref="I1:I1048576" action="insertCol"/>
+  <rcc rId="1675" sId="1" xfDxf="1" dxf="1">
+    <nc r="I1" t="inlineStr">
+      <is>
+        <t>Unit2inSNX</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1676" sId="1">
+    <nc r="I25" t="inlineStr">
+      <is>
+        <t>ASWU2705180~ASW~F10K.1</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog361.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="1677" sId="1" ref="J1:J1048576" action="insertCol"/>
+  <rcc rId="1678" sId="1">
+    <nc r="J1" t="inlineStr">
+      <is>
+        <t>Unit3inSNX</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1679" sId="1">
+    <nc r="J25" t="inlineStr">
+      <is>
+        <t>ASWU2705170~ASW~F10K.2</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog362.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="1680" sId="8" eol="1" ref="A9:XFD9" action="insertRow"/>
+  <rcc rId="1681" sId="8">
+    <nc r="A9" t="inlineStr">
+      <is>
+        <t>YINV_YINS_101</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1682" sId="8">
+    <nc r="B9" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1683" sId="8">
+    <nc r="C9" t="inlineStr">
+      <is>
+        <t>ASWU2705180</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1684" sId="8">
+    <nc r="D9" t="inlineStr">
+      <is>
+        <t>PAYLOAD</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog363.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rrc rId="1685" sId="10" eol="1" ref="A13:XFD13" action="insertRow"/>
+  <rcc rId="1686" sId="10">
+    <nc r="A13" t="inlineStr">
+      <is>
+        <t>YINV_YINS_101</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1687" sId="10">
+    <nc r="B13" t="inlineStr">
+      <is>
+        <t>admin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1688" sId="10">
+    <nc r="C13" t="inlineStr">
+      <is>
+        <t>Admin</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1689" sId="10">
+    <nc r="D13" t="inlineStr">
+      <is>
+        <t>OPR1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1690" sId="10">
+    <nc r="E13" t="inlineStr">
+      <is>
+        <t>CPX11</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1691" sId="10">
+    <nc r="F13" t="inlineStr">
+      <is>
+        <t>FCY111</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1692" sId="10">
+    <nc r="G13" t="inlineStr">
+      <is>
+        <t>YRD1111</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1693" sId="10">
+    <nc r="H13" t="inlineStr">
+      <is>
+        <t>YardInspection</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog364.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1694" sId="21">
+    <nc r="H1" t="inlineStr">
+      <is>
+        <t>n4YInspEnterContainer</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1695" sId="21">
+    <nc r="A3" t="inlineStr">
+      <is>
+        <t>YINV_YINS_101</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog365.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1696" sId="21">
+    <nc r="H3" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog366.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1697" sId="10">
+    <oc r="H13" t="inlineStr">
+      <is>
+        <t>YardInspection</t>
+      </is>
+    </oc>
+    <nc r="H13" t="inlineStr">
+      <is>
+        <t>Yard Inspection</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog367.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1698" sId="21">
+    <nc r="I1" t="inlineStr">
+      <is>
+        <t>n4YInspBUndleContainer2</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1699" sId="21">
+    <nc r="I3" t="inlineStr">
+      <is>
+        <t>ASWU2705170</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog368.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1700" sId="8">
+    <nc r="E1" t="inlineStr">
+      <is>
+        <t>UnitAttached</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1701" sId="8">
+    <nc r="E9" t="inlineStr">
+      <is>
+        <t>ASWU2705170</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog369.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1702" sId="8">
+    <nc r="F1" t="inlineStr">
+      <is>
+        <t>DeleteUnit1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1703" sId="8">
+    <nc r="F9" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1704" sId="8">
+    <nc r="G1" t="inlineStr">
+      <is>
+        <t>DeleteUnit2</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1705" sId="8">
+    <nc r="G9" t="inlineStr">
+      <is>
+        <t>ASWU2705180</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="delete"/>
+  <rcv guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" action="add"/>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog37.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="59" sId="3" xfDxf="1" dxf="1">
@@ -23314,6 +24089,25 @@
   </rcc>
   <rcv guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" action="delete"/>
   <rcv guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog370.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1706" sId="8">
+    <nc r="H1" t="inlineStr">
+      <is>
+        <t>DeleteUnit3</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1707" sId="8">
+    <nc r="H9" t="inlineStr">
+      <is>
+        <t>ASWU2705170</t>
+      </is>
+    </nc>
+  </rcc>
 </revisions>
 </file>
 
@@ -25204,8 +25998,8 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="18">
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="19">
   <userInfo guid="{0FC3EEC7-1253-40C9-80FE-72015618EED8}" name="ITLAdmin" id="-2068730528" dateTime="2018-04-13T11:51:21"/>
   <userInfo guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" name="itluser" id="-446795219" dateTime="2018-04-13T11:51:26"/>
   <userInfo guid="{44866337-4EB8-44FB-BDBC-D3FE257C9028}" name="ITLAdmin" id="-2068734883" dateTime="2018-04-26T11:22:09"/>
@@ -25224,6 +26018,7 @@
   <userInfo guid="{1B798433-1A94-48A7-AAE8-8E50EBC29F29}" name="itluser" id="-446813434" dateTime="2018-06-25T18:05:22"/>
   <userInfo guid="{A362D75E-4E39-49D0-8B9D-E19BB878EFC7}" name="itluser" id="-446792401" dateTime="2018-06-27T13:17:27"/>
   <userInfo guid="{DCCF7D31-EB2E-4962-A2BC-0BA8BDB3EA47}" name="itluser" id="-446794865" dateTime="2018-06-29T14:13:37"/>
+  <userInfo guid="{AE37B969-B9E8-407D-AD25-C9352A863F89}" name="ITL-USER" id="-1580083848" dateTime="2018-07-03T15:32:40"/>
 </users>
 </file>
 
@@ -25505,11 +26300,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" state="hidden">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" state="hidden">
       <selection activeCell="H18" sqref="H18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" state="hidden">
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" state="hidden">
       <selection activeCell="H18" sqref="H18"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -25520,22 +26315,25 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="14"/>
+    <col min="5" max="5" width="12.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -25548,8 +26346,20 @@
       <c r="D1" s="14" t="s">
         <v>343</v>
       </c>
+      <c r="E1" s="14" t="s">
+        <v>630</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>631</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>632</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>633</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>303</v>
       </c>
@@ -25557,7 +26367,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>341</v>
       </c>
@@ -25571,7 +26381,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>335</v>
       </c>
@@ -25579,7 +26389,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>337</v>
       </c>
@@ -25587,7 +26397,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>338</v>
       </c>
@@ -25595,7 +26405,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>339</v>
       </c>
@@ -25603,22 +26413,48 @@
         <v>344</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>340</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>344</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>618</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>461</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>627</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>629</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>461</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>629</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="G9" sqref="G9"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection sqref="A1:D1"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="B1" sqref="B1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
@@ -25632,15 +26468,20 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -25659,8 +26500,14 @@
       <c r="F1" t="s">
         <v>599</v>
       </c>
+      <c r="H1" t="s">
+        <v>367</v>
+      </c>
+      <c r="I1" t="s">
+        <v>628</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>601</v>
       </c>
@@ -25680,13 +26527,26 @@
         <v>3050</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>618</v>
+      </c>
       <c r="E3" s="16" t="s">
         <v>246</v>
+      </c>
+      <c r="H3" t="s">
+        <v>344</v>
+      </c>
+      <c r="I3" t="s">
+        <v>629</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="I3" sqref="I3"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="B2" sqref="B2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25698,10 +26558,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26042,14 +26902,40 @@
         <v>448</v>
       </c>
     </row>
+    <row r="13" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>618</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>398</v>
+      </c>
+    </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="H10" sqref="H10"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="G15" sqref="G15"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="H2" sqref="H2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
@@ -26065,8 +26951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26180,12 +27066,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="E2" sqref="E2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="F2" sqref="F2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="E2" sqref="E2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
@@ -27064,11 +27950,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="AH13" sqref="AH13"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="AH13" sqref="AH13"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -27081,7 +27968,7 @@
   <dimension ref="A1:BL2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27451,12 +28338,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="B1">
+      <selection activeCell="F13" sqref="F13"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="B1">
       <selection activeCell="K1" sqref="K1"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="B1">
-      <selection activeCell="F13" sqref="F13"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -27804,11 +28691,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection sqref="A1:A1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection sqref="A1:A1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -27866,6 +28753,10 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="G11" sqref="G11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="G11" sqref="G11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -27914,11 +28805,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
       <selection activeCell="C2" sqref="C2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="C2" sqref="C2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -27931,8 +28822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28037,12 +28928,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="M1">
+      <selection activeCell="Q1" sqref="Q1"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="B2" sqref="B2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="M1">
-      <selection activeCell="Q1" sqref="Q1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -28052,10 +28943,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28064,9 +28955,12 @@
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="9.42578125" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="25.5703125" style="16" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -28088,8 +28982,20 @@
       <c r="G1" t="s">
         <v>14</v>
       </c>
+      <c r="H1" t="s">
+        <v>619</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>623</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>625</v>
+      </c>
+      <c r="K1" t="s">
+        <v>621</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -28112,12 +29018,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>242</v>
       </c>
@@ -28128,7 +29034,7 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>235</v>
       </c>
@@ -28139,7 +29045,7 @@
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>226</v>
       </c>
@@ -28150,7 +29056,7 @@
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>216</v>
       </c>
@@ -28161,7 +29067,7 @@
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>219</v>
       </c>
@@ -28172,7 +29078,7 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>247</v>
       </c>
@@ -28183,7 +29089,7 @@
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>298</v>
       </c>
@@ -28206,7 +29112,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>303</v>
       </c>
@@ -28229,7 +29135,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>341</v>
       </c>
@@ -28252,7 +29158,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>335</v>
       </c>
@@ -28274,8 +29180,10 @@
       <c r="G13" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>337</v>
       </c>
@@ -28298,7 +29206,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>338</v>
       </c>
@@ -28321,7 +29229,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>339</v>
       </c>
@@ -28344,7 +29252,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>340</v>
       </c>
@@ -28367,32 +29275,34 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>397</v>
       </c>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>596</v>
       </c>
@@ -28415,20 +29325,55 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>601</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>618</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>620</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>624</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>626</v>
+      </c>
+      <c r="K25" s="16" t="s">
+        <v>622</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="A7">
-      <selection activeCell="H22" sqref="H22"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="J25" sqref="J25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="G9" sqref="G9"/>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="A7">
+      <selection activeCell="H22" sqref="H22"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -28448,7 +29393,7 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28529,12 +29474,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="N9" sqref="N9"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="A2" sqref="A2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="N9" sqref="N9"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -28546,8 +29491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <selection activeCell="AI2" sqref="AI2:AI3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28868,12 +29813,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="Z1">
+      <selection activeCell="AI2" sqref="AI2:AI3"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="G15" sqref="G15"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="Z1">
-      <selection activeCell="AI2" sqref="AI2:AI3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -28890,6 +29835,9 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -28903,7 +29851,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28961,12 +29909,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="K12" sqref="K12"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="G15" sqref="G15"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="K12" sqref="K12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
@@ -28982,8 +29930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29122,12 +30070,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="O1">
+      <selection activeCell="Y1" sqref="Y1"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="G15" sqref="G15"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="O1">
-      <selection activeCell="Y1" sqref="Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="O1">
@@ -29143,8 +30091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE2"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29480,13 +30428,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="J1">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="V1">
+      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="V1">
-      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}" topLeftCell="J1">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -29506,7 +30454,7 @@
   <dimension ref="A1:AT25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29978,12 +30926,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="G15" sqref="G15"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
@@ -30000,7 +30948,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="Q1" sqref="Q1:Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30162,12 +31110,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="Q1" sqref="Q1:Y1"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
       <selection activeCell="G15" sqref="G15"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="Q1" sqref="Q1:Y1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}">
@@ -30183,8 +31131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AI2" sqref="AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30409,14 +31357,14 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="G15" sqref="G15"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
     <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}" topLeftCell="W1">
       <selection activeCell="AI2" sqref="AI2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
+    </customSheetView>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" topLeftCell="W1">
       <selection activeCell="AI2" sqref="AI2"/>
@@ -30425,6 +31373,7 @@
     </customSheetView>
   </customSheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -30433,7 +31382,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30501,13 +31450,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
-      <selection activeCell="G15" sqref="G15"/>
+    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
+      <selection activeCell="G1" sqref="G1"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{AE57F689-A611-481B-AACE-13E1C8730C10}">
-      <selection activeCell="G1" sqref="G1"/>
+    <customSheetView guid="{084005ED-0756-4EF6-8351-F9B323091E9B}">
+      <selection activeCell="G15" sqref="G15"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" r:id="rId2"/>
     </customSheetView>

</xml_diff>

<commit_message>
Aswini - Updated Scripts
</commit_message>
<xml_diff>
--- a/Basic Test Suite/TestData/TestData.xlsx
+++ b/Basic Test Suite/TestData/TestData.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ITL-USER\Desktop\TestComplete\Basic Test Suite\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ITL-USER\Desktop\Latest\Basic Test Suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="8" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="cdsds" sheetId="14" state="hidden" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="638">
   <si>
     <t>Flow Name</t>
   </si>
@@ -1835,118 +1835,130 @@
     <t>Successfully</t>
   </si>
   <si>
+    <t>EquipmentType</t>
+  </si>
+  <si>
+    <t>EquipmentOperator</t>
+  </si>
+  <si>
+    <t>EquipmentWeigth</t>
+  </si>
+  <si>
+    <t>NMGS</t>
+  </si>
+  <si>
+    <t>n4Accesory</t>
+  </si>
+  <si>
+    <t>EquipmentOwner</t>
+  </si>
+  <si>
+    <t>n4Vesselid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VVANA </t>
+  </si>
+  <si>
+    <t>n4UnitID</t>
+  </si>
+  <si>
+    <t>n4EquipmntType</t>
+  </si>
+  <si>
+    <t>n4EquipmntLineOperator</t>
+  </si>
+  <si>
+    <t>n4VesselFreigthKind</t>
+  </si>
+  <si>
+    <t>n4VesselGrossWeigth</t>
+  </si>
+  <si>
+    <t>n4VesselVGMWeigth</t>
+  </si>
+  <si>
+    <t>n4VesselPortofLoad</t>
+  </si>
+  <si>
+    <t>n4VesselPortOfDischarge</t>
+  </si>
+  <si>
+    <t>n4VesselCategory</t>
+  </si>
+  <si>
+    <t>Import</t>
+  </si>
+  <si>
+    <t>UnitIdEquip</t>
+  </si>
+  <si>
+    <t>DINU857531</t>
+  </si>
+  <si>
+    <t>YINV_YINS_101</t>
+  </si>
+  <si>
+    <t>Unit1inSNX</t>
+  </si>
+  <si>
+    <t>ASWU2705190~ASW~F10L.1</t>
+  </si>
+  <si>
+    <t>SnxName</t>
+  </si>
+  <si>
+    <t>ReceiveEmptyUnit2200.xml</t>
+  </si>
+  <si>
+    <t>Unit2inSNX</t>
+  </si>
+  <si>
+    <t>ASWU2705180~ASW~F10K.1</t>
+  </si>
+  <si>
+    <t>Unit3inSNX</t>
+  </si>
+  <si>
+    <t>ASWU2705170~ASW~F10K.2</t>
+  </si>
+  <si>
+    <t>PAYLOAD</t>
+  </si>
+  <si>
+    <t>n4YInspBUndleContainer2</t>
+  </si>
+  <si>
+    <t>ASWU2705170</t>
+  </si>
+  <si>
+    <t>UnitAttached</t>
+  </si>
+  <si>
+    <t>DeleteUnit1</t>
+  </si>
+  <si>
+    <t>DeleteUnit2</t>
+  </si>
+  <si>
+    <t>DeleteUnit3</t>
+  </si>
+  <si>
+    <t>ACCESSORY</t>
+  </si>
+  <si>
+    <t>n4yardSlot</t>
+  </si>
+  <si>
+    <t>F01k.1</t>
+  </si>
+  <si>
     <t>J20591_1</t>
   </si>
   <si>
-    <t>EquipmentType</t>
-  </si>
-  <si>
-    <t>EquipmentOperator</t>
-  </si>
-  <si>
-    <t>EquipmentWeigth</t>
-  </si>
-  <si>
-    <t>NMGS</t>
-  </si>
-  <si>
-    <t>n4Accesory</t>
-  </si>
-  <si>
-    <t>EquipmentOwner</t>
-  </si>
-  <si>
-    <t>n4Vesselid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VVANA </t>
-  </si>
-  <si>
-    <t>n4UnitID</t>
-  </si>
-  <si>
-    <t>n4EquipmntType</t>
-  </si>
-  <si>
-    <t>n4EquipmntLineOperator</t>
-  </si>
-  <si>
-    <t>n4VesselFreigthKind</t>
-  </si>
-  <si>
-    <t>n4VesselGrossWeigth</t>
-  </si>
-  <si>
-    <t>n4VesselVGMWeigth</t>
-  </si>
-  <si>
-    <t>n4VesselPortofLoad</t>
-  </si>
-  <si>
-    <t>n4VesselPortOfDischarge</t>
-  </si>
-  <si>
-    <t>n4VesselCategory</t>
-  </si>
-  <si>
-    <t>Import</t>
-  </si>
-  <si>
-    <t>UnitIdEquip</t>
-  </si>
-  <si>
-    <t>DINU857531</t>
-  </si>
-  <si>
-    <t>DINU7540155</t>
-  </si>
-  <si>
-    <t>YINV_YINS_101</t>
-  </si>
-  <si>
-    <t>Unit1inSNX</t>
-  </si>
-  <si>
-    <t>ASWU2705190~ASW~F10L.1</t>
-  </si>
-  <si>
-    <t>SnxName</t>
-  </si>
-  <si>
-    <t>ReceiveEmptyUnit2200.xml</t>
-  </si>
-  <si>
-    <t>Unit2inSNX</t>
-  </si>
-  <si>
-    <t>ASWU2705180~ASW~F10K.1</t>
-  </si>
-  <si>
-    <t>Unit3inSNX</t>
-  </si>
-  <si>
-    <t>ASWU2705170~ASW~F10K.2</t>
-  </si>
-  <si>
-    <t>PAYLOAD</t>
-  </si>
-  <si>
-    <t>n4YInspBUndleContainer2</t>
-  </si>
-  <si>
-    <t>ASWU2705170</t>
-  </si>
-  <si>
-    <t>UnitAttached</t>
-  </si>
-  <si>
-    <t>DeleteUnit1</t>
-  </si>
-  <si>
-    <t>DeleteUnit2</t>
-  </si>
-  <si>
-    <t>DeleteUnit3</t>
+    <t>DINU1259753</t>
+  </si>
+  <si>
+    <t>CHSASW1~ASW~CH20</t>
   </si>
 </sst>
 </file>
@@ -2024,7 +2036,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{AE37B969-B9E8-407D-AD25-C9352A863F89}" diskRevisions="1" revisionId="1707" version="376">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C411681A-71DB-4E01-9B5F-57A3CC3A76E1}" diskRevisions="1" revisionId="1753" version="389">
   <header guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" dateTime="2018-04-13T11:49:43" maxSheetId="10" userName="itluser" r:id="rId7" minRId="7">
     <sheetIdMap count="9">
       <sheetId val="1"/>
@@ -8702,6 +8714,344 @@
     </sheetIdMap>
   </header>
   <header guid="{AE37B969-B9E8-407D-AD25-C9352A863F89}" dateTime="2018-07-04T11:47:42" maxSheetId="23" userName="ITL-USER" r:id="rId376" minRId="1706" maxRId="1707">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{A6346C5D-87AC-478D-8F81-4BCEC5BDC075}" dateTime="2018-07-05T15:27:53" maxSheetId="23" userName="ITL-USER" r:id="rId377" minRId="1708" maxRId="1712">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{2F8535A4-33DD-4153-938A-193A1CCB1E2F}" dateTime="2018-07-05T15:28:07" maxSheetId="23" userName="ITL-USER" r:id="rId378" minRId="1713">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{FD7DA3CC-D397-449E-884C-797086688BCE}" dateTime="2018-07-05T15:28:40" maxSheetId="23" userName="ITL-USER" r:id="rId379" minRId="1714">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{6E0F2C3E-3156-4D40-9AFA-9BE53369C21A}" dateTime="2018-07-05T15:41:15" maxSheetId="23" userName="ITL-USER" r:id="rId380" minRId="1715" maxRId="1719">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{069B21B8-2780-47E9-ACD6-6A4B4CE1E255}" dateTime="2018-07-05T15:42:24" maxSheetId="23" userName="ITL-USER" r:id="rId381" minRId="1720" maxRId="1721">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{B6C09675-7481-4228-8BCC-5B46721DCF03}" dateTime="2018-07-05T15:42:51" maxSheetId="23" userName="ITL-USER" r:id="rId382" minRId="1722">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{5F7F5544-F16E-487B-9C57-34BDA145EED4}" dateTime="2018-07-05T17:44:38" maxSheetId="23" userName="ITL-USER" r:id="rId383" minRId="1723" maxRId="1725">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{88EE706E-4970-4C7C-A9F9-5D175C166B46}" dateTime="2018-07-05T18:12:29" maxSheetId="23" userName="ITL-USER" r:id="rId384" minRId="1726" maxRId="1733">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{77DCCF27-2C19-4CB2-8C12-A4DB7D604AE4}" dateTime="2018-07-05T18:22:44" maxSheetId="23" userName="ITL-USER" r:id="rId385" minRId="1734">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{CDEC1230-8FCB-4E59-B1C9-37FA19FF6C8C}" dateTime="2018-07-06T09:55:13" maxSheetId="23" userName="ITL-USER" r:id="rId386" minRId="1735" maxRId="1742">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{CFBE0092-BACF-4965-A80C-CDDE392173B4}" dateTime="2018-07-06T09:55:34" maxSheetId="23" userName="ITL-USER" r:id="rId387" minRId="1743" maxRId="1750">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{DFDC7A2F-5628-49E2-88F6-2E09B0961305}" dateTime="2018-07-06T09:59:49" maxSheetId="23" userName="ITL-USER" r:id="rId388" minRId="1751">
+    <sheetIdMap count="22">
+      <sheetId val="14"/>
+      <sheetId val="1"/>
+      <sheetId val="9"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+      <sheetId val="5"/>
+      <sheetId val="6"/>
+      <sheetId val="7"/>
+      <sheetId val="8"/>
+      <sheetId val="21"/>
+      <sheetId val="10"/>
+      <sheetId val="11"/>
+      <sheetId val="12"/>
+      <sheetId val="17"/>
+      <sheetId val="18"/>
+      <sheetId val="20"/>
+      <sheetId val="19"/>
+      <sheetId val="16"/>
+      <sheetId val="15"/>
+      <sheetId val="13"/>
+      <sheetId val="22"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{C411681A-71DB-4E01-9B5F-57A3CC3A76E1}" dateTime="2018-07-06T10:54:12" maxSheetId="23" userName="ITL-USER" r:id="rId389" minRId="1752" maxRId="1753">
     <sheetIdMap count="22">
       <sheetId val="14"/>
       <sheetId val="1"/>
@@ -24111,6 +24461,310 @@
 </revisions>
 </file>
 
+<file path=xl/revisions/revisionLog371.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1708" sId="1">
+    <oc r="A23" t="inlineStr">
+      <is>
+        <t>J20591_1</t>
+      </is>
+    </oc>
+    <nc r="A23" t="inlineStr">
+      <is>
+        <t>J20591_2</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1709" sId="8" odxf="1">
+    <nc r="A10" t="inlineStr">
+      <is>
+        <t>J20591_2</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1710" sId="8" xfDxf="1" dxf="1">
+    <nc r="B10" t="inlineStr">
+      <is>
+        <t>DINU8889512</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1711" sId="8" xfDxf="1" dxf="1">
+    <nc r="C10" t="inlineStr">
+      <is>
+        <t>DINU857531</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1712" sId="8">
+    <nc r="D10" t="inlineStr">
+      <is>
+        <t>Acessory</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog372.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1713" sId="8">
+    <oc r="D10" t="inlineStr">
+      <is>
+        <t>Acessory</t>
+      </is>
+    </oc>
+    <nc r="D10" t="inlineStr">
+      <is>
+        <t>ACCESSORY</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog373.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1714" sId="11" xfDxf="1" dxf="1">
+    <oc r="H2" t="inlineStr">
+      <is>
+        <t>DINU7540155</t>
+      </is>
+    </oc>
+    <nc r="H2" t="inlineStr">
+      <is>
+        <t>DINU8889512</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog374.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1715" sId="11" xfDxf="1" dxf="1">
+    <nc r="Q1" t="inlineStr">
+      <is>
+        <t>n4yardSlot</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1716" sId="11">
+    <nc r="Q2" t="inlineStr">
+      <is>
+        <t>F01k.1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1717" sId="21" odxf="1">
+    <nc r="A4" t="inlineStr">
+      <is>
+        <t>J20591_2</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1718" sId="13" odxf="1">
+    <nc r="A4" t="inlineStr">
+      <is>
+        <t>J20591_2</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1719" sId="21" xfDxf="1" dxf="1">
+    <nc r="B4" t="inlineStr">
+      <is>
+        <t>DINU8889512</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog375.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1720" sId="13">
+    <nc r="S4" t="inlineStr">
+      <is>
+        <t>S1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1721" sId="13">
+    <nc r="AB4">
+      <v>45</v>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog376.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1722" sId="13">
+    <nc r="AC4" t="inlineStr">
+      <is>
+        <t>C</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog377.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1723" sId="8">
+    <oc r="B10" t="inlineStr">
+      <is>
+        <t>DINU8889512</t>
+      </is>
+    </oc>
+    <nc r="B10" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1724" sId="21">
+    <oc r="B4" t="inlineStr">
+      <is>
+        <t>DINU8889512</t>
+      </is>
+    </oc>
+    <nc r="B4" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1725" sId="11">
+    <oc r="H2" t="inlineStr">
+      <is>
+        <t>DINU8889512</t>
+      </is>
+    </oc>
+    <nc r="H2" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog378.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1726" sId="1">
+    <oc r="A23" t="inlineStr">
+      <is>
+        <t>J20591_2</t>
+      </is>
+    </oc>
+    <nc r="A23" t="inlineStr">
+      <is>
+        <t>J20591_1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1727" sId="8">
+    <oc r="A10" t="inlineStr">
+      <is>
+        <t>J20591_2</t>
+      </is>
+    </oc>
+    <nc r="A10" t="inlineStr">
+      <is>
+        <t>J20591_1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1728" sId="21">
+    <oc r="A4" t="inlineStr">
+      <is>
+        <t>J20591_2</t>
+      </is>
+    </oc>
+    <nc r="A4" t="inlineStr">
+      <is>
+        <t>J20591_1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1729" sId="13">
+    <oc r="A4" t="inlineStr">
+      <is>
+        <t>J20591_2</t>
+      </is>
+    </oc>
+    <nc r="A4" t="inlineStr">
+      <is>
+        <t>J20591_1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1730" sId="1" xfDxf="1" dxf="1">
+    <nc r="A26" t="inlineStr">
+      <is>
+        <t>DINU1259753</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1731" sId="8" odxf="1">
+    <oc r="B10" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </oc>
+    <nc r="B10" t="inlineStr">
+      <is>
+        <t>DINU1259753</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1732" sId="21" odxf="1">
+    <oc r="B4" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </oc>
+    <nc r="B4" t="inlineStr">
+      <is>
+        <t>DINU1259753</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1733" sId="13" odxf="1">
+    <nc r="B4" t="inlineStr">
+      <is>
+        <t>DINU1259753</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog379.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1734" sId="11" odxf="1">
+    <oc r="H2" t="inlineStr">
+      <is>
+        <t>ASWU2705190</t>
+      </is>
+    </oc>
+    <nc r="H2" t="inlineStr">
+      <is>
+        <t>DINU1259753</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+</revisions>
+</file>
+
 <file path=xl/revisions/revisionLog38.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <rcc rId="60" sId="3" xfDxf="1" dxf="1">
@@ -24122,6 +24776,169 @@
   </rcc>
   <rcv guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" action="delete"/>
   <rcv guid="{6CC03DA8-51D3-44D9-9803-6B69FF56AB89}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog380.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1735" sId="1">
+    <nc r="H10" t="inlineStr">
+      <is>
+        <t>ASWU2705190~ASW~F10L.1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1736" sId="1">
+    <nc r="H11" t="inlineStr">
+      <is>
+        <t>ASWU2705190~ASW~F10L.1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1737" sId="1">
+    <nc r="H12" t="inlineStr">
+      <is>
+        <t>ASWU2705190~ASW~F10L.1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1738" sId="1">
+    <nc r="H13" t="inlineStr">
+      <is>
+        <t>ASWU2705190~ASW~F10L.1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1739" sId="1">
+    <nc r="H14" t="inlineStr">
+      <is>
+        <t>ASWU2705190~ASW~F10L.1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1740" sId="1">
+    <nc r="H15" t="inlineStr">
+      <is>
+        <t>ASWU2705190~ASW~F10L.1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1741" sId="1">
+    <nc r="H16" t="inlineStr">
+      <is>
+        <t>ASWU2705190~ASW~F10L.1</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="1742" sId="1">
+    <nc r="H17" t="inlineStr">
+      <is>
+        <t>ASWU2705190~ASW~F10L.1</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog381.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1743" sId="1" odxf="1">
+    <nc r="K10" t="inlineStr">
+      <is>
+        <t>ReceiveEmptyUnit2200.xml</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1744" sId="1" odxf="1">
+    <nc r="K11" t="inlineStr">
+      <is>
+        <t>ReceiveEmptyUnit2200.xml</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1745" sId="1" odxf="1">
+    <nc r="K12" t="inlineStr">
+      <is>
+        <t>ReceiveEmptyUnit2200.xml</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1746" sId="1" odxf="1">
+    <nc r="K13" t="inlineStr">
+      <is>
+        <t>ReceiveEmptyUnit2200.xml</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1747" sId="1" odxf="1">
+    <nc r="K14" t="inlineStr">
+      <is>
+        <t>ReceiveEmptyUnit2200.xml</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1748" sId="1" odxf="1">
+    <nc r="K15" t="inlineStr">
+      <is>
+        <t>ReceiveEmptyUnit2200.xml</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1749" sId="1" odxf="1">
+    <nc r="K16" t="inlineStr">
+      <is>
+        <t>ReceiveEmptyUnit2200.xml</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+  <rcc rId="1750" sId="1" odxf="1">
+    <nc r="K17" t="inlineStr">
+      <is>
+        <t>ReceiveEmptyUnit2200.xml</t>
+      </is>
+    </nc>
+    <odxf/>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog382.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1751" sId="1">
+    <nc r="I12" t="inlineStr">
+      <is>
+        <t>CHSASW1~ASW~CH20</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog383.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1752" sId="1">
+    <oc r="H10" t="inlineStr">
+      <is>
+        <t>ASWU2705190~ASW~F10L.1</t>
+      </is>
+    </oc>
+    <nc r="H10"/>
+  </rcc>
+  <rcc rId="1753" sId="1">
+    <oc r="K10" t="inlineStr">
+      <is>
+        <t>ReceiveEmptyUnit2200.xml</t>
+      </is>
+    </oc>
+    <nc r="K10"/>
+  </rcc>
 </revisions>
 </file>
 
@@ -25998,8 +26815,8 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="19">
+<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="20">
   <userInfo guid="{0FC3EEC7-1253-40C9-80FE-72015618EED8}" name="ITLAdmin" id="-2068730528" dateTime="2018-04-13T11:51:21"/>
   <userInfo guid="{A67DA2CD-5A32-48AB-8C17-215B95672A36}" name="itluser" id="-446795219" dateTime="2018-04-13T11:51:26"/>
   <userInfo guid="{44866337-4EB8-44FB-BDBC-D3FE257C9028}" name="ITLAdmin" id="-2068734883" dateTime="2018-04-26T11:22:09"/>
@@ -26019,6 +26836,7 @@
   <userInfo guid="{A362D75E-4E39-49D0-8B9D-E19BB878EFC7}" name="itluser" id="-446792401" dateTime="2018-06-27T13:17:27"/>
   <userInfo guid="{DCCF7D31-EB2E-4962-A2BC-0BA8BDB3EA47}" name="itluser" id="-446794865" dateTime="2018-06-29T14:13:37"/>
   <userInfo guid="{AE37B969-B9E8-407D-AD25-C9352A863F89}" name="ITL-USER" id="-1580083848" dateTime="2018-07-03T15:32:40"/>
+  <userInfo guid="{C411681A-71DB-4E01-9B5F-57A3CC3A76E1}" name="ITL-USER" id="-1580110567" dateTime="2018-07-05T18:46:10"/>
 </users>
 </file>
 
@@ -26315,10 +27133,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26347,16 +27165,16 @@
         <v>343</v>
       </c>
       <c r="E1" s="14" t="s">
+        <v>628</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>629</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>630</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>631</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>632</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -26423,7 +27241,7 @@
     </row>
     <row r="9" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>344</v>
@@ -26432,10 +27250,10 @@
         <v>461</v>
       </c>
       <c r="D9" s="16" t="s">
+        <v>625</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>627</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>629</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>344</v>
@@ -26444,7 +27262,21 @@
         <v>461</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>629</v>
+        <v>627</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>635</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>636</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>615</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>632</v>
       </c>
     </row>
   </sheetData>
@@ -26468,7 +27300,7 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
@@ -26486,39 +27318,39 @@
         <v>0</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C1" s="16" t="s">
+        <v>597</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>596</v>
+      </c>
+      <c r="E1" t="s">
+        <v>601</v>
+      </c>
+      <c r="F1" t="s">
         <v>598</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>597</v>
-      </c>
-      <c r="E1" t="s">
-        <v>602</v>
-      </c>
-      <c r="F1" t="s">
-        <v>599</v>
       </c>
       <c r="H1" t="s">
         <v>367</v>
       </c>
       <c r="I1" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>5</v>
@@ -26529,7 +27361,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E3" s="16" t="s">
         <v>246</v>
@@ -26538,7 +27370,15 @@
         <v>344</v>
       </c>
       <c r="I3" t="s">
-        <v>629</v>
+        <v>627</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>635</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>636</v>
       </c>
     </row>
   </sheetData>
@@ -26904,7 +27744,7 @@
     </row>
     <row r="13" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B13" s="16" t="s">
         <v>3</v>
@@ -26949,7 +27789,7 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -26964,7 +27804,7 @@
     <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -26984,37 +27824,40 @@
         <v>594</v>
       </c>
       <c r="G1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="H1" t="s">
+        <v>604</v>
+      </c>
+      <c r="I1" t="s">
         <v>605</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>606</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>607</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>608</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>609</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>610</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>611</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>612</v>
       </c>
-      <c r="P1" t="s">
-        <v>613</v>
+      <c r="Q1" t="s">
+        <v>633</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>56</v>
       </c>
@@ -27034,10 +27877,10 @@
         <v>595</v>
       </c>
       <c r="G2" t="s">
-        <v>604</v>
-      </c>
-      <c r="H2" t="s">
-        <v>617</v>
+        <v>603</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>636</v>
       </c>
       <c r="I2">
         <v>2200</v>
@@ -27061,7 +27904,10 @@
         <v>7</v>
       </c>
       <c r="P2" t="s">
-        <v>614</v>
+        <v>613</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>634</v>
       </c>
     </row>
   </sheetData>
@@ -28943,10 +29789,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28983,16 +29829,16 @@
         <v>14</v>
       </c>
       <c r="H1" t="s">
+        <v>617</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>621</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>623</v>
+      </c>
+      <c r="K1" t="s">
         <v>619</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>623</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>625</v>
-      </c>
-      <c r="K1" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -29111,6 +29957,7 @@
       <c r="G10" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="K10" s="16"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
@@ -29134,6 +29981,12 @@
       <c r="G11" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="H11" s="16" t="s">
+        <v>618</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
@@ -29157,6 +30010,15 @@
       <c r="G12" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="H12" s="16" t="s">
+        <v>618</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>637</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="13" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
@@ -29180,8 +30042,14 @@
       <c r="G13" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="H13" s="16" t="s">
+        <v>618</v>
+      </c>
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
+      <c r="K13" s="16" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
@@ -29205,6 +30073,12 @@
       <c r="G14" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="H14" s="16" t="s">
+        <v>618</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
@@ -29228,6 +30102,12 @@
       <c r="G15" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="H15" s="16" t="s">
+        <v>618</v>
+      </c>
+      <c r="K15" s="16" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
@@ -29251,6 +30131,12 @@
       <c r="G16" s="14" t="s">
         <v>15</v>
       </c>
+      <c r="H16" s="16" t="s">
+        <v>618</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>620</v>
+      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
@@ -29273,6 +30159,12 @@
       </c>
       <c r="G17" s="14" t="s">
         <v>15</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>618</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>620</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -29304,7 +30196,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
-        <v>596</v>
+        <v>635</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>3</v>
@@ -29327,12 +30219,12 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="B25" s="16" t="s">
         <v>3</v>
@@ -29353,16 +30245,21 @@
         <v>15</v>
       </c>
       <c r="H25" s="16" t="s">
+        <v>618</v>
+      </c>
+      <c r="I25" s="16" t="s">
+        <v>622</v>
+      </c>
+      <c r="J25" s="16" t="s">
+        <v>624</v>
+      </c>
+      <c r="K25" s="16" t="s">
         <v>620</v>
       </c>
-      <c r="I25" s="16" t="s">
-        <v>624</v>
-      </c>
-      <c r="J25" s="16" t="s">
-        <v>626</v>
-      </c>
-      <c r="K25" s="16" t="s">
-        <v>622</v>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>636</v>
       </c>
     </row>
   </sheetData>
@@ -29489,7 +30386,7 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI3"/>
+  <dimension ref="A1:AI4"/>
   <sheetViews>
     <sheetView topLeftCell="Z1" workbookViewId="0">
       <selection activeCell="AI2" sqref="AI2:AI3"/>
@@ -29809,6 +30706,23 @@
       </c>
       <c r="AI3" s="16" t="s">
         <v>364</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>635</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>636</v>
+      </c>
+      <c r="S4" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="AB4" s="14">
+        <v>45</v>
+      </c>
+      <c r="AC4" s="14" t="s">
+        <v>419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>